<commit_message>
feat(ferramentas): melhorar extração de dados para planilha de funcionalidades v2.0
MELHORIAS NA EXTRAÇÃO:
- Nome: busca em rf.nome, titulo, e estruturas aninhadas
- Descrição: prioriza resumo_executivo > descricao.objetivo > objetivos[]
- Regras: extrai apenas títulos (linguagem simples, nível coordenação)
- Limita descrição a 200 caracteres (sucinta)
- Limita regras às 5 primeiras (mais importantes)

ESTATÍSTICAS v2.0:
- 106 RFs extraídos (1 com erro de parse YAML)
- 80 RFs com nome preenchido (75%)
- 81 RFs com descrição preenchida (76%)
- 106 RFs com regras (100%)

FUNÇÃO extrair_texto():
- Suporte a estruturas complexas (dict, list, string)
- Extração recursiva de campos (objetivo, problema_resolvido, etc)

REGRAS SIMPLIFICADAS:
- Usa apenas campo 'titulo' das regras_negocio
- Remove detalhes técnicos (implementacao, validacoes, etc)
- Linguagem acessível para coordenação

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/funcionalidades.xlsx
+++ b/funcionalidades.xlsx
@@ -508,16 +508,19 @@
           <t>RF001</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr"/>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Sistema de Parâmetros e Configurações Centralizadas</t>
+        </is>
+      </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Implementar o Sistema de Parâmetros e Configurações Centralizadas do IControlIT, responsável por gerenciar todas as configurações do sistema de forma flexível, segura e auditável, permitindo que administradores personalizem comportamentos do sistema sem necessidade de alteração de código.
-</t>
+          <t>Implementar o Sistema de Parâmetros e Configurações Centralizadas do IControlIT, responsável por gerenciar todas as configurações do sistema de forma flexível, segura e auditável, permitindo que ad...</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>O código do parâmetro (Cd_Parametro) deve ser único por Fornecedor. Valor do parâmetro deve ser validado conforme tipo de dado declarado (String, Integer, Decimal, Boolean, Date, JSON). Parâmetros de sistema (Fl_Sistema = 1) não podem ser editados ou excluídos via interface. Parâmetros sensíveis (Fl_Sensivel = 1) devem ter valores criptografados em AES-256. Se Opcoes_Validas preenchido, valor deve estar na lista de opções separadas por vírgula. Parâmetros obrigatórios (Fl_Obrigatorio = 1) não podem ter valor nulo. Todas as operações (CREATE, UPDATE, DELETE, ACCESS) devem ser registradas em Sistema_Parametro_Historico. Feature flags podem ser globais (Id_Fornecedor = NULL) ou específicas por Fornecedor; flag específica tem prioridade. Features com Tipo_Rollout = Percentage devem calcular hash determinístico do Id_Usuario para consistência. Apenas uma configuração de e-mail pode ser principal (Fl_Principal = 1) por Fornecedor. Configurações SMTP devem ter servidor, porta (1-65535) e credenciais válidas. Cada Tipo_Limite deve ser único por Fornecedor; atualizar Uso_Atual quando operações afetadas ocorrerem. Enviar alertas quando Uso_Atual/Limite &gt;= Percentual_Alerta; evitar duplicação com flag Fl_Alerta_Enviado. Isolamento multi-tenant; usuário só acessa dados do próprio Fornecedor; Super Admin bypassa filtro. Parâmetros tipo JSON devem ter JSON válido; aceitar apenas objetos {} ou arrays [].</t>
+          <t>O código do parâmetro (Cd_Parametro) deve ser único por Fornecedor. Valor do parâmetro deve ser validado conforme tipo de dado declarado (String, Integer, Decimal, Boolean, Date, JSON). Parâmetros de sistema (Fl_Sistema = 1) não podem ser editados ou excluídos via interface. Parâmetros sensíveis (Fl_Sensivel = 1) devem ter valores criptografados em AES-256. Se Opcoes_Validas preenchido, valor deve estar na lista de opções separadas por vírgula.</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr"/>
@@ -528,7 +531,11 @@
           <t>RF002</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>Sistema de Configurações e Parametrização Avançada</t>
+        </is>
+      </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Estabelecer um sistema centralizado de configurações infraestruturais e de integração que permita ao IControlIT gerenciar dinamicamente (sem restart) todas as configurações críticas do sistema.</t>
@@ -536,7 +543,7 @@
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>Configurações seguem hierarquia de precedência: Usuário → Departamento → Empresa → Fornecedor → Global.. Valores marcados como sensíveis (Fl_Criptografado = 1) são automaticamente criptografados com AES-256-GCM usando Azure Key Vault antes de persistir.. Ao alterar configuração, sistema valida tipo de dado antes de persistir. Tipos suportados: String, Integer, Decimal, Boolean, JSON, Enum, DateTime.. Sistema suporta validações customizadas: regex (emails, URLs), ranges (min/max para números), valores permitidos (enum), datas futuras/passadas.. Ao criar ou atualizar configuração, sistema automaticamente invalida cache Redis via pub/sub (zero downtime).. Toda alteração de configuração gera versionamento automático com diff JSON completo (valor anterior vs novo), preservando histórico imutável.. Rollback executa restauração completa do valor anterior em 1-click, gerando nova versão no histórico (não altera versões antigas).. Feature flags suportam 4 estratégias de rollout progressivo: Percentual (ex: 10% dos usuários), Usuário (lista de IDs), Perfil (ex: apenas Desenvolvedores), Empresa (lista de empresas).. Configurações sensíveis (Fl_Criptografado = 1) aparecem como ******** para todos os perfis exceto Super Admin com permissão SYS.CONFIGURACOES.DECRYPT.. Export/Import de configurações valida schema YAML antes de importar, executa dry-run obrigatório, e registra auditoria completa de migração.. Auditoria SOX completa registra: quem alterou, quando, IP, user-agent, motivo da mudança, ticket de mudança (obrigatório para PRD), diff JSON.. Notificações automáticas enviadas via Slack/Teams quando configuração crítica (Fl_Critica = 1) é alterada, incluindo diff, autor e motivo.. Configurações marcadas como somente leitura (Fl_SomenteLeitura = 1) bloqueiam edição e exclusão, retornando HTTP 403 Forbidden.. Dry-run simula impacto da mudança sem persistir, retornando: quantos usuários/empresas serão afetados, quais serviços precisam invalidar cache, e riscos conhecidos.. Feature flags com data de expiração (Dt_Expiracao) são automaticamente desabilitadas por job diário, gerando notificação para desenvolvedores responsáveis.. Criar configuração. Listar configurações. Visualizar configuração. Atualizar configuração. Excluir configuração (soft delete). Validar tipo de dado antes de persistir. Validar unicidade de chave por tenant. Validar regex/ranges/valores permitidos. Validar schema YAML em import. Isolamento de tenant (multi-tenancy). Permissões RBAC granulares. Criptografia AES-256-GCM via Azure Key Vault. Auditoria SOX completa. Proteção de configurações somente leitura. Versionamento automático com diff JSON. Rollback 1-click para qualquer versão. Cache hot-reload (pub/sub Redis). Feature flags com 4 estratégias de rollout. Export/Import YAML/JSON entre ambientes. Dry-run de impacto antes de aplicar mudança. Notificações automáticas Slack/Teams. Expiração automática de feature flags. Hierarquia multi-tenant com precedência. Documentação inline e tooltips.</t>
+          <t>Configurações seguem hierarquia de precedência: Usuário → Departamento → Empresa → Fornecedor → Global.. Valores marcados como sensíveis (Fl_Criptografado = 1) são automaticamente criptografados com AES-256-GCM usando Azure Key Vault antes de persistir.. Ao alterar configuração, sistema valida tipo de dado antes de persistir. Tipos suportados: String, Integer, Decimal, Boolean, JSON, Enum, DateTime.. Sistema suporta validações customizadas: regex (emails, URLs), ranges (min/max para números), valores permitidos (enum), datas futuras/passadas.. Ao criar ou atualizar configuração, sistema automaticamente invalida cache Redis via pub/sub (zero downtime).</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr"/>
@@ -547,11 +554,14 @@
           <t>RF003</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Sistema de Logs, Monitoramento e Observabilidade</t>
+        </is>
+      </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Implementar o Sistema de Logs, Monitoramento e Observabilidade do IControlIT, fornecendo visibilidade completa da saúde do sistema, troubleshooting rápido de problemas, métricas de performance e compliance com requisitos de auditoria (LGPD, SOX, ISO 27001).
-</t>
+          <t>Implementar o Sistema de Logs, Monitoramento e Observabilidade do IControlIT, fornecendo visibilidade completa da saúde do sistema, troubleshooting rápido de problemas, métricas de performance e co...</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -561,13 +571,6 @@
 . Correlation IDs Obrigatórios - Todo request HTTP/API deve ter correlation ID (GUID) propagado em todos os logs relacionados (frontend → API → banco → filas → jobs). Permite rastrear request completo mesmo em sistemas distribuídos.
 . Mascaramento Automático de Dados Sensíveis - CPF, senhas, cartões de crédito e tokens de API devem ser mascarados ANTES de logar (substituição por ***). Compliance LGPD (não logar dados pessoais) e PCI-DSS (não logar dados de cartão). CPF: ***.***.*89-**, Senha: ***, Cartão: **** **** **** 1111.
 . Sampling em Produção - Em produção, apenas 10% dos requests bem-sucedidos (HTTP 2xx) devem ser logados (Info/Debug), mas 100% dos erros (HTTP 4xx/5xx) devem ser sempre logados. Reduz volume/custo mantendo capacidade de diagnóstico completa em falhas.
-. 100% de Erros Sempre Logados - Erros (Level=Error ou Fatal) devem ser SEMPRE logados, independente de sampling ou ambiente. Nunca suprimir logs de exceções, validações falhadas, timeout, acesso negado, etc. Crítico para troubleshooting.
-. Circuit Breaker para Logging - Se sistema de logs centralizado falhar (Seq/Elasticsearch indisponível), aplicação deve degradar graciosamente: escrever logs em arquivo local temporário e NÃO travar/lançar exceção. Logging não pode derrubar aplicação principal.
-. Retenção Automática por Tipo - Logs têm retenção automática baseada em tipo e severidade: Info/Debug = 90 dias (LGPD), Warning/Error = 1 ano (troubleshooting histórico), Logs de Segurança/Auditoria = 7 anos (SOX/ISO 27001). Job diário deleta logs expirados.
-. Métricas RED (Rate, Errors, Duration) - Coletar métricas RED para todos os endpoints: Rate (requests/segundo), Errors (% de erros), Duration (P50/P95/P99 latency). Expor endpoint /metrics (Prometheus format) para monitoramento externo.
-. Health Checks /health Endpoint - Implementar endpoint /health que valida dependências críticas (banco, cache, filas, APIs externas) e retorna HTTP 200 (healthy) ou 503 (unhealthy). Usado por Kubernetes liveness/readiness probes e load balancers.
-. Alertas Automáticos - Gerar alertas proativos para condições críticas: error rate &gt; 5% (últimos 5 min), P95 latency &gt; 3s, disco &gt; 85%, memória &gt; 90%, dependência crítica offline. Integrar com PagerDuty/Opsgenie para notificar equipe 24/7.
-. Tracing Distribuído OpenTelemetry - Implementar tracing distribuído seguindo padrão OpenTelemetry (W3C Trace Context). Propagar Trace-Id e Span-Id entre serviços para reconstruir chamadas completas (frontend → API → banco → filas → jobs). Exportar traces para Jaeger/Zipkin ou Application Insights.
 .</t>
         </is>
       </c>
@@ -579,11 +582,14 @@
           <t>RF004</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr"/>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>Sistema de Auditoria e Logs do Sistema</t>
+        </is>
+      </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Implementar o Sistema de Auditoria Completa do IControlIT, registrando todas as operações críticas do sistema para compliance (LGPD Art. 37/38/46, SOX Seção 404, ISO 27001), troubleshooting, segurança e análise forense. Diferente do RF-003 (logs técnicos de aplicação), RF-004 audita ações de usuários e mudanças de dados de negócio com retenção obrigatória de 7 anos.
-</t>
+          <t>Implementar o Sistema de Auditoria Completa do IControlIT, registrando todas as operações críticas do sistema para compliance (LGPD Art. 37/38/46, SOX Seção 404, ISO 27001), troubleshooting, segura...</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -593,16 +599,6 @@
 . Diff Estruturado (JSON Patch RFC 6902) - Calcular diff estruturado entre estado anterior e novo usando JSON Patch (RFC 6902) e armazenar no campo Diff_JSON. Formato: [{"op":"replace","path":"/Nome","value":"João Silva"}]. Permite queries SQL eficientes para perguntas como "quem alterou o CPF?" ou "qual campo foi modificado mais vezes?".
 . Retenção Diferenciada por Categoria (SOX/LGPD) - Categorias críticas (FINANCIAL, LGPD, SECURITY, EXPORT, ACCESS, CONFIG, CRUD) têm retenção 7 anos (SOX Seção 404, LGPD Art. 37/38/46, ISO 27001). Categorias normais (AUTH, ADMIN, PRINT) têm retenção 1 ano. Job diário arquiva registros &gt; 1 ano em Azure Blob Cold Storage e deleta após expiração.
 . Imutabilidade Garantida (Append-Only) - Registros de auditoria são imutáveis após criação. Tabela Sistema_Auditoria não permite UPDATE ou DELETE. Apenas INSERT (criar) e SELECT (ler). Triggers de banco de dados bloqueiam qualquer tentativa de alteração/exclusão (RAISE ERROR). Proteção contra adulteração de evidências forenses.
-. Assinatura Digital SHA-256 - Registros críticos (FINANCIAL, SECURITY, LGPD, CONFIG) têm hash SHA-256 calculado sobre (Timestamp + UserId + Entidade + EntidadeId + DadosNovos_JSON). Stored em campo Hash_SHA256. Permite validar integridade: recalcular hash e comparar com armazenado detecta adulteração. Endpoint /api/auditoria/{id}/validar-integridade.
-. Detecção de Anomalias - Detectar automaticamente padrões suspeitos: Exportações excessivas (&gt;100 em 1h), Acesso multi-tenant anormal (&gt;50 empresas/dia), Operações fora de horário (22h-6h exceto jobs automáticos). Gerar alerta para segurança/compliance. Dashboard "Detecção de Anomalias" mostra eventos suspeitos ordenados por score de risco.
-. Auditoria de LGPD - Operações LGPD têm tipos específicos: LGPD_ACCESS (acesso a dados pessoais), LGPD_EXPORT (exportação/portabilidade), LGPD_CONSENT (aceite/revogação de consentimento), LGPD_DELETION (exclusão de dados pessoais), LGPD_PORTABILITY (solicitação de portabilidade). Retenção obrigatória 7 anos (LGPD Art. 37, 38, 46). Dashboard "Relatório LGPD" para auditorias.
-. Timeline de Entidade - Endpoint /api/auditoria/timeline?entidade={nome}&amp;id={guid} retorna histórico cronológico completo de mudanças de uma entidade específica. Mostra quem alterou o quê, quando, de onde (IP), snapshot antes/depois, diff estruturado. Permite reconstruir estado da entidade em qualquer momento do passado.
-. Contexto Enriquecido - Todo registro de auditoria inclui contexto completo: IP (origem do request), User-Agent (navegador/app), Correlation ID (rastreamento end-to-end), Tenant (multi-tenancy), Request ID (rastreamento interno), Session ID (sessão do usuário). Permite correlacionar auditoria com logs técnicos (RF-003) e rastrear ataques/fraudes.
-. Arquivamento Automático (Cold Storage) - Registros &gt; 1 ano são automaticamente arquivados em Azure Blob Storage (tier Cold) por job noturno. Mantém-se registro em banco com flag Arquivado=true e AzureBlobUri apontando para arquivo JSON compactado. Reduz custo de banco (50M+ registros) mantendo compliance de retenção 7 anos.
-. Segregação de Funções (SOX) - Detectar automaticamente violações de segregação de funções: Mesmo usuário cria E aprova (ex: fatura), Desenvolvedor acessa dados produção sem ticket, Admin altera próprias permissões sem aprovação. Gerar alerta crítico para auditoria. Dashboard "Violações SOX" lista eventos ordenados por criticidade.
-. Auditoria de Configurações Críticas - Alterações em configurações de sistema críticas (parâmetros, feature flags, permissões) exigem campo Justificativa obrigatório (min 20 caracteres). Tipo CONFIG com retenção 7 anos (SOX). Endpoint rejeita request sem justificativa (HTTP 400). Dashboard "Mudanças Críticas" mostra alterações em parâmetros com justificativa.
-. Busca Full-Text Otimizada - Índice full-text em campos Descricao, DadosAnteriores_JSON, DadosNovos_JSON permite busca rápida em milhões de registros. Queries suportadas: busca por CPF mascarado, email, nome de usuário, IP, ID de entidade. Endpoint /api/auditoria/buscar?q={termo}&amp;periodo={dias}&amp;tipo={categoria}.
-. Alertas de Retention Expirando - Job semanal verifica registros cuja retenção expira em 30 dias e envia alerta para compliance/auditoria. Permite decisão antes da exclusão automática: estender retenção (caso específico), exportar para arquivo externo, ou deixar expirar. Dashboard "Retenção" mostra próximas expirações ordenadas por data.
 .</t>
         </is>
       </c>
@@ -614,11 +610,19 @@
           <t>RF005</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr"/>
-      <c r="C6" s="3" t="inlineStr"/>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Internacionalização (i18n) e Localização</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>Idioma Padrão Obrigatório (pt-BR). Detecção Automática de Idioma Preferido. Fallback em Cascata. Formatação Regional Automática. Validação de Código de Idioma (ISO 639-1 + ISO 3166-1). Código de Idioma Único. Ativação de Idioma Requer Mínimo 80% de Tradução. Estrutura Hierárquica de Chaves (Namespaces). Suporte a Interpolação de Variáveis. Validação de Interpolações no Upload. Formatos de Arquivo Suportados (JSON, PO, XLSX). Validação de HTML Balanceado. Limite de Tamanho de Tradução (Aviso). Detecção de Traduções Idênticas ao Original (Aviso). Versionamento Completo de Uploads. Backup Automático Antes de Sobrescrever. Cache Redis para Performance. Tradução Automática via Azure Translator (Opcional). Permissões RBAC para Gestão de Traduções. Lazy Loading de Traduções no Frontend. Tratamento de Pluralização. Bandeiras e Ícones de Idiomas.</t>
+          <t>Idioma Padrão Obrigatório (pt-BR). Detecção Automática de Idioma Preferido. Fallback em Cascata. Formatação Regional Automática. Validação de Código de Idioma (ISO 639-1 + ISO 3166-1).</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr"/>
@@ -634,10 +638,16 @@
           <t>Gestão de Clientes (Multi-Tenancy SaaS)</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr"/>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Cliente representa a empresa que assinou a plataforma IControlIT e é a raiz
+da hierarquia organizacional do sistema SaaS multi-tenant. Cada Cliente possui
+isolamento total de dados via Row-Level Se...</t>
+        </is>
+      </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>Sem regras documentadas.</t>
+          <t>Cliente como Tenant Raiz. CNPJ Único por Cliente. Validação de Dígitos Verificadores do CNPJ. Razão Social Obrigatória. Consulta ReceitaWS Automática.</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr"/>
@@ -648,18 +658,21 @@
           <t>RF007</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr"/>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Login e Autenticação</t>
+        </is>
+      </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prover ao sistema IControlIT um mecanismo seguro, robusto e auditável de autenticação de usuários
+          <t>Prover ao sistema IControlIT um mecanismo seguro, robusto e auditável de autenticação de usuários
 baseado em JWT (JSON Web Token), garantindo controle de acesso, proteção anti brute-force,
-recuperação de senha, gestão de sessões e auditoria completa.
-</t>
+recupera...</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>Autenticação por Email e Senha. JWT Token com Expiração de 8 Horas. Bloqueio Após 5 Tentativas Falhas. Requisitos Mínimos de Senha. Senha Case-Sensitive. Token de Recuperação Válido por 24 Horas. Não Reutilizar Últimas 5 Senhas. Primeiro Acesso Obriga Troca de Senha. Timeout por Inatividade de 30 Minutos. Auditoria de Todas as Tentativas de Login. Mensagem Genérica para Credenciais Inválidas. Notificação de Login em Novo Dispositivo. Exibição de Logo Corporativa do Tenant no Login.</t>
+          <t>Autenticação por Email e Senha. JWT Token com Expiração de 8 Horas. Bloqueio Após 5 Tentativas Falhas. Requisitos Mínimos de Senha. Senha Case-Sensitive.</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr"/>
@@ -667,21 +680,24 @@
     <row r="9" ht="40" customHeight="1">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>RF007_old</t>
-        </is>
-      </c>
-      <c r="B9" s="3" t="inlineStr"/>
+          <t>RF007</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Login e Autenticação</t>
+        </is>
+      </c>
       <c r="C9" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prover ao sistema IControlIT um mecanismo seguro, robusto e auditável de autenticação de usuários
+          <t>Prover ao sistema IControlIT um mecanismo seguro, robusto e auditável de autenticação de usuários
 baseado em JWT (JSON Web Token), garantindo controle de acesso, proteção anti brute-force,
-recuperação de senha, gestão de sessões e auditoria completa.
-</t>
+recupera...</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>Autenticação por Email e Senha. JWT Token com Expiração de 8 Horas. Bloqueio Após 5 Tentativas Falhas. Requisitos Mínimos de Senha. Senha Case-Sensitive. Token de Recuperação Válido por 24 Horas. Não Reutilizar Últimas 5 Senhas. Primeiro Acesso Obriga Troca de Senha. Timeout por Inatividade de 30 Minutos. Auditoria de Todas as Tentativas de Login. Mensagem Genérica para Credenciais Inválidas. Notificação de Login em Novo Dispositivo.</t>
+          <t>Autenticação por Email e Senha. JWT Token com Expiração de 8 Horas. Bloqueio Após 5 Tentativas Falhas. Requisitos Mínimos de Senha. Senha Case-Sensitive.</t>
         </is>
       </c>
       <c r="E9" s="3" t="inlineStr"/>
@@ -692,7 +708,11 @@
           <t>RF012</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr"/>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Usuários do Sistema</t>
+        </is>
+      </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
           <t>Gerenciar usuários administrativos e operacionais do sistema IControlIT, incluindo autenticação, autorização, gestão de perfis, senhas, sessões, integração com Active Directory e auditoria de acessos.</t>
@@ -700,7 +720,7 @@
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>Login único por Fornecedor (multi-tenancy). Política de senha forte (mínimo 8 caracteres, maiúscula, minúscula, número, especial). Bloqueio automático após 5 tentativas falhas em 15 minutos. Expiração de senha após 90 dias com notificação 7 dias antes. Token JWT expira após 8 horas, refresh token após 30 dias. Permissões efetivas = Permissões do Perfil + Permissões Customizadas (apenas adicionam). Histórico de 12 senhas previne reutilização. MFA via TOTP (código 6 dígitos, janela 30s). Integração Active Directory (autenticação LDAP, sincronização automática). Detecção de login suspeito (IP/país/horário anômalo) com notificação por e-mail. Reset de senha via e-mail com token temporário (válido 1 hora, uso único). Máximo 5 sessões simultâneas por usuário (6ª sessão invalida a mais antiga). Auditoria completa de todos os acessos (sucesso/falha, IP, geolocalização, dispositivo). Primeiro acesso força troca de senha. E-mail único por Fornecedor (multi-tenancy). Detalhamento de Contas e Contatos (níveis 1=Básico, 2=Intermediário, 3=Completo). Status de desativação (1=Ativo, 2=Inativo, 3=Desativado Permanentemente).</t>
+          <t>Login único por Fornecedor (multi-tenancy). Política de senha forte (mínimo 8 caracteres, maiúscula, minúscula, número, especial). Bloqueio automático após 5 tentativas falhas em 15 minutos. Expiração de senha após 90 dias com notificação 7 dias antes. Token JWT expira após 8 horas, refresh token após 30 dias.</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr"/>
@@ -711,17 +731,20 @@
           <t>RF013</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr"/>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Perfis de Acesso (RBAC)</t>
+        </is>
+      </c>
       <c r="C11" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Implementar um sistema completo de Gestão de Perfis de Acesso baseado em RBAC (Role-Based Access Control)
-para controlar o que cada usuário pode fazer no sistema IControlIT através de perfis (roles) e permissões granulares.
-</t>
+          <t>Implementar um sistema completo de Gestão de Perfis de Acesso baseado em RBAC (Role-Based Access Control)
+para controlar o que cada usuário pode fazer no sistema IControlIT através de perfis (roles...</t>
         </is>
       </c>
       <c r="D11" s="3" t="inlineStr">
         <is>
-          <t>Nome do perfil deve ser único dentro do tenant (Fornecedor). Perfis de Sistema são não-editáveis (nome/descrição). Super Admin tem acesso total irrestrito (bypassa validações). Formato de permissão padronizado (modulo:recurso:acao). Alterações em permissões críticas exigem auditoria detalhada com justificativa. Middleware valida permissões em TODA requisição à API (exceto endpoints públicos). Permissões do usuário são cacheadas por 5 minutos. Perfil com usuários vinculados não pode ser deletado. Auditoria automática de alterações via BaseAuditableEntity. Uso de Fl_Ativo (BIT) ao invés de Fl_Desativado (INT).</t>
+          <t>Nome do perfil deve ser único dentro do tenant (Fornecedor). Perfis de Sistema são não-editáveis (nome/descrição). Super Admin tem acesso total irrestrito (bypassa validações). Formato de permissão padronizado (modulo:recurso:acao). Alterações em permissões críticas exigem auditoria detalhada com justificativa.</t>
         </is>
       </c>
       <c r="E11" s="3" t="inlineStr"/>
@@ -732,15 +755,19 @@
           <t>RF014</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr"/>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Configurações do Usuário</t>
+        </is>
+      </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
-          <t>Fornecer ao usuário autenticado a capacidade de gerenciar autonomamente suas informações pessoais, credenciais de segurança (senha) e preferências de interface (idioma, tema, timezone), sem necessidade de intervenção administrativa.</t>
+          <t>Fornecer ao usuário autenticado a capacidade de gerenciar autonomamente suas informações pessoais, credenciais de segurança (senha) e preferências de interface (idioma, tema, timezone), sem necessi...</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>Nome, email, CPF e empresa do usuário são exibidos como somente leitura. Telefone deve seguir formato brasileiro (XX) XXXXX-XXXX ou (XX) XXXX-XXXX. Para alterar senha, usuário deve informar senha atual corretamente. Nova senha deve ter mínimo 8 caracteres, incluindo maiúscula, minúscula, número e caractere especial. Nova senha não pode ser igual à senha atual. Senhas comuns são bloqueadas (123456, password, senha123, admin123, qwerty, etc). Senha não pode conter nome do usuário ou parte do email. Campo de confirmação deve ser idêntico ao campo de nova senha. Idioma selecionado é salvo no perfil do usuário e aplicado imediatamente. Sistema suporta 3 idiomas: pt-BR (padrão), en-US, es-ES. Usuário pode escolher entre temas: light, dark, auto. Sistema oferece lista de timezones IANA comuns (América, Europa, Ásia). Em telas menores (&lt; 1024px), menu lateral de navegação vira drawer overlay. Alteração de idioma em qualquer parte do sistema reflete na tela de configurações. Tela de configurações só é acessível por usuários autenticados. Usuário só pode visualizar e editar suas próprias configurações.</t>
+          <t>Nome, email, CPF e empresa do usuário são exibidos como somente leitura. Telefone deve seguir formato brasileiro (XX) XXXXX-XXXX ou (XX) XXXX-XXXX. Para alterar senha, usuário deve informar senha atual corretamente. Nova senha deve ter mínimo 8 caracteres, incluindo maiúscula, minúscula, número e caractere especial. Nova senha não pode ser igual à senha atual.</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr"/>
@@ -751,16 +778,19 @@
           <t>RF015</t>
         </is>
       </c>
-      <c r="B13" s="3" t="inlineStr"/>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Locais e Endereços</t>
+        </is>
+      </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Permitir que o sistema gerencie a estrutura física e geográfica da empresa através de uma hierarquia completa de locais (País → Estado → Cidade → Edifício → Andar → Sala → Rack → Posição), integrada com validação automática de endereços e geocodificação.
-</t>
+          <t>Permitir que o sistema gerencie a estrutura física e geográfica da empresa através de uma hierarquia completa de locais (País → Estado → Cidade → Edifício → Andar → Sala → Rack → Posição), integrad...</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>CEPs brasileiros devem ter exatamente 8 dígitos numéricos no formato XXXXX-XXX ou XXXXXXXX. Validação via ViaCEP API.. Apenas um local pode ser marcado como Principal (Fl_Principal = true) por tenant. Ao marcar novo como principal, desmarcar automaticamente o anterior.. Hierarquia obrigatória: Sala pertence a Andar, Andar a Edifício, Edifício a Endereço, Endereço a Tenant.. Racks devem atender padrões: Altura 1-48U, Profundidade 600/800/1000mm, Peso &gt; 0kg, Potência &gt; 0W.. Posições em racks (U1-U48) não podem se sobrepor. Ao instalar equipamento em U10-U12, todas estas posições são marcadas como ocupadas.. Tipos de sala: Datacenter/Sala_Servidores/CPD/Sala_Tecnica permitem racks. Escritório/Reunião/Armazenamento NÃO permitem.. Geocodificação automática assíncrona via Google Maps Geocoding API. Se falhar, não impede salvamento do endereço.. Histórico de movimentações é imutável (append-only). Somente INSERT, nunca UPDATE ou DELETE.. Campo Sg_Estado deve conter sigla válida de UF brasileira (AC, AL, ..., TO). Sistema padroniza para UPPERCASE.. Requisições para APIs externas (ViaCEP, Google Maps) com timeout 5s. Circuit breaker após 3 falhas consecutivas (modo aberto 60s).</t>
+          <t>CEPs brasileiros devem ter exatamente 8 dígitos numéricos no formato XXXXX-XXX ou XXXXXXXX. Validação via ViaCEP API.. Apenas um local pode ser marcado como Principal (Fl_Principal = true) por tenant. Ao marcar novo como principal, desmarcar automaticamente o anterior.. Hierarquia obrigatória: Sala pertence a Andar, Andar a Edifício, Edifício a Endereço, Endereço a Tenant.. Racks devem atender padrões: Altura 1-48U, Profundidade 600/800/1000mm, Peso &gt; 0kg, Potência &gt; 0W.. Posições em racks (U1-U48) não podem se sobrepor. Ao instalar equipamento em U10-U12, todas estas posições são marcadas como ocupadas.</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr"/>
@@ -771,18 +801,21 @@
           <t>RF016</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr"/>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Categorias de Ativos</t>
+        </is>
+      </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Especificar o Sistema de Gestão de Categorias do IControlIT, responsável por classificar e
+          <t>Especificar o Sistema de Gestão de Categorias do IControlIT, responsável por classificar e
 organizar ativos, serviços de telecom, tipos de chamados e demais entidades do sistema através
-de uma estrutura hierárquica e customizável de categorias.
-</t>
+de uma estr...</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>Hierarquia máxima de 10 níveis. Validação de loops na hierarquia. Taxa de depreciação válida. Atributos obrigatórios devem ser preenchidos. Valores únicos devem ser únicos. Tipos de dados validados. Categorias de sistema não podem ser excluídas. Inativação em cascata opcional. Atributos herdados. Templates públicos compartilhados. Isolamento multi-tenant.</t>
+          <t>Hierarquia máxima de 10 níveis. Validação de loops na hierarquia. Taxa de depreciação válida. Atributos obrigatórios devem ser preenchidos. Valores únicos devem ser únicos.</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr"/>
@@ -793,18 +826,21 @@
           <t>RF017</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr"/>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Hierarquia Corporativa</t>
+        </is>
+      </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Permitir a criação, manutenção e gestão de uma estrutura hierárquica corporativa
+          <t>Permitir a criação, manutenção e gestão de uma estrutura hierárquica corporativa
 composta por Centro de Custo, Departamento, Setor e Seção, garantindo isolamento
-multi-tenant, auditoria completa, controle de orçamento e rastreabilidade.
-</t>
+multi-tenant, auditoria completa, c...</t>
         </is>
       </c>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>Código Único por Fornecedor. Hierarquia Obrigatória em Cascata. Não Pode Inativar com Filhos Ativos. Gestor Deve Ser Consumidor Ativo. Budget Mensal Deve Ser Positivo. Centro de Custo Vinculado à Filial. Código Deve Ser UPPER_SNAKE_CASE. Não Alterar Código com Histórico. Isolamento por Fornecedor (Multi-tenancy). Auditoria Completa de Alterações. Nome Obrigatório e Limite de Caracteres. Propagação de Inativação em Cascata (Opcional). Validação de E-mail de Gestor. Relatório de Consumo por CC/Depto/Setor/Seção. Alerta de Budget Excedido.</t>
+          <t>Código Único por Fornecedor. Hierarquia Obrigatória em Cascata. Não Pode Inativar com Filhos Ativos. Gestor Deve Ser Consumidor Ativo. Budget Mensal Deve Ser Positivo.</t>
         </is>
       </c>
       <c r="E15" s="3" t="inlineStr"/>
@@ -815,7 +851,11 @@
           <t>RF018</t>
         </is>
       </c>
-      <c r="B16" s="3" t="inlineStr"/>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Cargos</t>
+        </is>
+      </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
           <t>Cadastrar, manter e controlar a estrutura organizacional relacionada a cargos, hierarquias, alçadas de aprovação e competências.</t>
@@ -823,7 +863,7 @@
       </c>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>Código de cargo único por Fornecedor (multi-tenancy). Nome de cargo obrigatório (3-150 caracteres). Hierarquia sem ciclos (validação de grafo). Alçada de aprovação monótona crescente (supervisor &gt;= subordinado). Cargo não pode ser deletado se tiver ocupantes ativos. Centro de custo padrão deve existir e estar ativo. Competência requerida deve ser válida (nível 1-5). Faixa salarial com validação de ordem (Piso &lt; Teto, &gt;= salário mínimo). Perfil de sistema sugerido não é obrigatório (opcional). Auditoria de todas as mudanças (CREATE, UPDATE, DELETE). Isolamento por tenant (ClienteId em todas as operações). Permissões RBAC obrigatórias para cada operação.</t>
+          <t>Código de cargo único por Fornecedor (multi-tenancy). Nome de cargo obrigatório (3-150 caracteres). Hierarquia sem ciclos (validação de grafo). Alçada de aprovação monótona crescente (supervisor &gt;= subordinado). Cargo não pode ser deletado se tiver ocupantes ativos.</t>
         </is>
       </c>
       <c r="E16" s="3" t="inlineStr"/>
@@ -834,7 +874,11 @@
           <t>RF019</t>
         </is>
       </c>
-      <c r="B17" s="3" t="inlineStr"/>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Tipos de Ativos</t>
+        </is>
+      </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
           <t>Permitir a categorização, classificação e padronização de todos os ativos de TI e Telecom através de um sistema hierárquico de tipos de ativos.</t>
@@ -842,7 +886,7 @@
       </c>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>Código Único por Fornecedor. Hierarquia de Tipos (Até 5 Níveis). Categoria Principal Válida. Depreciação Obrigatória para Hardware. Não Permitir Exclusão com Ativos Associados. Não Permitir Exclusão com Subtipos. Taxa de Depreciação Válida. Tipos de Sistema Não Editáveis. Recalcular Hierarquia ao Mudar Pai. Auditoria Completa de Alterações. Ícone e Cor para Identificação Visual. Ordem de Exibição Customizável. Não Permitir Loop Hierárquico. Importação em Massa com Validação. Soft Delete com Possibilidade de Restauração.</t>
+          <t>Código Único por Fornecedor. Hierarquia de Tipos (Até 5 Níveis). Categoria Principal Válida. Depreciação Obrigatória para Hardware. Não Permitir Exclusão com Ativos Associados.</t>
         </is>
       </c>
       <c r="E17" s="3" t="inlineStr"/>
@@ -853,15 +897,19 @@
           <t>RF020</t>
         </is>
       </c>
-      <c r="B18" s="3" t="inlineStr"/>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Documentos e Anexos</t>
+        </is>
+      </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
-          <t>Implementar um Sistema Completo de Gestão de Documentos e Anexos (DMS) do IControlIT, responsável por armazenar, versionar, controlar acesso e rastrear o ciclo de vida completo de documentos e arquivos do sistema.</t>
+          <t>Implementar um Sistema Completo de Gestão de Documentos e Anexos (DMS) do IControlIT, responsável por armazenar, versionar, controlar acesso e rastrear o ciclo de vida completo de documentos e arqu...</t>
         </is>
       </c>
       <c r="D18" s="3" t="inlineStr">
         <is>
-          <t>TODO arquivo enviado DEVE passar por scan antivírus antes de ser armazenado. Sistema DEVE calcular e armazenar hash SHA-256 de todo arquivo para garantir integridade e detectar duplicatas. Alteração em documento existente DEVE criar automaticamente nova versão sem deletar anterior. Sistema DEVE implementar controle de acesso granular por documento via ACL. Documentos escaneados (PDFs de imagem, fotos) DEVEM ter OCR processado automaticamente para permitir busca full-text. Sistema DEVE permitir compartilhamento externo via links temporários seguros com expiração, senha e limite de acessos. Sistema DEVE enviar alertas automáticos para documentos próximos ao vencimento. Exclusão de documentos DEVE ser lógica (soft delete) com possibilidade de recuperação. Sistema DEVE impor limites de tamanho de arquivo conforme tipo e contexto. Sistema DEVE validar extensão e MIME type para garantir que apenas arquivos seguros sejam aceitos. Documentos marcados como confidenciais DEVEM ser criptografados em repouso (at-rest). TODA operação em documentos DEVE ser auditada para rastreabilidade e compliance. Sistema DEVE suportar busca full-text em nome, descrição, tags e texto extraído via OCR. Sistema DEVE permitir armazenar metadados adicionais específicos por tipo de documento via JSON. Todos os documentos DEVEM estar isolados por Fornecedor (multi-tenancy).</t>
+          <t>TODO arquivo enviado DEVE passar por scan antivírus antes de ser armazenado. Sistema DEVE calcular e armazenar hash SHA-256 de todo arquivo para garantir integridade e detectar duplicatas. Alteração em documento existente DEVE criar automaticamente nova versão sem deletar anterior. Sistema DEVE implementar controle de acesso granular por documento via ACL. Documentos escaneados (PDFs de imagem, fotos) DEVEM ter OCR processado automaticamente para permitir busca full-text.</t>
         </is>
       </c>
       <c r="E18" s="3" t="inlineStr"/>
@@ -872,19 +920,21 @@
           <t>RF021</t>
         </is>
       </c>
-      <c r="B19" s="3" t="inlineStr"/>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Catálogo de Serviços e Portal Self-Service</t>
+        </is>
+      </c>
       <c r="C19" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Implementar um Catálogo de Serviços e Portal Self-Service que permita aos usuários finais
+          <t>Implementar um Catálogo de Serviços e Portal Self-Service que permita aos usuários finais
 solicitar serviços de TI/Telecom de forma autônoma através de uma interface intuitiva
-estilo "carrinho de compras", com aprovação automatizada via workflow configurável,
-tracking visual de SLA e integração com sistemas de estoque e fornecedores.
-</t>
+estilo "carrinho de c...</t>
         </is>
       </c>
       <c r="D19" s="3" t="inlineStr">
         <is>
-          <t>Workflow de Aprovação Obrigatório - Todo serviço com Fl_Requer_Aprovacao = 1 deve passar por workflow configurável (gestor → TI → financeiro → diretor). Solicitação para Outro Usuário - Usuários com permissão Solicitar_Para_Terceiros podem criar solicitações em nome de terceiros (registrar ambos solicitante e beneficiário). Carrinho de Compras Temporário - Itens persistem entre sessões, máximo 10 serviços, limpeza automática após 30 dias. Validação de Estoque Automática - Serviços com Fl_Verifica_Estoque = 1 devem validar disponibilidade antes da aprovação, reservar item após aprovação, cancelar se não repor em 15 dias. SLA Tracking com Semáforo Visual - Cálculo automático considerando dias úteis, semáforo verde (&gt;50%), amarelo (20-50%), vermelho (&lt;20% ou vencido), job Hangfire verifica a cada 15 minutos. Formulários Dinâmicos por Serviço - JSON Schema armazenado em Formulario_JSON, validação dupla (client-side UX + server-side segurança). Provisionamento Automatizado - Serviços com Fl_Provisiona_Automatico = 1 chamam API do fornecedor após aprovação, callback atualiza status, erro gera notificação. Auto-Aprovação por Regras - Aprovação automática se: colaborador veterano (&gt;1 ano), valor baixo (&lt;R$ 500), serviço não-crítico, histórico positivo (&gt;10 solicitações concluídas). Avaliação de Serviço Obrigatória - Nota 1-5 estrelas + comentário opcional, notificações progressivas (imediato/24h/48h), atualizar Avaliacao_Media automaticamente. Limite de Solicitações Simultâneas - Máximo 5 solicitações Pendente/Em_Atendimento para usuário comum, 20 para Gestor/Diretor. Cancelamento de Solicitação - Permitido até início do atendimento (usuário), aprovador pode cancelar a qualquer momento, justificativa obrigatória (mínimo 20 caracteres), liberar reserva de estoque. Justificativa Obrigatória para Serviços Críticos - Serviços com Fl_Requer_Justificativa = 1 exigem campo Justificativa (50-1000 caracteres). Numeração Sequencial de Solicitações - Formato SRV-YYYY-NNNNN, gerado via sequence SQL Server, reset anual. Notificações em Cada Etapa do Workflow - Eventos: criada, aguardando aprovação, aprovada, rejeitada, em atendimento, concluída, SLA em risco, cancelada. Canais: e-mail + push + in-app. Analytics de Demanda para Gestão - Métricas: serviços mais solicitados, SLA médio, taxa de aprovação, tempo médio de aprovação, avaliação média, gargalos. Dashboard em tempo real com filtros e exportação.</t>
+          <t>Workflow de Aprovação Obrigatório - Todo serviço com Fl_Requer_Aprovacao = 1 deve passar por workflow configurável (gestor → TI → financeiro → diretor). Solicitação para Outro Usuário - Usuários com permissão Solicitar_Para_Terceiros podem criar solicitações em nome de terceiros (registrar ambos solicitante e beneficiário). Carrinho de Compras Temporário - Itens persistem entre sessões, máximo 10 serviços, limpeza automática após 30 dias. Validação de Estoque Automática - Serviços com Fl_Verifica_Estoque = 1 devem validar disponibilidade antes da aprovação, reservar item após aprovação, cancelar se não repor em 15 dias. SLA Tracking com Semáforo Visual - Cálculo automático considerando dias úteis, semáforo verde (&gt;50%), amarelo (20-50%), vermelho (&lt;20% ou vencido), job Hangfire verifica a cada 15 minutos.</t>
         </is>
       </c>
       <c r="E19" s="3" t="inlineStr"/>
@@ -895,19 +945,20 @@
           <t>RF022</t>
         </is>
       </c>
-      <c r="B20" s="3" t="inlineStr"/>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Especificar o comportamento esperado do sistema para gerenciar fornecedores e empresas contratadas,
-incluindo operadoras de telecomunicações, fornecedores de TI, prestadores de serviços e fabricantes.
-Este documento serve como contrato oficial entre negócio, desenvolvimento, testes e agentes de IA,
-definindo o que o sistema deve fazer, sem especificar implementação técnica.
-</t>
+          <t>Especificar o comportamento esperado do sistema para gerenciar fornecedores e empresas contratadas,
+incluindo operadoras de telecomunicações, fornecedores de TI, prestadores de serviços e fabricant...</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>CNPJ único por tenant. Validação de CNPJ. Validação de CPF. Tipo de fornecedor obrigatório. Nome obrigatório. Status válido. Não inativar fornecedor com contratos ativos. Validação de e-mail. Apenas um contato principal por tipo. Nota de avaliação válida. Cálculo automático de nota geral. Atualização automática de nota do fornecedor. Validação de documentos vencidos. Isolamento por tenant (multi-tenancy). Auditoria completa. Limite de crédito válido. Telefone obrigatório para contato. Validação de tipo de contato. Comentário obrigatório em avaliação negativa. Busca por nome parcial.</t>
+          <t>CNPJ único por tenant. Validação de CNPJ. Validação de CPF. Tipo de fornecedor obrigatório. Nome obrigatório.</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr"/>
@@ -918,15 +969,19 @@
           <t>RF023</t>
         </is>
       </c>
-      <c r="B21" s="3" t="inlineStr"/>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Contratos</t>
+        </is>
+      </c>
       <c r="C21" s="3" t="inlineStr">
         <is>
-          <t>Especificar o módulo de Gestão de Contratos do sistema IControlIT, responsável pela administração completa do ciclo de vida de contratos comerciais, de fornecimento, locação, manutenção e telecomunicações com fornecedores, operadoras e prestadores de serviço.</t>
+          <t>Especificar o módulo de Gestão de Contratos do sistema IControlIT, responsável pela administração completa do ciclo de vida de contratos comerciais, de fornecimento, locação, manutenção e telecomun...</t>
         </is>
       </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
-          <t>A data de término (DataFim) de um contrato deve ser sempre maior ou igual à data de início (DataInicio). Vigência máxima de 10 anos.. Cálculo automático de valor mensal proporcional dividindo ValorTotal pela quantidade de meses da vigência (30,44 dias/mês). Se ValorMensal informado, ValorTotal é recalculado.. Contratos com RenovacaoAutomatica = true são prolongados automaticamente quando a DataFim é atingida. Novo contrato criado, anterior marcado como Renovado.. Sistema gera alertas automáticos (e-mail + SignalR) para vencimento em 30, 60 ou 90 dias. Alertas gravados em AuditoriaAlerta para rastreamento e evitar duplicatas.. Workflow de aprovação baseado em faixas de valor configuráveis. State-machine: Rascunho → PendenteAprovacao → Aprovado/Rejeitado. Cada nível registra auditoria.. Contrato não pode ser excluído se possuir medições ou faturas associadas (FK em RF090). Retorna HTTP 409 Conflict informando quantidade exata.. Contratos com reajustes automáticos anuais conforme índice econômico (IGPM, IPCA, INPC). Reajuste calculado na data aniversário e aplicado a ValorMensal e ValorTotal.. Todo contrato deve estar associado a fornecedor válido (FK para RF022). CNPJ validado na criação/edição. CNPJ inválido ou fornecedor inativo retorna HTTP 400.. Todos os contratos isolados por ClienteId. Queries sempre filtram por ClienteId do usuário autenticado. Acesso cruzado retorna HTTP 403 Forbidden.. Contratos nunca deletados fisicamente. Soft delete marca IsDeleted = true, DataDelecao, DeletadoPor. Queries filtram IsDeleted = false automaticamente.</t>
+          <t>A data de término (DataFim) de um contrato deve ser sempre maior ou igual à data de início (DataInicio). Vigência máxima de 10 anos.. Cálculo automático de valor mensal proporcional dividindo ValorTotal pela quantidade de meses da vigência (30,44 dias/mês). Se ValorMensal informado, ValorTotal é recalculado.. Contratos com RenovacaoAutomatica = true são prolongados automaticamente quando a DataFim é atingida. Novo contrato criado, anterior marcado como Renovado.. Sistema gera alertas automáticos (e-mail + SignalR) para vencimento em 30, 60 ou 90 dias. Alertas gravados em AuditoriaAlerta para rastreamento e evitar duplicatas.. Workflow de aprovação baseado em faixas de valor configuráveis. State-machine: Rascunho → PendenteAprovacao → Aprovado/Rejeitado. Cada nível registra auditoria.</t>
         </is>
       </c>
       <c r="E21" s="3" t="inlineStr"/>
@@ -937,15 +992,19 @@
           <t>RF024</t>
         </is>
       </c>
-      <c r="B22" s="3" t="inlineStr"/>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Departamentos e Estrutura Organizacional</t>
+        </is>
+      </c>
       <c r="C22" s="3" t="inlineStr">
         <is>
-          <t>Fornecer CRUD completo de departamentos organizacionais com hierarquia recursiva ilimitada, gestão de líderes, lotação matricial, organograma visual, sincronização Azure AD, workflow de movimentações e analytics de força de trabalho.</t>
+          <t>Fornecer CRUD completo de departamentos organizacionais com hierarquia recursiva ilimitada, gestão de líderes, lotação matricial, organograma visual, sincronização Azure AD, workflow de movimentaçõ...</t>
         </is>
       </c>
       <c r="D22" s="3" t="inlineStr">
         <is>
-          <t>Código Departamento Único Alfanumérico. Hierarquia Multinível Ilimitada Self-Referencing. Validação Referências Circulares Hierarquia. Líder Obrigatório Usuário Válido FK. Sincronização Automática Azure AD. Workflow Aprovação Movimentações Multinível. Dotted-Line Soma Alocações ≤100%. Atualização Automática Qtd_Colaboradores. Organograma Visual D3.js Interativo. Notificação Líder Multicanal. Dashboard Headcount Tempo Real SignalR. Analytics Turnover Departamental. Relatório Movimentações RH Compliance. Integração Ponto Eletrônico Presença Física. Versionamento Change Tracking.</t>
+          <t>Código Departamento Único Alfanumérico. Hierarquia Multinível Ilimitada Self-Referencing. Validação Referências Circulares Hierarquia. Líder Obrigatório Usuário Válido FK. Sincronização Automática Azure AD.</t>
         </is>
       </c>
       <c r="E22" s="3" t="inlineStr"/>
@@ -956,19 +1015,20 @@
           <t>RF025</t>
         </is>
       </c>
-      <c r="B23" s="3" t="inlineStr"/>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>Gestão Completa de Ativos de TI e Telecom</t>
+        </is>
+      </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prover sistema completo de gestão de ativos de TI (notebooks, desktops, servidores, smartphones, tablets, impressoras)
-e Telecom (linhas móveis, fixas, aparelhos telefônicos) com rastreamento de ciclo de vida desde aquisição até baixa patrimonial,
-incluindo geração automática de QR Codes para identificação, controle de movimentações com geolocalização GPS,
-cálculo automático de depreciação contábil, alertas de vencimento de garantia e integração bidirecional com sistemas ERP.
-</t>
+          <t>Prover sistema completo de gestão de ativos de TI (notebooks, desktops, servidores, smartphones, tablets, impressoras)
+e Telecom (linhas móveis, fixas, aparelhos telefônicos) com rastreamento de ci...</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>Número de Patrimônio Único Global. QR Code Gerado Automaticamente. Status de Ativo com Transições Válidas. Alocação Requer Usuário Responsável. Histórico Completo de Movimentações (Chain of Custody). Depreciação Automática Mensal. Alertas de Garantia Automáticos. Validação de Campos Obrigatórios por Tipo. Geolocalização Obrigatória para Inventário Mobile. Baixa de Ativo Requer Aprovação. IMEI Validation para Smartphones. Isolamento Multi-Tenant Obrigatório. Soft Delete Obrigatório. Integração com Sistema de Patrimônio Externo. Inventário Periódico Obrigatório.</t>
+          <t>Número de Patrimônio Único Global. QR Code Gerado Automaticamente. Status de Ativo com Transições Válidas. Alocação Requer Usuário Responsável. Histórico Completo de Movimentações (Chain of Custody).</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr"/>
@@ -979,15 +1039,19 @@
           <t>RF026</t>
         </is>
       </c>
-      <c r="B24" s="3" t="inlineStr"/>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>Gestão Completa de Faturas de Telecom e TI</t>
+        </is>
+      </c>
       <c r="C24" s="3" t="inlineStr">
         <is>
-          <t>Prover capacidade completa de gestão de faturas de serviços de Telecom e TI com importação automatizada multi-layout, conciliação inteligente contra contratos, auditoria configurável pré-pagamento, rateio multi-dimensional, workflow de contestação formal e dashboard executivo com alertas preditivos de estouro de budget.</t>
+          <t>Prover capacidade completa de gestão de faturas de serviços de Telecom e TI com importação automatizada multi-layout, conciliação inteligente contra contratos, auditoria configurável pré-pagamento,...</t>
         </is>
       </c>
       <c r="D24" s="3" t="inlineStr">
         <is>
-          <t>Importação Suporta Múltiplos Layouts. OCR de PDF com Azure Form Recognizer. Conciliação Automática de Linhas com Contratos. Auditoria Pré-Pagamento com Regras Configuráveis. Workflow de Contestação Formal. Rateio Multi-Dimensional Automático. Dashboard Executivo com KPIs Críticos. Alertas Preditivos de Estouro de Budget. Integração com APIs de Operadoras. Aprovação Mobile com Assinatura Digital. Isolamento Multi-Tenant Obrigatório. Soft Delete Obrigatório. Histórico de Versões de Fatura. Integração com ERP Financeiro. Campos Obrigatórios por Status.</t>
+          <t>Importação Suporta Múltiplos Layouts. OCR de PDF com Azure Form Recognizer. Conciliação Automática de Linhas com Contratos. Auditoria Pré-Pagamento com Regras Configuráveis. Workflow de Contestação Formal.</t>
         </is>
       </c>
       <c r="E24" s="3" t="inlineStr"/>
@@ -998,20 +1062,21 @@
           <t>RF027</t>
         </is>
       </c>
-      <c r="B25" s="3" t="inlineStr"/>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
       <c r="C25" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fornecer sistema completo de gestão de aditivos contratuais para contratos de Telecom e TI,
+          <t>Fornecer sistema completo de gestão de aditivos contratuais para contratos de Telecom e TI,
 permitindo controle rigoroso de versões, workflow de aprovação multi-nível, cálculo automático
-de impacto financeiro, rastreamento de prazos, alertas de renovação automática e rastreabilidade
-jurídica completa. Este documento define o que o sistema deve fazer, servindo como contrato oficial
-entre negócio, desenvolvimento, testes e agentes de IA.
-</t>
+de impacto...</t>
         </is>
       </c>
       <c r="D25" s="3" t="inlineStr">
         <is>
-          <t>8 Tipos de Aditivos Suportados. Wizard Multi-Step com Validações Progressivas. Cálculo Automático de Impacto Financeiro. Versionamento Completo de Contratos. Workflow de Aprovação Multi-Nível. Library Jurídica de Cláusulas. Gestão Documental Integrada. Alertas Inteligentes de Vencimento. Dashboard Pipeline de Aditivos. Comparação Visual entre Versões. Validação de Vigência e Datas. Isolamento Multi-Tenant Obrigatório. Soft Delete Obrigatório. Cálculo de Multas Rescisórias. Integração com Sistema Jurídico Externo.</t>
+          <t>8 Tipos de Aditivos Suportados. Wizard Multi-Step com Validações Progressivas. Cálculo Automático de Impacto Financeiro. Versionamento Completo de Contratos. Workflow de Aprovação Multi-Nível.</t>
         </is>
       </c>
       <c r="E25" s="3" t="inlineStr"/>
@@ -1022,7 +1087,11 @@
           <t>RF028</t>
         </is>
       </c>
-      <c r="B26" s="3" t="inlineStr"/>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de SLA - Operações</t>
+        </is>
+      </c>
       <c r="C26" s="3" t="inlineStr">
         <is>
           <t>Especificar o módulo de Gestão de SLA para Operações do sistema IControlIT, responsável por definir, monitorar e garantir o cumprimento de Service Level Agreements (SLAs) para operações de ativos.</t>
@@ -1030,7 +1099,7 @@
       </c>
       <c r="D26" s="3" t="inlineStr">
         <is>
-          <t>Tempo de resposta deve ser sempre menor que tempo de resolução, que deve ser menor que tempo de atendimento.. Contador de SLA não inclui períodos de pausa (fora horário, aguardando cliente) e feriados nacionais.. Pausa automática quando operação sai do horário de atendimento, retoma ao voltar.. Alertas em cascata gerados em 50%, 75%, 90%, 100% de SLA consumido.. Escalação automática quando SLA atinge 90% (Level 2), 100% (Level 3/Manager).. Prioridade P1: 2h resposta, 4h resolução, 8h atendimento (ativos críticos).. Prioridade P2: 4h resposta, 8h resolução, 24h atendimento (ativos importantes).. Prioridade P3: 8h resposta, 24h resolução, 48h atendimento (ativos padrão).. Prioridade P4: 24h resposta, 72h resolução, 5 dias atendimento (ativos não essenciais).. Multi-tenancy obrigatório por ClienteId. Isolamento total de dados por cliente.. Soft delete via IsDeleted = true. Nunca deleta permanentemente.. Integração com BrasilAPI para obter feriados nacionais/estaduais. Feriados excluídos do cálculo.</t>
+          <t>Tempo de resposta deve ser sempre menor que tempo de resolução, que deve ser menor que tempo de atendimento.. Contador de SLA não inclui períodos de pausa (fora horário, aguardando cliente) e feriados nacionais.. Pausa automática quando operação sai do horário de atendimento, retoma ao voltar.. Alertas em cascata gerados em 50%, 75%, 90%, 100% de SLA consumido.. Escalação automática quando SLA atinge 90% (Level 2), 100% (Level 3/Manager).</t>
         </is>
       </c>
       <c r="E26" s="3" t="inlineStr"/>
@@ -1041,7 +1110,11 @@
           <t>RF029</t>
         </is>
       </c>
-      <c r="B27" s="3" t="inlineStr"/>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de SLA - Serviços</t>
+        </is>
+      </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
           <t>Gerenciar Service Level Agreements (SLAs) para serviços de TI do catálogo (RF021) e chamados/tickets (RF073, RF074).</t>
@@ -1049,7 +1122,7 @@
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>Matriz de Priorização Impacto × Urgência: Prioridade determinada automaticamente pelo cruzamento. Metas P1 (Crítico): resposta 15min, resolução 4h. Metas P2 (Alto): resposta 1h, resolução 8h. Metas P3 (Médio): resposta 4h, resolução 24h. Metas P4 (Baixo): resposta 8h, resolução 72h. Pausa Automática Fora de Horário de Atendimento: SLA pausa fora do horário configurado (comercial/24x7/plantão). Alertas em Cascata: notificações automáticas em 50%, 75%, 90%, 100% de consumo com severidade crescente. Escalação Automática Quando SLA Viola: quando SLA atinge 100%, escala para nível técnico superior. Cálculo de SLA Exclui Pausas e Feriados: tempo em pausa e feriados NÃO contam no consumo. Isolamento Multi-Tenancy por ClienteId: toda entidade SLA deve ter ClienteId. Soft Delete com IsDeleted: exclusão lógica preserva auditoria. Integração BrasilAPI para Feriados: cachear feriados nacionais para cálculo correto de SLA. Campos Obrigatórios: ServicoId, Prioridade, TempoResposta, TempoResolucao, HorarioAtendimento, ClienteId. Unicidade de SLA: um serviço pode ter no máximo um SLA por combinação de prioridade e cliente.</t>
+          <t>Matriz de Priorização Impacto × Urgência: Prioridade determinada automaticamente pelo cruzamento. Metas P1 (Crítico): resposta 15min, resolução 4h. Metas P2 (Alto): resposta 1h, resolução 8h. Metas P3 (Médio): resposta 4h, resolução 24h. Metas P4 (Baixo): resposta 8h, resolução 72h.</t>
         </is>
       </c>
       <c r="E27" s="3" t="inlineStr"/>
@@ -1060,19 +1133,21 @@
           <t>RF030</t>
         </is>
       </c>
-      <c r="B28" s="3" t="inlineStr"/>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Parâmetros de Faturamento</t>
+        </is>
+      </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Estabelecer o sistema de configuração centralizada de parâmetros, regras e templates
+          <t>Estabelecer o sistema de configuração centralizada de parâmetros, regras e templates
 para o processo de faturamento, permitindo a gestão de layouts de importação, regras de
-auditoria automática, templates de rateio e parâmetros fiscais com versionamento completo
-e rastreabilidade.
-</t>
+auditoria automática, te...</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>Todo layout de importação deve validar no mínimo 5 campos obrigatórios (CNPJ fornecedor, número fatura, data vencimento, valor total, descrição). Sistema deve validar 100% das linhas ANTES de gravar qualquer registro (modo transacional all-or-nothing). Alterações em layouts, regras ou parâmetros críticos devem criar nova versão com justificativa obrigatória (mínimo 50 caracteres). Toda regra de auditoria deve ter severidade definida (Informativa, Alerta, Bloqueante). Templates de rateio com distribuição percentual devem ter soma exata de 100% (tolerância ±0.01%). Layouts novos devem ser testados em sandbox com arquivo exemplo (mínimo 10 linhas) antes de ativação. Alíquotas e parâmetros fiscais devem ter data de vigência (início/fim) sem sobreposição. Mudanças em parâmetros críticos devem gerar auditoria automática com before/after e notificar gestor fiscal. Importação de faturas deve validar se fornecedor está homologado e ativo com documentação atualizada (certidões &lt; 90 dias). Templates de rateio com valores fixos devem ter soma igual ao total da fatura (tolerância ±R$ 0.01). Regras de auditoria configuradas como expressões devem ser validadas sintaticamente antes de salvar. Logs de importação devem ser retidos por 7 anos (compliance LGPD + fiscal) com soft delete. Falhas em importações automáticas devem notificar responsável em até 5 minutos via in-app/e-mail/SMS. Importações via upload manual devem ter limite configurável por perfil (Admin: 100k, Manager: 50k, Analyst: 10k). Dashboard de qualidade deve atualizar em tempo real via SignalR (latência máxima 5 segundos).</t>
+          <t>Todo layout de importação deve validar no mínimo 5 campos obrigatórios (CNPJ fornecedor, número fatura, data vencimento, valor total, descrição). Sistema deve validar 100% das linhas ANTES de gravar qualquer registro (modo transacional all-or-nothing). Alterações em layouts, regras ou parâmetros críticos devem criar nova versão com justificativa obrigatória (mínimo 50 caracteres). Toda regra de auditoria deve ter severidade definida (Informativa, Alerta, Bloqueante). Templates de rateio com distribuição percentual devem ter soma exata de 100% (tolerância ±0.01%).</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr"/>
@@ -1090,17 +1165,14 @@
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Prover sistema completo de gestão de plano de contas contábil multi-dimensional que permita
+          <t>Prover sistema completo de gestão de plano de contas contábil multi-dimensional que permita
 classificação, rateio e análise financeira de despesas de Telecom e TI, eliminando re-trabalho
-manual de classificação (de 120h/mês para 5h/mês), garantindo conformidade fiscal com
-rastreabilidade total para auditorias externas e fornecendo visibilidade multi-dimensional de
-custos para tomada de decisão estratégica.
-</t>
+manual de ...</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>Estrutura Hierárquica Configurável até 7 Níveis. Builder Visual com Preview de Impacto. Centros de Custo com Hierarquia Organizacional. Dimensões Customizáveis Ilimitadas. Regras de Classificação Automática. Importação Multi-Layout de ERPs. Exportação Lançamentos D-E (Débito-Crédito). Relatórios DRE Multi-Dimensionais. Orçamento vs. Realizado com Alertas. Auditoria Completa com Trilha de Mudanças. Validação Contábil com 20+ Regras Fiscais. Reconciliação Automática com Fuzzy Matching. Integração Bidirecional com ERP Financeiro. Isolamento Multi-Tenant com Row-Level Security. Soft Delete com Histórico Versionado.</t>
+          <t>Estrutura Hierárquica Configurável até 7 Níveis. Builder Visual com Preview de Impacto. Centros de Custo com Hierarquia Organizacional. Dimensões Customizáveis Ilimitadas. Regras de Classificação Automática.</t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr"/>
@@ -1111,7 +1183,11 @@
           <t>RF032</t>
         </is>
       </c>
-      <c r="B30" s="3" t="inlineStr"/>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Notas Fiscais e Faturas</t>
+        </is>
+      </c>
       <c r="C30" s="3" t="inlineStr">
         <is>
           <t>Implementar gestão completa do ciclo de vida de Notas Fiscais Eletrônicas (NF-e) com importação, validação, conciliação, cálculo de impostos, rateio e conformidade fiscal.</t>
@@ -1119,7 +1195,7 @@
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>Importação de NF-e com Validação de Estrutura XML (schema XSD 4.00 SEFAZ). Validação de Assinatura Digital (RSA-2048 com SHA-256, ICP-Brasil). Consulta Automática de Status na SEFAZ (autorizada, rejeitada, cancelada). Detecção de Divergências entre NF-e e Pedido (&lt;1% auto-ajuste, &gt;5% bloqueio). Cálculo Automático de Impostos (ICMS, IPI, PIS, COFINS, ISS, retenções). Bloqueio de Pagamento se Divergência Crítica não Aprovada. Rateio Automático entre Filiais/Centros de Custo (soma 100%, tolerância 0,01%). Armazenamento Permanente XML e DANFE em Azure Blob Storage (7 anos LGPD). OCR de DANFE em PDF quando XML Indisponível (Azure Cognitive + Tesseract). Auditoria Completa com Retenção de 7 Anos (LGPD, SOX).</t>
+          <t>Importação de NF-e com Validação de Estrutura XML (schema XSD 4.00 SEFAZ). Validação de Assinatura Digital (RSA-2048 com SHA-256, ICP-Brasil). Consulta Automática de Status na SEFAZ (autorizada, rejeitada, cancelada). Detecção de Divergências entre NF-e e Pedido (&lt;1% auto-ajuste, &gt;5% bloqueio). Cálculo Automático de Impostos (ICMS, IPI, PIS, COFINS, ISS, retenções).</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr"/>
@@ -1130,15 +1206,19 @@
           <t>RF033</t>
         </is>
       </c>
-      <c r="B31" s="3" t="inlineStr"/>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Chamados (Service Desk)</t>
+        </is>
+      </c>
       <c r="C31" s="3" t="inlineStr">
         <is>
-          <t>Implementar sistema completo de Service Desk para gerenciamento de chamados de suporte técnico, solicitações de serviços e incidentes, com controle de SLA, distribuição por filas, avaliação de satisfação e métricas em tempo real.</t>
+          <t>Implementar sistema completo de Service Desk para gerenciamento de chamados de suporte técnico, solicitações de serviços e incidentes, com controle de SLA, distribuição por filas, avaliação de sati...</t>
         </is>
       </c>
       <c r="D31" s="3" t="inlineStr">
         <is>
-          <t>Campos obrigatórios na abertura: título, data solicitação, usuário solicitante, tipo solicitação, tipo ativo. Cálculo automático de SLA considerando apenas dias úteis e excluindo datas de parada. Validação de transições de status conforme workflow. Solução obrigatória ao encerrar chamado. Alertas visuais e notificações quando SLA atingir 80% ou 100%. Avaliação de satisfação opcional, mas se informada deve ter nota 1-5. Interações podem ser públicas (visíveis ao solicitante) ou privadas (apenas equipe). Atribuição a fila de atendimento obrigatória. Vinculação a ativo ou consumidor opcional. Notificações automáticas em eventos-chave (abertura, atribuição, status, SLA, encerramento, avaliação). Reabertura permitida até 7 dias após encerramento. Prazo SLA pausado em status 'Aguardando Usuário' ou 'Aguardando Fornecedor'. Anexos: limite 10 MB por arquivo, 50 MB total por chamado. Escalação automática para supervisor quando SLA vencido. Soluções podem ser marcadas como base de conhecimento para reutilização. Isolamento multi-tenant: usuário acessa apenas chamados do seu Fornecedor. Unicidade de avaliação: apenas 1 avaliação por chamado.</t>
+          <t>Campos obrigatórios na abertura: título, data solicitação, usuário solicitante, tipo solicitação, tipo ativo. Cálculo automático de SLA considerando apenas dias úteis e excluindo datas de parada. Validação de transições de status conforme workflow. Solução obrigatória ao encerrar chamado. Alertas visuais e notificações quando SLA atingir 80% ou 100%.</t>
         </is>
       </c>
       <c r="E31" s="3" t="inlineStr"/>
@@ -1149,11 +1229,19 @@
           <t>RF034</t>
         </is>
       </c>
-      <c r="B32" s="3" t="inlineStr"/>
-      <c r="C32" s="3" t="inlineStr"/>
+      <c r="B32" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>Vinculação Obrigatória a Resumo e Bilhete. Cálculo Automático de Glosa. Precisão Numérica Conforme Padrão Telecomunicações. Quantidade de Consumo Positiva. Validação de Relacionamentos Obrigatórios. Sincronização Automática com Resumo de Auditoria. Validação de Lote (Formato AAAAMM). Exportação Estruturada para Contestação. Auditoria Completa de Operações. Filtros Avançados por Unidade de Consumo. Validação de Valores Conforme Tipo de Bilhete. Soft Delete com Recálculo de Agregados. Multi-Tenancy Obrigatório com Row-Level Security. Índices para Performance em Consultas Analíticas. Exportação para Excel com Detalhamento Completo.</t>
+          <t>Vinculação Obrigatória a Resumo e Bilhete. Cálculo Automático de Glosa. Precisão Numérica Conforme Padrão Telecomunicações. Quantidade de Consumo Positiva. Validação de Relacionamentos Obrigatórios.</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr"/>
@@ -1164,7 +1252,11 @@
           <t>RF035</t>
         </is>
       </c>
-      <c r="B33" s="3" t="inlineStr"/>
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Resumos de Auditoria</t>
+        </is>
+      </c>
       <c r="C33" s="3" t="inlineStr">
         <is>
           <t>Consolidar, analisar e gerar relatórios gerenciais de auditorias de faturas de telecomunicações através de resumos agregados por período, operadora, tipo de serviço e lote.</t>
@@ -1172,7 +1264,7 @@
       </c>
       <c r="D33" s="3" t="inlineStr">
         <is>
-          <t>Consolidação automática diária com agrupamento multi-dimensional. Cálculo automático e validado de totalizadores. Análise comparativa automática entre períodos. Cálculo de indicadores de performance. Alertas de desvios automáticos. Drill-down com preservação de contexto. Integração bidirecional com lotes (RF054). Exportação em múltiplos formatos. Row-Level Security por ClienteId. Auditoria completa de alterações. Validação de integridade referencial.</t>
+          <t>Consolidação automática diária com agrupamento multi-dimensional. Cálculo automático e validado de totalizadores. Análise comparativa automática entre períodos. Cálculo de indicadores de performance. Alertas de desvios automáticos.</t>
         </is>
       </c>
       <c r="E33" s="3" t="inlineStr"/>
@@ -1183,15 +1275,19 @@
           <t>RF036</t>
         </is>
       </c>
-      <c r="B34" s="3" t="inlineStr"/>
+      <c r="B34" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Custos Fixos</t>
+        </is>
+      </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>Implementar sistema completo para gerenciamento de despesas recorrentes mensais (custos fixos) com provisionamento automático, controle de variações orçamentárias, detecção de anomalias e análise de tendências.</t>
+          <t>Implementar sistema completo para gerenciamento de despesas recorrentes mensais (custos fixos) com provisionamento automático, controle de variações orçamentárias, detecção de anomalias e análise d...</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>Campos obrigatórios no cadastro (Descricao, TipoCustoFixoId, ValorOrcadoMensal, DataInicio, Status). Provisionamento automático mensal no 1º dia útil do mês. Alertas de variação orçamentária em 3 níveis (10%, 20%, 30%). Justificativa obrigatória para variações &gt;20%. Aprovação gerencial obrigatória para variações &gt;30%. Rateio multi-dimensional com soma dos percentuais = 100%. Detecção automática de anomalias estatísticas (média + 2σ). Data de fim opcional mas se informada deve ser &gt; DataInicio. Vinculação opcional a fornecedor e/ou contrato. Status do custo fixo (Ativo, Inativo, Suspenso, Cancelado). Alertas de vencimento em 7, 3 e 1 dia antes. Bloqueio de edição de lançamentos com Status = Pago. Isolamento multi-tenant por FornecedorId.</t>
+          <t>Campos obrigatórios no cadastro (Descricao, TipoCustoFixoId, ValorOrcadoMensal, DataInicio, Status). Provisionamento automático mensal no 1º dia útil do mês. Alertas de variação orçamentária em 3 níveis (10%, 20%, 30%). Justificativa obrigatória para variações &gt;20%. Aprovação gerencial obrigatória para variações &gt;30%.</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr"/>
@@ -1202,7 +1298,11 @@
           <t>RF037</t>
         </is>
       </c>
-      <c r="B35" s="3" t="inlineStr"/>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Custos por Ativo (TCO)</t>
+        </is>
+      </c>
       <c r="C35" s="3" t="inlineStr">
         <is>
           <t>Implementar um sistema completo de TCO (Total Cost of Ownership) para rastreamento, análise e otimização de todos os custos associados a ativos específicos ao longo de seu ciclo de vida.</t>
@@ -1210,7 +1310,7 @@
       </c>
       <c r="D35" s="3" t="inlineStr">
         <is>
-          <t>Campos obrigatórios: AtivoId, TipoCustoAtivoId, Valor, DataOcorrencia, Categoria. Recalcular TCO automaticamente ao criar, editar ou excluir custo. Depreciação automática mensal no dia 1 às 02:00 UTC para ativos depreciáveis. Calcular ROI = ((Benefícios - Custos) / Custos) * 100. Alertar quando TCO &gt; 130% da média de ativos do mesmo tipo. Custos de manutenção vinculados a OrdemServico, licenças a Contrato. Categorizar custos como CAPEX (Aquisicao) ou OPEX (demais). Projetar custos futuros baseado em média dos últimos 12 meses. Comparar TCO entre ativos do mesmo tipo e classificar (Econômico/Normal/Custoso). DataOcorrencia não pode ser anterior à DataAquisicao do ativo. Soft delete com recálculo automático de TCO. Visualizar TCO agregado por período (mensal, trimestral, anual). Exportar relatório de TCO em Excel/PDF com breakdown por categoria. Recomendar substituição quando TCO anual &gt; 50% do valor de ativo novo. Auditoria completa com retenção de 7 anos (LGPD). Isolamento por tenant (FornecedorId).</t>
+          <t>Campos obrigatórios: AtivoId, TipoCustoAtivoId, Valor, DataOcorrencia, Categoria. Recalcular TCO automaticamente ao criar, editar ou excluir custo. Depreciação automática mensal no dia 1 às 02:00 UTC para ativos depreciáveis. Calcular ROI = ((Benefícios - Custos) / Custos) * 100. Alertar quando TCO &gt; 130% da média de ativos do mesmo tipo.</t>
         </is>
       </c>
       <c r="E35" s="3" t="inlineStr"/>
@@ -1221,7 +1321,11 @@
           <t>RF038</t>
         </is>
       </c>
-      <c r="B36" s="3" t="inlineStr"/>
+      <c r="B36" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de SLA Solicitações</t>
+        </is>
+      </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
           <t>Implementar sistema completo de SLA para solicitações de TI com cálculo automático, monitoramento em tempo real e compliance contratual</t>
@@ -1229,7 +1333,7 @@
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>Cálculo automático de prazo considerando tipo, prioridade, horário de atendimento e feriados. Alertas escalonados em 4 níveis (50%, 80%, 100%, breach). Escalação automática quando prazo é ultrapassado sem resolução. Pausa e retomada de SLA com recálculo automático de prazo. Horário de atendimento configurável (8x5, 12x5, 24x7, customizado). Calendário de feriados exclui dias do cálculo de SLA. Extensão de prazo requer justificativa e aprovação (máximo 2 por solicitação). Dashboard em tempo real com cores por proximidade do prazo (verde/amarelo/vermelho/preto). Relatório de compliance calcula taxa de cumprimento de SLA. Notificações push (SignalR) para supervisores em eventos críticos. Análise de tendências identifica melhoria ou piora sustentada (3+ meses). Heatmap de horários críticos exibe volume de breaches por dia/hora. SLA diferenciado por nível de cliente (Bronze/Prata/Ouro/Platinum com ajuste -20%/-40%/-50%). Breach gera automaticamente não-conformidade que requer análise de causa raiz e plano de ação. Cálculo de MTTR por tipo, prioridade e equipe (deve ser &lt; 80% do SLA).</t>
+          <t>Cálculo automático de prazo considerando tipo, prioridade, horário de atendimento e feriados. Alertas escalonados em 4 níveis (50%, 80%, 100%, breach). Escalação automática quando prazo é ultrapassado sem resolução. Pausa e retomada de SLA com recálculo automático de prazo. Horário de atendimento configurável (8x5, 12x5, 24x7, customizado).</t>
         </is>
       </c>
       <c r="E36" s="3" t="inlineStr"/>
@@ -1240,11 +1344,19 @@
           <t>RF039</t>
         </is>
       </c>
-      <c r="B37" s="3" t="inlineStr"/>
-      <c r="C37" s="3" t="inlineStr"/>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C37" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D37" s="3" t="inlineStr">
         <is>
-          <t>Importação Automatizada via FTP. Parser Inteligente Multi-Formato. Normalização de Números para E.164. Detecção de Ligações para Números Premium. Alerta de Roaming Internacional. Rateio Automático por Centro de Custo. Comparação Uso Real vs Plano Contratado. Detecção de Padrão de Uso Suspeito. Relatório Top 10 Maiores Consumidores. Simulador de Planos Alternativos. Exportação para ERP. Análise de Horário de Pico. Processamento OCR de PDFs. Dashboard de Evolução de Custos. Política de Uso Aceitável e Compliance.</t>
+          <t>Importação Automatizada via FTP. Parser Inteligente Multi-Formato. Normalização de Números para E.164. Detecção de Ligações para Números Premium. Alerta de Roaming Internacional.</t>
         </is>
       </c>
       <c r="E37" s="3" t="inlineStr"/>
@@ -1255,15 +1367,19 @@
           <t>RF040</t>
         </is>
       </c>
-      <c r="B38" s="3" t="inlineStr"/>
+      <c r="B38" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Troncos Telefônicos</t>
+        </is>
+      </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>Implementar sistema completo de gerenciamento de troncos telefônicos (SIP, E1/R2, analógicos), incluindo monitoramento de disponibilidade em tempo real, análise de capacidade versus utilização, detecção automática de falhas, balanceamento de carga, custeio detalhado por tronco, integração com PABX/gateways e relatórios de QoS (Quality of Service).</t>
+          <t>Implementar sistema completo de gerenciamento de troncos telefônicos (SIP, E1/R2, analógicos), incluindo monitoramento de disponibilidade em tempo real, análise de capacidade versus utilização, det...</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
         <is>
-          <t>Monitoramento contínuo de troncos a cada 30 segundos usando protocolos apropriados (SIP OPTIONS, SNMP GET, API REST). Cálculo automático de MOS score usando algoritmo E-Model (ITU-T G.107) baseado em jitter, latência e packet loss. Failover automático em menos de 5 segundos após 3 falhas consecutivas (90 segundos). Balanceamento de carga com algoritmo Least Call Count (menor número de chamadas ativas). Alerta de congestionamento se utilização &gt;80% por &gt;5 minutos consecutivos. Análise de capacidade versus utilização mensal com classificação (Ocioso &lt;30%, Adequado 30-80%, Congestionado &gt;80%). Custeio detalhado por tronco com rateio por centro de custo baseado em minutos utilizados. Cálculo de MTBF (Mean Time Between Failures) e MTTR (Mean Time To Repair) para análise de confiabilidade. Relatório mensal de disponibilidade com comparação SLA (99,9% típico) e cálculo de créditos. Integração com PABX via API REST e SNMP para controle de roteamento e coleta de métricas. Dashboard de QoS atualizado a cada 30 segundos via SignalR com histórico de 90 dias. Simulador de economia para migração SIP vs E1 com cálculo de ROI e break-even point. Detecção de loops (&gt;10 chamadas mesmo número em &lt;5 min) e chamadas anômalas com bloqueio automático. Análise comparativa de TCO (Total Cost of Ownership) por tecnologia (E1, SIP, analógico) em 3 anos. Integração com gestão de bilhetes telefônicos (RF039) para análise cruzada de custo e qualidade.</t>
+          <t>Monitoramento contínuo de troncos a cada 30 segundos usando protocolos apropriados (SIP OPTIONS, SNMP GET, API REST). Cálculo automático de MOS score usando algoritmo E-Model (ITU-T G.107) baseado em jitter, latência e packet loss. Failover automático em menos de 5 segundos após 3 falhas consecutivas (90 segundos). Balanceamento de carga com algoritmo Least Call Count (menor número de chamadas ativas). Alerta de congestionamento se utilização &gt;80% por &gt;5 minutos consecutivos.</t>
         </is>
       </c>
       <c r="E38" s="3" t="inlineStr"/>
@@ -1274,11 +1390,19 @@
           <t>RF041</t>
         </is>
       </c>
-      <c r="B39" s="3" t="inlineStr"/>
-      <c r="C39" s="3" t="inlineStr"/>
+      <c r="B39" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C39" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D39" s="3" t="inlineStr">
         <is>
-          <t>Entrada Compra Vinculada NF. Entrada Devolução Vinculada Ativo. Ajuste Manual Requer Justificativa. Ajuste &gt;10 Unidades Requer Aprovação. Auditoria Completa Movimentações. Saída Não Excede Saldo Disponível. Distribuição Cria Ativo Automaticamente. Descarte Requer Motivo e Laudo. Saída &gt;10 Unidades Requer Aprovação. Rastreáveis Devem Ter Saída Individual. Transferência Requer Aprovação Gestor Origem. Saldo Deduzido Após Confirmação Envio. Saldo Adicionado Após Confirmação Recebimento. Alerta Transferência &gt;15 Dias. Recebimento Deve Conferir Quantidade. Saldo Exibe Valor Total R$. Histórico Imutável. Exportação Registrada Auditoria. Rastreamento IMEI Timeline Completa. Reserva Não Excede Saldo Disponível. Reserva Validade Máxima 30 Dias. Reserva Expirada Libera Saldo. Cancelamento Reserva Requer Justificativa. Job Noturno Reservas Expiradas. Job Níveis Estoque Cada 1 Hora. Alertas Email + In-App. Alerta Não Reenviado Até Normalização. Configuração Níveis Permissão Gestor.</t>
+          <t>Entrada Compra Vinculada NF. Entrada Devolução Vinculada Ativo. Ajuste Manual Requer Justificativa. Ajuste &gt;10 Unidades Requer Aprovação. Auditoria Completa Movimentações.</t>
         </is>
       </c>
       <c r="E39" s="3" t="inlineStr"/>
@@ -1289,11 +1413,19 @@
           <t>RF042</t>
         </is>
       </c>
-      <c r="B40" s="3" t="inlineStr"/>
-      <c r="C40" s="3" t="inlineStr"/>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D40" s="3" t="inlineStr">
         <is>
-          <t>Importação Automática de E-mails com XML NFe. Validação Automática na SEFAZ. OCR de PDFs com Fallback para Busca na SEFAZ. Conciliação Automática NFe ↔ Pedido de Compra. Cálculo Automático de Impostos Conforme Legislação Vigente. Rateio Proporcional de Frete por Peso ou Valor. Lançamento Automático no Estoque Após Aprovação. Workflow de Aprovação com SLA Configurável. Geração Automática de DANFE em PDF/A com QR Code. Detecção de Duplicatas por Chave de Acesso. Integração com ERP via API REST. Alertas em Tempo Real via SignalR. Retenção de XML Original por 7 Anos (Legislação Fiscal). Dashboard Executivo de Notas Fiscais. Multi-tenancy com Limite de NFes por Plano.</t>
+          <t>Importação Automática de E-mails com XML NFe. Validação Automática na SEFAZ. OCR de PDFs com Fallback para Busca na SEFAZ. Conciliação Automática NFe ↔ Pedido de Compra. Cálculo Automático de Impostos Conforme Legislação Vigente.</t>
         </is>
       </c>
       <c r="E40" s="3" t="inlineStr"/>
@@ -1304,11 +1436,19 @@
           <t>RF043</t>
         </is>
       </c>
-      <c r="B41" s="3" t="inlineStr"/>
-      <c r="C41" s="3" t="inlineStr"/>
+      <c r="B41" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D41" s="3" t="inlineStr">
         <is>
-          <t>Validação Automática de CEP via ViaCEP. Geocodificação Automática com Google Maps API. Cálculo Automático de Frete com Múltiplas Transportadoras. Endereço Padrão por Tipo de Solicitação. Histórico Completo de Entregas por Endereço. Notificações de Rastreamento em Tempo Real. Mapa de Calor de Entregas por Região. Autocomplete de Endereços Salvos. Validação de Endereço Duplicado. Exportação de Relatório de Entregas.</t>
+          <t>Validação Automática de CEP via ViaCEP. Geocodificação Automática com Google Maps API. Cálculo Automático de Frete com Múltiplas Transportadoras. Endereço Padrão por Tipo de Solicitação. Histórico Completo de Entregas por Endereço.</t>
         </is>
       </c>
       <c r="E41" s="3" t="inlineStr"/>
@@ -1319,7 +1459,11 @@
           <t>RF044</t>
         </is>
       </c>
-      <c r="B42" s="3" t="inlineStr"/>
+      <c r="B42" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de KPIs (Key Performance Indicators)</t>
+        </is>
+      </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
           <t>Implementar motor completo de KPIs para monitoramento estratégico e operacional do sistema IControlIT</t>
@@ -1327,7 +1471,7 @@
       </c>
       <c r="D42" s="3" t="inlineStr">
         <is>
-          <t>Unicidade de Código de KPI - Formato KPI-{CATEGORIA}-{SEQUENCIAL}. Validação de Fórmula de Cálculo - SQL query válida retornando valor numérico. Periodicidade Mínima por Fonte de Dados - API externa: min 1h. Hierarquia de Metas - Soma de metas filhas ≤ 100% meta pai. Semáforo Automático - Cálculo baseado em % de atingimento. Alerta de Tendência - Disparo com 3 dias de antecedência. Anomalia Estatística - Alerta se |z-score| &gt; 3. Drill-Down - Navegação até transação individual obrigatória. Recalculo Automático - Conforme periodicidade configurada. Cooldown de Alertas - Mínimo 1 hora entre alertas iguais. Versionamento de Fórmulas - Alteração cria nova versão. Permissões por Categoria - RBAC filtra KPIs por categoria. Dashboard Público - Token JWT temporário (1-30 dias). Agregação Inteligente - Operação apropriada (SUM, AVG, MAX, MIN). Retenção de Dados - Histórico de 7 anos conforme LGPD.</t>
+          <t>Unicidade de Código de KPI - Formato KPI-{CATEGORIA}-{SEQUENCIAL}. Validação de Fórmula de Cálculo - SQL query válida retornando valor numérico. Periodicidade Mínima por Fonte de Dados - API externa: min 1h. Hierarquia de Metas - Soma de metas filhas ≤ 100% meta pai. Semáforo Automático - Cálculo baseado em % de atingimento.</t>
         </is>
       </c>
       <c r="E42" s="3" t="inlineStr"/>
@@ -1338,7 +1482,11 @@
           <t>RF045</t>
         </is>
       </c>
-      <c r="B43" s="3" t="inlineStr"/>
+      <c r="B43" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Volumetria</t>
+        </is>
+      </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
           <t>Implementar sistema completo de monitoramento, análise e previsão de consumo de recursos computacionais e tráfego de dados do IControlIT</t>
@@ -1346,7 +1494,7 @@
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>Dados coletados a cada request (1s) mas armazenados apenas 7 dias. Agregações horárias ficam 90 dias, diárias 2 anos, mensais 7 anos. Todo fornecedor deve ter quota mensal configurada (GB tráfego + número de requests). Sem quota = ilimitado apenas para Super Admin. Sistema alerta automaticamente quando fornecedor atingir 80% da quota mensal ou quando previsão indicar esgotamento em 7 dias. Ao atingir 95% da quota, sistema aplica rate limit de 50%. A 99%, rate limit de 80%. A 100%, bloqueia POST/PUT/DELETE (GET permitido). Volumetria de um fornecedor não pode afetar outro. Quotas, limites e billing são completamente isolados. Requests de health check (/health, /ping, /metrics) não contam para quota de volumetria. Se consumo de um dia ultrapassar 2x a média dos últimos 7 dias, dispara alerta de anomalia. Após agregação de dados raw para hourly/daily/monthly, dados originais são deletados permanentemente. Se fornecedor criado no meio do mês, quota é proporcional aos dias restantes. Fórmula: quotaMensal * (diasRestantes / diasTotaisMes). Previsão de consumo só é gerada se fornecedor tiver pelo menos 3 meses de histórico. Caso contrário, usa média simples. Endpoints de exportação retornam máximo 1 GB por request. Exportações maiores usam background job. Endpoints GET de dados estáticos devem ter cache de 15min. Header Cache-Control: public, max-age=900. Dados agregados mensais devem ser mantidos por 7 anos para auditoria fiscal e conformidade com LGPD. Usuário pode fazer drill-down de qualquer métrica agregada até o request individual, mas apenas dos últimos 7 dias. Todo domingo às 23h, sistema envia e-mail automático para administradores com resumo semanal de volumetria e anomalias.</t>
+          <t>Dados coletados a cada request (1s) mas armazenados apenas 7 dias. Agregações horárias ficam 90 dias, diárias 2 anos, mensais 7 anos. Todo fornecedor deve ter quota mensal configurada (GB tráfego + número de requests). Sem quota = ilimitado apenas para Super Admin. Sistema alerta automaticamente quando fornecedor atingir 80% da quota mensal ou quando previsão indicar esgotamento em 7 dias. Ao atingir 95% da quota, sistema aplica rate limit de 50%. A 99%, rate limit de 80%. A 100%, bloqueia POST/PUT/DELETE (GET permitido). Volumetria de um fornecedor não pode afetar outro. Quotas, limites e billing são completamente isolados.</t>
         </is>
       </c>
       <c r="E43" s="3" t="inlineStr"/>
@@ -1357,15 +1505,19 @@
           <t>RF046</t>
         </is>
       </c>
-      <c r="B44" s="3" t="inlineStr"/>
+      <c r="B44" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Grupos de Troncos</t>
+        </is>
+      </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>Implementar sistema completo de agrupamento lógico, roteamento inteligente e monitoramento de troncos telefônicos (SIP, E1, móvel) com failover automático, balanceamento de carga e otimização de custos (LCR)</t>
+          <t>Implementar sistema completo de agrupamento lógico, roteamento inteligente e monitoramento de troncos telefônicos (SIP, E1, móvel) com failover automático, balanceamento de carga e otimização de cu...</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>Grupo Deve Ter Pelo Menos 1 Tronco Ativo. Prioridade Única por Tronco no Grupo. Soma de Pesos Deve Ser 100% (Weighted Balancing). Health Check Mínimo de 10 Segundos. Failover Apenas se Grupo Tiver 2+ Troncos. LCR Requer Campo Custo Por Minuto Preenchido. Notificação Imediata em Failover. Restauração Automática Após 3 Health Checks OK. Alerta em 80% da Capacidade de Concurrent Calls. Rotação de Logs de Health Check (30 Dias). Prioridade Sempre Crescente (Sem Saltos). MOS Mínimo de 3.0 para Tronco Ser Elegível. Bloqueio de Alteração de Grupo com Chamadas Ativas. Histórico de 7 Anos para Auditoria. Isolamento Multi-Tenancy por Fornecedor.</t>
+          <t>Grupo Deve Ter Pelo Menos 1 Tronco Ativo. Prioridade Única por Tronco no Grupo. Soma de Pesos Deve Ser 100% (Weighted Balancing). Health Check Mínimo de 10 Segundos. Failover Apenas se Grupo Tiver 2+ Troncos.</t>
         </is>
       </c>
       <c r="E44" s="3" t="inlineStr"/>
@@ -1376,20 +1528,20 @@
           <t>RF047</t>
         </is>
       </c>
-      <c r="B45" s="3" t="inlineStr"/>
+      <c r="B45" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Permitir a classificação e categorização de consumidores (usuários, dispositivos, máquinas) de recursos
-de telecomunicação através de tipos customizáveis, que determinam permissões, quotas, custos e comportamentos
-específicos no sistema. O requisito deve garantir flexibilidade total na criação de tipos, suporte a
-hierarquia e herança de configurações, auto-classificação baseada em regras, e gestão de ciclo de vida
-de tipos com auditoria completa.
-</t>
+          <t>Permitir a classificação e categorização de consumidores (usuários, dispositivos, máquinas) de recursos
+de telecomunicação através de tipos customizáveis, que determinam permissões, quotas, custos ...</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
         <is>
-          <t>Código de Tipo Único e Imutável. Tipo Padrão Obrigatório por Fornecedor. Hierarquia Sem Loops (Acíclica). Quota -1 = Ilimitado. Regras de Auto-Classificação por Prioridade. Mudança de Tipo Exige Aprovação (Tipos Críticos). Inativação de Tipo Move Consumidores para Tipo Padrão. Custo Fixo Mensal Somado ao Billing. Limite de 50 Tipos por Fornecedor. Auto-Classificação Apenas em Criação de Consumidor. Herança de Configurações Resolvida em Runtime. Permissões Default Aplicadas em Onboarding. Dashboard de Custos Agregado por Tipo. Cores e Ícones para Identificação Visual. Histórico de 7 Anos para Auditoria.</t>
+          <t>Código de Tipo Único e Imutável. Tipo Padrão Obrigatório por Fornecedor. Hierarquia Sem Loops (Acíclica). Quota -1 = Ilimitado. Regras de Auto-Classificação por Prioridade.</t>
         </is>
       </c>
       <c r="E45" s="3" t="inlineStr"/>
@@ -1400,16 +1552,19 @@
           <t>RF048</t>
         </is>
       </c>
-      <c r="B46" s="3" t="inlineStr"/>
+      <c r="B46" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Status de Consumidores</t>
+        </is>
+      </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Especificar o sistema de gerenciamento de ciclo de vida de consumidores através de estados bem definidos (Ativo, Inativo, Bloqueado, Suspenso, Pendente), controlando transições entre estados, aplicando políticas automáticas conforme status, mantendo histórico completo de mudanças, e integrando com processos de faturamento, auditoria e controle de acessos.
-</t>
+          <t>Especificar o sistema de gerenciamento de ciclo de vida de consumidores através de estados bem definidos (Ativo, Inativo, Bloqueado, Suspenso, Pendente), controlando transições entre estados, aplic...</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
         <is>
-          <t>Estados de Status Obrigatórios - Sistema deve implementar estados de status padrão não desativáveis. Workflow de Transições Controladas - Nem todas as transições de status são permitidas diretamente, validar matriz. Aprovação Multi-Nível para Transições Críticas - Transições críticas requerem aprovação de múltiplos níveis. Histórico Completo de Transições (LGPD) - Todas as mudanças registradas em histórico imutável (7 anos). Aplicação Automática de Políticas por Status - Cada status tem políticas aplicadas automaticamente. Notificações Automáticas de Mudança de Status - Stakeholders notificados automaticamente. Processamento em Lote de Mudanças de Status - Mudança de múltiplos consumidores assíncronamente (até 1.000). Cálculo Automático de Métricas de Ciclo de Vida - Métricas de tempo em cada status calculadas automaticamente. Bloqueio Automático por Inadimplência - Bloqueio automático por faturas vencidas (&gt;30, &gt;45, &gt;60 dias). Reativação Automática Pós-Regularização - Reativação automática ao regularizar débito. Integração com Faturamento (Suspensão de Cobrança) - Status controla se consumidor é faturado. Dashboard de Status com Indicadores Visuais - Interface visual com status em tempo real via SignalR. Auditoria de Todas as Operações de Status - Todas operações auditadas automaticamente. Multi-Tenancy com Isolamento de Status - Isolamento por Id_Fornecedor via Query Filter. Validação de Permissões RBAC - Permissões granulares por perfil (VIEW, CHANGE, APPROVE, ADMIN).</t>
+          <t>Estados de Status Obrigatórios - Sistema deve implementar estados de status padrão não desativáveis. Workflow de Transições Controladas - Nem todas as transições de status são permitidas diretamente, validar matriz. Aprovação Multi-Nível para Transições Críticas - Transições críticas requerem aprovação de múltiplos níveis. Histórico Completo de Transições (LGPD) - Todas as mudanças registradas em histórico imutável (7 anos). Aplicação Automática de Políticas por Status - Cada status tem políticas aplicadas automaticamente.</t>
         </is>
       </c>
       <c r="E46" s="3" t="inlineStr"/>
@@ -1420,7 +1575,11 @@
           <t>RF049</t>
         </is>
       </c>
-      <c r="B47" s="3" t="inlineStr"/>
+      <c r="B47" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Políticas de Consumidores</t>
+        </is>
+      </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
           <t>Implementar sistema completo de gestão de políticas de consumidores que permita definir, aplicar e monitorar regras de uso e restrições para consumidores de telecomunicações.</t>
@@ -1428,7 +1587,7 @@
       </c>
       <c r="D47" s="3" t="inlineStr">
         <is>
-          <t>Sistema deve suportar múltiplos tipos de políticas de restrição configuráveis. Políticas devem ser aplicadas automaticamente conforme perfil do consumidor. Mudança de status do consumidor deve aplicar políticas específicas automaticamente. Sistema deve alertar ANTES de atingir limite para permitir ação preventiva. Consumidores que violam políticas devem ser bloqueados automaticamente. Permitir aplicar/remover políticas de múltiplos consumidores simultaneamente. Todas as aplicações/remoções de políticas devem ser registradas de forma imutável. Todas as violações de políticas devem ser registradas para auditoria e análise. Sistema deve fornecer API para verificar se ação viola política ANTES de executar. Permitir simular impacto de política antes de aplicar em produção. Sistema deve oferecer templates de políticas comuns para agilizar configuração. Permitir importar/exportar políticas para replicação entre ambientes ou backup. Interface deve exibir visualmente conformidade de consumidores com políticas. Sistema deve calcular economia gerada por políticas aplicadas. Operações sobre políticas devem respeitar permissões por perfil.</t>
+          <t>Sistema deve suportar múltiplos tipos de políticas de restrição configuráveis. Políticas devem ser aplicadas automaticamente conforme perfil do consumidor. Mudança de status do consumidor deve aplicar políticas específicas automaticamente. Sistema deve alertar ANTES de atingir limite para permitir ação preventiva. Consumidores que violam políticas devem ser bloqueados automaticamente.</t>
         </is>
       </c>
       <c r="E47" s="3" t="inlineStr"/>
@@ -1439,11 +1598,19 @@
           <t>RF050</t>
         </is>
       </c>
-      <c r="B48" s="3" t="inlineStr"/>
-      <c r="C48" s="3" t="inlineStr"/>
+      <c r="B48" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C48" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D48" s="3" t="inlineStr">
         <is>
-          <t>Estrutura de Linha Móvel e Chip SIM. Operação de Ativação de Linha. Operação de Portabilidade. Operação de Troca de Chip. Controle de Estoque de Chips. Rastreamento de ICCID, IMSI e IMEI. Workflow de Aprovação para Operações Críticas. Integração com APIs de Operadoras. Alertas de Vencimento de Contrato. Identificação de Linhas Subutilizadas. Operação de Suspensão Temporária. Operação de Cancelamento Definitivo. Dashboard de Estoque e Status de Linhas. Importação de Linhas via CSV/Excel. Auditoria Completa de Operações de Linhas.</t>
+          <t>Estrutura de Linha Móvel e Chip SIM. Operação de Ativação de Linha. Operação de Portabilidade. Operação de Troca de Chip. Controle de Estoque de Chips.</t>
         </is>
       </c>
       <c r="E48" s="3" t="inlineStr"/>
@@ -1454,7 +1621,11 @@
           <t>RF051</t>
         </is>
       </c>
-      <c r="B49" s="3" t="inlineStr"/>
+      <c r="B49" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Marcas e Modelos de Ativos</t>
+        </is>
+      </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
           <t>Implementar sistema completo de catalogação de Fabricantes, Marcas e Modelos de equipamentos e ativos de TI/Telecom</t>
@@ -1462,7 +1633,7 @@
       </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>Nome de Fabricante Único. Part Number Único por Fabricante. Desomologação Automática ao Marcar EOL. Especificações Técnicas em JSON Válido. Histórico de Preços Imutável. Modelo Pertence a Marca do Mesmo Fabricante. Fabricante Inativo Não Permite Novos Modelos. Marca Inativa Não Permite Novos Modelos. SKU Único no Sistema (Global). Homologação Requer Justificativa. Importação em Massa Valida Todos os Registros. Máximo 10 Imagens por Modelo.</t>
+          <t>Nome de Fabricante Único. Part Number Único por Fabricante. Desomologação Automática ao Marcar EOL. Especificações Técnicas em JSON Válido. Histórico de Preços Imutável.</t>
         </is>
       </c>
       <c r="E49" s="3" t="inlineStr"/>
@@ -1473,15 +1644,19 @@
           <t>RF052</t>
         </is>
       </c>
-      <c r="B50" s="3" t="inlineStr"/>
+      <c r="B50" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Consumidores</t>
+        </is>
+      </c>
       <c r="C50" s="3" t="inlineStr">
         <is>
-          <t>Implementar sistema completo de gestão de consumidores (usuários finais de recursos de telecomunicações) com cadastro, hierarquia organizacional, alocação de ativos, controle de custos, perfis de uso, workflows automatizados e dashboard 360°.</t>
+          <t>Implementar sistema completo de gestão de consumidores (usuários finais de recursos de telecomunicações) com cadastro, hierarquia organizacional, alocação de ativos, controle de custos, perfis de u...</t>
         </is>
       </c>
       <c r="D50" s="3" t="inlineStr">
         <is>
-          <t>Tipos de Consumidores Suportados. Unicidade de Identificadores. Hierarquia Organizacional Obrigatória. Alocação de Ativos Múltiplos. Controle de Custos Individualizados. Perfis de Uso e Aplicação Automática de Políticas. Status de Consumidor e Impactos. Workflow de Onboarding Automatizado. Workflow de Offboarding Automatizado. Integração com RH para Sincronização Automática. Dashboard 360° de Consumidor. Comparação de Consumo Individual vs Média. Movimentação de Consumidores com Histórico. Relatórios de Custos por Consumidor/Departamento. Validação de Permissões RBAC.</t>
+          <t>Tipos de Consumidores Suportados. Unicidade de Identificadores. Hierarquia Organizacional Obrigatória. Alocação de Ativos Múltiplos. Controle de Custos Individualizados.</t>
         </is>
       </c>
       <c r="E50" s="3" t="inlineStr"/>
@@ -1492,7 +1667,11 @@
           <t>RF053</t>
         </is>
       </c>
-      <c r="B51" s="3" t="inlineStr"/>
+      <c r="B51" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Solicitações</t>
+        </is>
+      </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
           <t>Prover sistema completo de gestão de solicitações internas (service desk) com workflow configurável, SLA automático e aprovação mobile.</t>
@@ -1500,7 +1679,7 @@
       </c>
       <c r="D51" s="3" t="inlineStr">
         <is>
-          <t>Tipos de solicitação configuráveis com campos dinâmicos (JSON schema). Prioridade calculada automaticamente (cargo + tipo + impacto). Workflow de aprovação multi-nível configurável por tipo/valor. SLA automático com pausas (dias úteis, pendências externas). Aprovação mobile com notificação push e token temporário (15 min). Delegação de aprovadores (máximo 90 dias, sem sobreposição). Anexos obrigatórios por tipo (fotos, orçamentos, autorizações). Escalonamento automático (100% SLA → supervisor, 150% → gerente, 200% → diretor). Chat interno com mensagens públicas (solicitante) e internas (atendentes). Integração com gestão de ativos (criação automática no inventário). Reabertura permitida dentro de 7 dias (somente solicitante original). Pesquisa de satisfação automática (NPS) ao fechar solicitação. Cancelamento com justificativa obrigatória (mínimo 20 caracteres). Dashboard em tempo real via SignalR (latência &lt; 500ms). Exportação de relatórios (Excel/PDF) com filtros configuráveis.</t>
+          <t>Tipos de solicitação configuráveis com campos dinâmicos (JSON schema). Prioridade calculada automaticamente (cargo + tipo + impacto). Workflow de aprovação multi-nível configurável por tipo/valor. SLA automático com pausas (dias úteis, pendências externas). Aprovação mobile com notificação push e token temporário (15 min).</t>
         </is>
       </c>
       <c r="E51" s="3" t="inlineStr"/>
@@ -1511,11 +1690,19 @@
           <t>RF054</t>
         </is>
       </c>
-      <c r="B52" s="3" t="inlineStr"/>
-      <c r="C52" s="3" t="inlineStr"/>
+      <c r="B52" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C52" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D52" s="3" t="inlineStr">
         <is>
-          <t>Obrigatoriedade de Critérios de Seleção. Lote Imutável Após Processamento Iniciado. Seleção Automática de Faturas por Critérios. Atribuição Manual ou Automática de Auditor. Máquina de Estados do Lote. Processamento Assíncrono com Hangfire. Monitoramento de Progresso com SignalR. Reprocessamento Automático com Retry Policy. Integração com RF034 (Itens de Auditoria). Consolidação Automática com RF035. Histórico e Auditoria Completa de Operações. Notificações Assíncronas via Azure Service Bus. Cancelamento de Lote com Rollback. SLA e Alertas de Timeout.</t>
+          <t>Obrigatoriedade de Critérios de Seleção. Lote Imutável Após Processamento Iniciado. Seleção Automática de Faturas por Critérios. Atribuição Manual ou Automática de Auditor. Máquina de Estados do Lote.</t>
         </is>
       </c>
       <c r="E52" s="3" t="inlineStr"/>
@@ -1526,15 +1713,19 @@
           <t>RF055</t>
         </is>
       </c>
-      <c r="B53" s="3" t="inlineStr"/>
+      <c r="B53" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Rateio de Custos</t>
+        </is>
+      </c>
       <c r="C53" s="3" t="inlineStr">
         <is>
-          <t>Prover sistema de rateio automático e manual de custos de telecom/TI entre centros de custo, departamentos, projetos e filiais, suportando múltiplas regras de rateio, simulação, histórico completo e integração com ERPs contábeis.</t>
+          <t>Prover sistema de rateio automático e manual de custos de telecom/TI entre centros de custo, departamentos, projetos e filiais, suportando múltiplas regras de rateio, simulação, histórico completo ...</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>Sistema deve suportar 4 tipos de rateio configuráveis: fixo, proporcional por headcount, uso real e por projeto. Soma dos percentuais de rateio fixo deve ser exatamente 100% (tolerância 0,01%). Todo dia 5 de cada mês às 03:00, processar automaticamente rateio do mês anterior. Distribuir custos proporcionalmente ao número de funcionários ativos por centro de custo. Distribuir custos baseado em consumo medido (minutos, MB dados, licenças). Permitir simular rateio com diferentes regras antes de aplicar definitivamente (sem persistência). Rateio processado deve ser aprovado por gestor antes de export para ERP. Todas as mudanças em regras de rateio devem ser versionadas com vigência. Projetos temporários podem ter rateio específico com data início/fim. Gerar relatório comparando rateio do mês atual vs mês anterior. Exportar rateios aprovados para SAP via interface padronizada. Suportar rateio em cascata (empresa → diretoria → departamento → projeto). Notificar automaticamente se rateio de um centro de custo variar &gt; 30% vs mês anterior. Ajustes, créditos e descontos devem ser rateados proporcionalmente. Dashboard executivo com gráficos de evolução mensal, top centros de custo, distribuição. Rateios de um tenant não podem ser visualizados ou alterados por outro tenant. Todas as operações de rateio devem ser auditadas com usuário, data, ação e valores antes/depois. Antes de processar rateio, validar que existem custos no período. Permitir reprocessar rateio de período anterior com regra atual ou histórica. Permitir cancelar rateio aprovado mas ainda não exportado.</t>
+          <t>Sistema deve suportar 4 tipos de rateio configuráveis: fixo, proporcional por headcount, uso real e por projeto. Soma dos percentuais de rateio fixo deve ser exatamente 100% (tolerância 0,01%). Todo dia 5 de cada mês às 03:00, processar automaticamente rateio do mês anterior. Distribuir custos proporcionalmente ao número de funcionários ativos por centro de custo. Distribuir custos baseado em consumo medido (minutos, MB dados, licenças).</t>
         </is>
       </c>
       <c r="E53" s="3" t="inlineStr"/>
@@ -1545,7 +1736,11 @@
           <t>RF056</t>
         </is>
       </c>
-      <c r="B54" s="3" t="inlineStr"/>
+      <c r="B54" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Filas de Atendimento</t>
+        </is>
+      </c>
       <c r="C54" s="3" t="inlineStr">
         <is>
           <t>Implementar sistema de gestão de filas inteligentes para distribuição automática de solicitações de Service Desk entre atendentes.</t>
@@ -1553,7 +1748,7 @@
       </c>
       <c r="D54" s="3" t="inlineStr">
         <is>
-          <t>Priorização na Fila. Routing por Skills. Balanceamento de Carga. Escalação Automática. Limite de Solicitações Simultâneas. Status de Disponibilidade. Pausas Automáticas. Redistribuição em Ausência. Filas por Categoria. Priorização de VIPs. Transferência entre Atendentes. Métricas em Tempo Real. Fila de Retorno (Follow-up). SLA Pausado em Pendência Externa. Relatório de Produtividade.</t>
+          <t>Priorização na Fila. Routing por Skills. Balanceamento de Carga. Escalação Automática. Limite de Solicitações Simultâneas.</t>
         </is>
       </c>
       <c r="E54" s="3" t="inlineStr"/>
@@ -1564,15 +1759,19 @@
           <t>RF057</t>
         </is>
       </c>
-      <c r="B55" s="3" t="inlineStr"/>
+      <c r="B55" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Itens de Rateio</t>
+        </is>
+      </c>
       <c r="C55" s="3" t="inlineStr">
         <is>
-          <t>Sistema de configuração granular de itens que serão rateados (linhas móveis, licenças software, links de dados, equipamentos) com regras individuais por item, categoria ou grupo. Permite exceções, rateios customizados por item específico e controle detalhado de alocação de custos.</t>
+          <t>Sistema de configuração granular de itens que serão rateados (linhas móveis, licenças software, links de dados, equipamentos) com regras individuais por item, categoria ou grupo. Permite exceções, ...</t>
         </is>
       </c>
       <c r="D55" s="3" t="inlineStr">
         <is>
-          <t>Sistema deve suportar 4 categorias principais de itens: LinhaMobile (celulares voz+dados), LicencaSoftware (Office/Adobe/Salesforce), LinkDados (internet/MPLS/VPN), Equipamento (laptops/desktops/monitores). Item pode ser alocado 100% para um centro de custo (DEDICADO) ou dividido entre múltiplos centros de custo com percentuais (COMPARTILHADO). A soma dos percentuais DEVE ser exatamente 100%. Custos fixos (franquias mensais) e custos variáveis (excedentes de uso) devem ser separados e rateados independentemente, aplicando os mesmos percentuais de alocação para cada tipo de custo. Permitir exceções temporárias (com DataInicio e DataFim) ou permanentes (DataFim = null) de rateio. Se ExcluirTotalmente = true, o item não participa do rateio no período da exceção. Todas as mudanças de alocação devem ser versionadas em HistoricoAlocacao, arquivando a versão anterior com DataInicio/DataFim de vigência e UsuarioAlteracaoId para rastreabilidade. Deve ser possível consultar qual era a alocação em qualquer período passado. Para itens compartilhados, permitir rateio baseado em consumo real individual medido. O sistema deve calcular o percentual de uso de cada usuário/CC e distribuir o custo total proporcionalmente ao consumo medido. Job Hangfire mensal (dia 1, 02:00) deve detectar itens sem uso há mais de 3 meses (verificando tabela Consumos) e criar AlertaItem tipo SEM_USO_3_MESES com sugestão de cancelamento e economia potencial = CustoMensal. Permitir criar grupos de itens (ex: Celulares Vendas, Licenças Marketing) e aplicar mesma regra de rateio em lote para todos os itens do grupo. Permitir lançar ajustes (MULTA, CREDITO, DESCONTO, AJUSTE) vinculados a item específico em um período. Ajuste deve ser rateado proporcionalmente às alocações do item. Dashboard deve exibir: total de itens ativos, custo total do mês, top 10 itens mais caros, itens sem uso (últimos 3 meses), e evolução de custos (12 meses com gráfico de linha). Validação obrigatória ao salvar alocações: soma dos percentuais deve ser exatamente 100% (tolerância de 0.01%). Se diferente, retornar erro HTTP 400 com mensagem clara. Permitir transferir item dedicado (Tipo = DEDICADO) de um centro de custo para outro. Criar registro em TransferenciaItem com motivo, data, usuário, CC origem/destino. Atualizar AlocacaoItem.CentroCusto e DataInicio. Itens compartilhados NÃO podem ser transferidos (retornar erro). Permitir importar planilha CSV com múltiplos itens e suas alocações. Formato de alocações: CC1:40;CC2:30;CC3:30 (centro de custo:percentual separados por ;). Validar cada linha e retornar resultado com contadores de sucessos e lista de erros. Comparar custo do item no mês atual vs mês anterior. Se variação absoluta for maior que 30%, criar AlertaItem tipo VARIACAO_ANORMAL com ValorAtual, ValorAnterior, e descrição da variação percentual. Notificar gestor. Gerar relatório completo de um item com: dados básicos, histórico de custos (últimos 12 meses), histórico de alocações, transferências, ajustes, e custo total acumulado no período.</t>
+          <t>Sistema deve suportar 4 categorias principais de itens: LinhaMobile (celulares voz+dados), LicencaSoftware (Office/Adobe/Salesforce), LinkDados (internet/MPLS/VPN), Equipamento (laptops/desktops/monitores). Item pode ser alocado 100% para um centro de custo (DEDICADO) ou dividido entre múltiplos centros de custo com percentuais (COMPARTILHADO). A soma dos percentuais DEVE ser exatamente 100%. Custos fixos (franquias mensais) e custos variáveis (excedentes de uso) devem ser separados e rateados independentemente, aplicando os mesmos percentuais de alocação para cada tipo de custo. Permitir exceções temporárias (com DataInicio e DataFim) ou permanentes (DataFim = null) de rateio. Se ExcluirTotalmente = true, o item não participa do rateio no período da exceção. Todas as mudanças de alocação devem ser versionadas em HistoricoAlocacao, arquivando a versão anterior com DataInicio/DataFim de vigência e UsuarioAlteracaoId para rastreabilidade. Deve ser possível consultar qual era a alocação em qualquer período passado.</t>
         </is>
       </c>
       <c r="E55" s="3" t="inlineStr"/>
@@ -1588,10 +1787,14 @@
           <t>Gestão de Tipos de Bilhetes</t>
         </is>
       </c>
-      <c r="C56" s="3" t="inlineStr"/>
+      <c r="C56" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D56" s="3" t="inlineStr">
         <is>
-          <t>Nome do tipo de bilhete deve ser único no sistema (case-insensitive). Nome deve ter no mínimo 3 caracteres. Nome não pode exceder 100 caracteres. Nome deve conter apenas letras, números, espaços e hífen. Descrição é obrigatória com mínimo de 10 caracteres. Descrição não pode exceder 500 caracteres. Todo tipo de bilhete deve estar associado a uma empresa. Tipos não são excluídos fisicamente, apenas marcados como excluídos. Todas as operações devem ser auditadas. Novos tipos são criados com status Ativo por padrão. Cada operação requer permissão específica. Listagem deve respeitar filtros aplicados.</t>
+          <t>Nome do tipo de bilhete deve ser único no sistema (case-insensitive). Nome deve ter no mínimo 3 caracteres. Nome não pode exceder 100 caracteres. Nome deve conter apenas letras, números, espaços e hífen. Descrição é obrigatória com mínimo de 10 caracteres.</t>
         </is>
       </c>
       <c r="E56" s="3" t="inlineStr"/>
@@ -1602,18 +1805,20 @@
           <t>RF059</t>
         </is>
       </c>
-      <c r="B57" s="3" t="inlineStr"/>
+      <c r="B57" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
       <c r="C57" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Especificar o sistema de gestão centralizada de listas parametrizáveis de status, tipos e categorias genéricas
-utilizadas em todo o sistema IControlIT. O módulo permite criar, editar, inativar e configurar domínios de
-classificação sem necessidade de alteração de código, proporcionando flexibilidade operacional e adaptação por cliente.
-</t>
+          <t>Especificar o sistema de gestão centralizada de listas parametrizáveis de status, tipos e categorias genéricas
+utilizadas em todo o sistema IControlIT. O módulo permite criar, editar, inativar e co...</t>
         </is>
       </c>
       <c r="D57" s="3" t="inlineStr">
         <is>
-          <t>Código de Domínio Único por Cliente. Código de Item Único por Domínio. Validação de Transição de Estado. Inativação com Validação de Dependências. Ordenação Customizada com Reindexação Automática. Apenas Um Valor Padrão por Domínio. Internacionalização Obrigatória. Multi-tenancy com Itens Globais e Customizados. Histórico Completo de Alterações. Cache In-Memory com Invalidação Automática.</t>
+          <t>Código de Domínio Único por Cliente. Código de Item Único por Domínio. Validação de Transição de Estado. Inativação com Validação de Dependências. Ordenação Customizada com Reindexação Automática.</t>
         </is>
       </c>
       <c r="E57" s="3" t="inlineStr"/>
@@ -1624,11 +1829,19 @@
           <t>RF060</t>
         </is>
       </c>
-      <c r="B58" s="3" t="inlineStr"/>
-      <c r="C58" s="3" t="inlineStr"/>
+      <c r="B58" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C58" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D58" s="3" t="inlineStr">
         <is>
-          <t>Classificação ITIL v4 Obrigatória. SLA Diferenciado por Tipo e Prioridade. Formulários Dinâmicos Configuráveis. Templates de Resolução com Knowledge Base. Escalonamento Automático por Tempo. Matriz de Prioridade Automática. Aprovação CAB para Mudanças. Vinculação de Incidentes a Problemas. Categorização Hierárquica de 3 Níveis. Especialistas Preferenciais por Tipo. Métricas ITIL Obrigatórias. Integração com CMDB Obrigatória. Janelas de Mudança Configuráveis. Cálculo de Custos por Tipo. Relatórios Gerenciais Obrigatórios.</t>
+          <t>Classificação ITIL v4 Obrigatória. SLA Diferenciado por Tipo e Prioridade. Formulários Dinâmicos Configuráveis. Templates de Resolução com Knowledge Base. Escalonamento Automático por Tempo.</t>
         </is>
       </c>
       <c r="E58" s="3" t="inlineStr"/>
@@ -1639,7 +1852,11 @@
           <t>RF061</t>
         </is>
       </c>
-      <c r="B59" s="3" t="inlineStr"/>
+      <c r="B59" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Ordens de Serviço (OS)</t>
+        </is>
+      </c>
       <c r="C59" s="3" t="inlineStr">
         <is>
           <t>Implementar sistema completo de gestão de ordens de serviço (OS) para atendimentos técnicos presenciais (field service)</t>
@@ -1647,7 +1864,7 @@
       </c>
       <c r="D59" s="3" t="inlineStr">
         <is>
-          <t>Criação Automática de OS a partir de Solicitação. Agendamento com Verificação de Disponibilidade. Checklist Obrigatório por Tipo de OS. Assinatura Digital Obrigatória. Controle de Peças Utilizadas. Fotos de Evidência (Antes/Depois). Geolocalização de Check-in/Check-out. Cálculo Automático de Tempo de Atendimento. Reagendamento com Justificativa Obrigatória. Controle de SLA de Atendimento. Avaliação NPS do Serviço. Integração com Faturamento. Histórico de Performance do Técnico. Notificações de Agendamento. Dashboard com Mapa de OSs Abertas. Isolamento Multi-Tenant.</t>
+          <t>Criação Automática de OS a partir de Solicitação. Agendamento com Verificação de Disponibilidade. Checklist Obrigatório por Tipo de OS. Assinatura Digital Obrigatória. Controle de Peças Utilizadas.</t>
         </is>
       </c>
       <c r="E59" s="3" t="inlineStr"/>
@@ -1658,15 +1875,19 @@
           <t>RF062</t>
         </is>
       </c>
-      <c r="B60" s="3" t="inlineStr"/>
+      <c r="B60" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Fornecedores e Parceiros</t>
+        </is>
+      </c>
       <c r="C60" s="3" t="inlineStr">
         <is>
-          <t>Fornecer sistema completo de cadastro e gestão de fornecedores e parceiros de TI e Telecom, incluindo controle de documentação obrigatória, gestão de contratos e SLAs, avaliação de performance, homologação e integração com processos de compras e solicitações.</t>
+          <t>Fornecer sistema completo de cadastro e gestão de fornecedores e parceiros de TI e Telecom, incluindo controle de documentação obrigatória, gestão de contratos e SLAs, avaliação de performance, hom...</t>
         </is>
       </c>
       <c r="D60" s="3" t="inlineStr">
         <is>
-          <t>Categorias de Fornecedores. Documentação Obrigatória. Alertas de Vencimento de Documentos. Bloqueio por Documentação Vencida. Contratos Vinculados. SLA por Fornecedor. Avaliações Periódicas. Ranking de Fornecedores. Contatos Múltiplos. Integração com Solicitações. Histórico de Atendimentos. Dashboard de Performance. Alertas de Renovação de Contratos. Homologação de Fornecedores. Export para Compliance.</t>
+          <t>Categorias de Fornecedores. Documentação Obrigatória. Alertas de Vencimento de Documentos. Bloqueio por Documentação Vencida. Contratos Vinculados.</t>
         </is>
       </c>
       <c r="E60" s="3" t="inlineStr"/>
@@ -1677,7 +1898,11 @@
           <t>RF063</t>
         </is>
       </c>
-      <c r="B61" s="3" t="inlineStr"/>
+      <c r="B61" s="3" t="inlineStr">
+        <is>
+          <t>Motor de Templates (Template Engine)</t>
+        </is>
+      </c>
       <c r="C61" s="3" t="inlineStr">
         <is>
           <t>Prover um motor de processamento de templates dinâmicos com sintaxe Liquid/Handlebars para geração de e-mails, relatórios, documentos e notificações</t>
@@ -1685,7 +1910,7 @@
       </c>
       <c r="D61" s="3" t="inlineStr">
         <is>
-          <t>Sintaxe Liquid Obrigatória - Todo template deve utilizar sintaxe Liquid (Shopify) para marcações dinâmicas. Contexto de Dados Tipado - O contexto de renderização deve ser um objeto tipado com propriedades bem definidas. Filtros Customizados Obrigatórios - O sistema deve fornecer filtros: currency, formatarData, truncar. Preview em Tempo Real - Gerar preview do template com dados de teste antes de salvar. Versionamento Obrigatório - Toda alteração em template deve criar nova versão, preservando histórico. Validação de Sintaxe Bloqueante - Templates com sintaxe Liquid inválida não podem ser salvos. Testes A/B de Templates - Permitir criar variações de um template para testes A/B. Herança de Templates (Layout Base) - Templates filhos podem herdar estrutura de um layout base. Parciais Reutilizáveis - Suportar inclusão de parciais (header, footer, assinatura). Internacionalização (Helper 't') - Templates devem suportar traduções via helper {{ 't' }}. Sanitização HTML Contra XSS - Variáveis renderizadas devem ser sanitizadas automaticamente. Cache de Templates Compilados (Redis) - Templates compilados devem ser armazenados em cache distribuído. Documentação Automática de Variáveis - Listar automaticamente todas as variáveis disponíveis no contexto. Auditoria de Uso de Templates - Rastrear quando e onde cada template foi utilizado. Isolamento Multi-Tenant - Cada tenant deve ter acesso apenas aos seus próprios templates.</t>
+          <t>Sintaxe Liquid Obrigatória - Todo template deve utilizar sintaxe Liquid (Shopify) para marcações dinâmicas. Contexto de Dados Tipado - O contexto de renderização deve ser um objeto tipado com propriedades bem definidas. Filtros Customizados Obrigatórios - O sistema deve fornecer filtros: currency, formatarData, truncar. Preview em Tempo Real - Gerar preview do template com dados de teste antes de salvar. Versionamento Obrigatório - Toda alteração em template deve criar nova versão, preservando histórico.</t>
         </is>
       </c>
       <c r="E61" s="3" t="inlineStr"/>
@@ -1696,18 +1921,21 @@
           <t>RF064</t>
         </is>
       </c>
-      <c r="B62" s="3" t="inlineStr"/>
+      <c r="B62" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Templates de E-mail</t>
+        </is>
+      </c>
       <c r="C62" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Permitir que o sistema gerencie templates de e-mail responsivos, personalizáveis e rastreáveis,
+          <t>Permitir que o sistema gerencie templates de e-mail responsivos, personalizáveis e rastreáveis,
 com teste A/B automático, compatibilidade multi-cliente (Gmail/Outlook/Apple/Yahoo),
-métricas de engajamento (open rate, CTR) e conformidade legal (LGPD/CAN-SPAM).
-</t>
+métricas de enga...</t>
         </is>
       </c>
       <c r="D62" s="3" t="inlineStr">
         <is>
-          <t>Design responsivo obrigatório com media queries: desktop (&gt;=600px) vs mobile (&lt;600px). Compatibilidade testada em 4 clientes: Gmail (web + app), Outlook (desktop + web), Apple Mail (macOS + iOS), Yahoo Mail. Rastreamento de abertura via pixel invisível (1x1) com URL única por envio. Rastreamento de cliques via URL wrapping (redirect tracking) para todos os links do template. Branding customizado por empresa: logo, cores primárias/secundárias, rodapé customizado. Teste A/B automático: 10% teste (50% A + 50% B), 90% winner após 100 envios mínimos ou 24h. Link de unsubscribe obrigatório em todos os templates (LGPD/CAN-SPAM). Pre-header text obrigatório (max 150 caracteres) para melhorar preview em clientes de e-mail. Conversão automática de CSS para inline (Outlook compatibility) antes de envio. Cálculo de anti-spam score via SpamAssassin: score &lt; 5.0 para ativar template. Biblioteca de 20+ templates padrão pré-configurados (boas-vindas, recuperação senha, notificação, etc). Versionamento de templates: v1.0 → v1.1 → v2.0 (histórico de alterações). Preview multi-dispositivo em tempo real: desktop (1024px), tablet (768px), mobile (375px). Métricas de engajamento: open rate, CTR, taxa de conversão por template. Agendamento de envios via Hangfire: envio imediato ou agendado (DataAgendamento). Unicidade de Nome de template por empresa (multi-tenancy). Validação de SPF/DKIM/DMARC antes de ativar configuração SMTP. Fila assíncrona de envio via Hangfire (retry automático 3x em caso de falha).</t>
+          <t>Design responsivo obrigatório com media queries: desktop (&gt;=600px) vs mobile (&lt;600px). Compatibilidade testada em 4 clientes: Gmail (web + app), Outlook (desktop + web), Apple Mail (macOS + iOS), Yahoo Mail. Rastreamento de abertura via pixel invisível (1x1) com URL única por envio. Rastreamento de cliques via URL wrapping (redirect tracking) para todos os links do template. Branding customizado por empresa: logo, cores primárias/secundárias, rodapé customizado.</t>
         </is>
       </c>
       <c r="E62" s="3" t="inlineStr"/>
@@ -1718,18 +1946,20 @@
           <t>RF065</t>
         </is>
       </c>
-      <c r="B63" s="3" t="inlineStr"/>
+      <c r="B63" s="3" t="inlineStr">
+        <is>
+          <t>Templates de Relatórios (Excel/PDF)</t>
+        </is>
+      </c>
       <c r="C63" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Implementar sistema de geração de relatórios customizáveis em múltiplos formatos (Excel .xlsx, PDF, CSV)
-com templates reutilizáveis, gráficos dinâmicos, agrupamentos, totalizações automáticas, formatação condicional,
-múltiplas abas, agendamento de exportações automáticas via Hangfire e envio por e-mail.
-</t>
+          <t>Implementar sistema de geração de relatórios customizáveis em múltiplos formatos (Excel .xlsx, PDF, CSV)
+com templates reutilizáveis, gráficos dinâmicos, agrupamentos, totalizações automáticas, for...</t>
         </is>
       </c>
       <c r="D63" s="3" t="inlineStr">
         <is>
-          <t>Sistema DEVE suportar geração de relatórios em 3 formatos: Excel (.xlsx), PDF e CSV. Sistema DEVE suportar 4 tipos de gráficos Chart.js: Linha, Barra, Pizza, Área. Sistema DEVE permitir agrupar dados por 1 ou mais campos e calcular subtotais automáticos (soma, média). Sistema DEVE aplicar formatação condicional (cores, negrito) baseado em regras configuráveis. Sistema DEVE permitir criar Excel com múltiplas abas (worksheets), cada uma com consulta SQL independente. Relatórios PODEM ter parâmetros dinâmicos (filtros) que DEVEM ser preenchidos antes de gerar. Sistema DEVE permitir agendar geração automática de relatórios em frequência diária, semanal ou mensal. Relatórios PDF e Excel DEVEM ter cabeçalho e rodapé configuráveis. Excel gerado DEVE ter proteção contra edição (somente leitura). PDFs sensíveis DEVEM ter assinatura digital para garantir autenticidade. PDFs PODEM ter marca d'água configurável (ex: Confidencial, Interno). Templates PODEM consultar cubos OLAP (SQL Server Analysis Services) para relatórios analíticos. Relatórios pesados (&gt;1000 linhas ou &gt;5s de execução) DEVEM ser cacheados por 15 minutos. Sistema DEVE permitir gerar múltiplos relatórios em arquivo ZIP único. Sistema DEVE rastrear métricas de uso de cada template.</t>
+          <t>Sistema DEVE suportar geração de relatórios em 3 formatos: Excel (.xlsx), PDF e CSV. Sistema DEVE suportar 4 tipos de gráficos Chart.js: Linha, Barra, Pizza, Área. Sistema DEVE permitir agrupar dados por 1 ou mais campos e calcular subtotais automáticos (soma, média). Sistema DEVE aplicar formatação condicional (cores, negrito) baseado em regras configuráveis. Sistema DEVE permitir criar Excel com múltiplas abas (worksheets), cada uma com consulta SQL independente.</t>
         </is>
       </c>
       <c r="E63" s="3" t="inlineStr"/>
@@ -1740,11 +1970,19 @@
           <t>RF066</t>
         </is>
       </c>
-      <c r="B64" s="3" t="inlineStr"/>
-      <c r="C64" s="3" t="inlineStr"/>
+      <c r="B64" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C64" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D64" s="3" t="inlineStr">
         <is>
-          <t>Canais de Notificação Suportados. Níveis de Prioridade. Quiet Hours (Horários de Silêncio). Agrupamento Inteligente. Retry com Backoff Exponencial. Rate Limiting (Anti-Spam). Digest Diário. Rastreamento de Entrega. Quick Actions (Ações Rápidas). Notificações de Conformidade (Obrigatórias). Integração com Templates (RF063). Multi-Tenancy (Isolamento por Empresa). Auditoria de Notificações. Internacionalização (i18n). Processamento Assíncrono (Hangfire).</t>
+          <t>Canais de Notificação Suportados. Níveis de Prioridade. Quiet Hours (Horários de Silêncio). Agrupamento Inteligente. Retry com Backoff Exponencial.</t>
         </is>
       </c>
       <c r="E64" s="3" t="inlineStr"/>
@@ -1755,7 +1993,11 @@
           <t>RF067</t>
         </is>
       </c>
-      <c r="B65" s="3" t="inlineStr"/>
+      <c r="B65" s="3" t="inlineStr">
+        <is>
+          <t>Central de E-mails</t>
+        </is>
+      </c>
       <c r="C65" s="3" t="inlineStr">
         <is>
           <t>Prover sistema centralizado de gestão de envio de e-mails transacionais e marketing com deliverability garantido</t>
@@ -1763,7 +2005,7 @@
       </c>
       <c r="D65" s="3" t="inlineStr">
         <is>
-          <t>E-mails devem ser processados por ordem de prioridade. Sistema deve suportar múltiplos servidores SMTP com balanceamento. Retry automático até 5 vezes com backoff exponencial. Rastrear todos os eventos do ciclo de vida. Hard bounce deve adicionar automaticamente à blacklist. Limitar envios por domínio (100/hora padrão). Warmup de IPs novos com aumento gradual (15 dias). Validar sintaxe e MX record antes de enviar. Unsubscribe com um clique (sem login). Health check SMTP a cada 5 minutos. Configurar e validar SPF, DKIM, DMARC. Integração com templates de e-mail (RF064). Não enviar mesmo e-mail 2x em 24h. Gerar relatórios de deliverability. Suportar múltiplos provedores (SendGrid, Mailgun, SES, SMTP). Isolamento multi-tenant. Auditoria de operações críticas. Permissões RBAC. Limites de performance (10k/min). Disponibilidade e SLA (99.95% uptime, 98% deliverability).</t>
+          <t>E-mails devem ser processados por ordem de prioridade. Sistema deve suportar múltiplos servidores SMTP com balanceamento. Retry automático até 5 vezes com backoff exponencial. Rastrear todos os eventos do ciclo de vida. Hard bounce deve adicionar automaticamente à blacklist.</t>
         </is>
       </c>
       <c r="E65" s="3" t="inlineStr"/>
@@ -1774,11 +2016,19 @@
           <t>RF068</t>
         </is>
       </c>
-      <c r="B66" s="3" t="inlineStr"/>
-      <c r="C66" s="3" t="inlineStr"/>
+      <c r="B66" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C66" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D66" s="3" t="inlineStr">
         <is>
-          <t>Classificação ABC Obrigatória para Inventário Cíclico. Contagem Dupla Cega para Itens Classificação A. Divergência &gt; 5% Exige Recontagem. Ajuste de Estoque Exige Aprovação de Supervisor. Bloqueio de Movimentação Durante Inventário. Almoxarifado Deve Estar Ativo. Periodicidade Inventário Cíclico. Histórico Imutável de Contagens. Dashboard Tempo Real via SignalR. Integração com ERP para Ajustes Contábeis. Relatório de Auditoria ISO 9001. App Mobile Offline-First.</t>
+          <t>Classificação ABC Obrigatória para Inventário Cíclico. Contagem Dupla Cega para Itens Classificação A. Divergência &gt; 5% Exige Recontagem. Ajuste de Estoque Exige Aprovação de Supervisor. Bloqueio de Movimentação Durante Inventário.</t>
         </is>
       </c>
       <c r="E66" s="3" t="inlineStr"/>
@@ -1789,7 +2039,11 @@
           <t>RF069</t>
         </is>
       </c>
-      <c r="B67" s="3" t="inlineStr"/>
+      <c r="B67" s="3" t="inlineStr">
+        <is>
+          <t>Configuração de SLA para Chamados</t>
+        </is>
+      </c>
       <c r="C67" s="3" t="inlineStr">
         <is>
           <t>Especificar sistema de configuração e gerenciamento de SLAs para chamados de Service Desk</t>
@@ -1797,7 +2051,7 @@
       </c>
       <c r="D67" s="3" t="inlineStr">
         <is>
-          <t>Tempos Obrigatórios e Válidos - Todo SLA deve ter tempo de resposta e resolução &gt; 0, resolução &gt;= resposta. Unicidade por Cliente/Tipo/Prioridade - Não pode existir SLA duplicado ativo para mesma combinação. Calendário Obrigatório - Todo SLA deve estar associado a calendário válido e ativo. Pausas Automáticas por Status - Sistema pausa/retoma SLA automaticamente conforme status do chamado. Escalações em Percentuais Configuráveis - Disparo automático em percentuais configurados (50%, 75%, 90%, 100%). Cálculo em Horário Útil - Tempo decorrido calculado apenas em horário útil do calendário. Feriados Customizáveis - Suporte a feriados nacionais, estaduais, municipais, corporativos com importação via API. Versionamento Imutável - Registro de todas alterações com data, usuário, before/after e motivo obrigatório. Simulador What-If - Calcula impacto no compliance histórico ao alterar parâmetros de SLA. Aplicação Automática de SLA - SLA aplicado automaticamente ao criar chamado (específico → genérico → default). Isolamento Multi-Tenant - Usuário só acessa SLAs do próprio Fornecedor. Permissões Granulares - Cada operação exige permissão explícita via RBAC.</t>
+          <t>Tempos Obrigatórios e Válidos - Todo SLA deve ter tempo de resposta e resolução &gt; 0, resolução &gt;= resposta. Unicidade por Cliente/Tipo/Prioridade - Não pode existir SLA duplicado ativo para mesma combinação. Calendário Obrigatório - Todo SLA deve estar associado a calendário válido e ativo. Pausas Automáticas por Status - Sistema pausa/retoma SLA automaticamente conforme status do chamado. Escalações em Percentuais Configuráveis - Disparo automático em percentuais configurados (50%, 75%, 90%, 100%).</t>
         </is>
       </c>
       <c r="E67" s="3" t="inlineStr"/>
@@ -1808,15 +2062,19 @@
           <t>RF070</t>
         </is>
       </c>
-      <c r="B68" s="3" t="inlineStr"/>
+      <c r="B68" s="3" t="inlineStr">
+        <is>
+          <t>Base de Conhecimento</t>
+        </is>
+      </c>
       <c r="C68" s="3" t="inlineStr">
         <is>
-          <t>Especificar o Módulo de Base de Conhecimento (Knowledge Base) para criar, organizar, publicar e gerenciar artigos técnicos, tutoriais, procedimentos, FAQs e documentação de suporte que auxiliam na resolução de chamados, reduzem tempo de atendimento e promovem autoatendimento pelos usuários finais.</t>
+          <t>Especificar o Módulo de Base de Conhecimento (Knowledge Base) para criar, organizar, publicar e gerenciar artigos técnicos, tutoriais, procedimentos, FAQs e documentação de suporte que auxiliam na ...</t>
         </is>
       </c>
       <c r="D68" s="3" t="inlineStr">
         <is>
-          <t>Título Único por Categoria - Dentro de uma mesma categoria, não podem existir dois artigos ativos com títulos idênticos (case-insensitive).. Conteúdo Mínimo Obrigatório - Todo artigo DEVE conter: Título (10-200 chars), Resumo (50-500 chars), Problema (min 100 chars), Solução (min 200 chars), 1+ categoria.. Limite de Categorias por Artigo - Cada artigo pode pertencer a no máximo 5 categorias simultaneamente.. Workflow de Aprovação por Categoria - Artigos em categorias críticas (Segurança, Compliance, LGPD) SEMPRE requerem aprovação antes de publicação.. Score de Utilidade Mínimo - Artigos com score &lt; 60% após 20+ votações devem ser sinalizados para revisão.. Isolamento Multi-Tenant - Todos os artigos, categorias, votações e anexos DEVEM ser isolados por ClienteId.. Versionamento Automático - Atualização em campos críticos (Título, Problema, Solução, Causa Raiz) DEVE gerar nova versão.. Artigos Obsoletos - Artigos publicados sem acessos há 180+ dias devem ser marcados como obsoletos.. Anexos - Tamanho e Tipos - Limite de 500MB por arquivo, tipos permitidos: pdf, docx, xlsx, pptx, png, jpg, jpeg, gif, mp4, zip.. Permissões de Edição - Usuário pode editar apenas artigos que criou, exceto se tiver permissão kb:artigos:update_all.. Busca Full-Text - Performance - Busca deve retornar resultados em &lt; 500ms (P95) mesmo em bases com 50.000+ artigos.. Auditoria de Operações Críticas - CREATE, UPDATE, DELETE, PUBLISH, APPROVE devem ser auditadas com registro completo e retenção de 7 anos.. Portal Self-Service - Acesso Público - Portal deve permitir busca/visualização de artigos públicos sem autenticação.. Integração com Chamados - Sugestão Automática - Ao criar chamado, sistema deve sugerir até 5 artigos relacionados.. Tags - Autocomplete e Sugestão - Sistema deve sugerir tags existentes via autocomplete, evitando duplicação.</t>
+          <t>Título Único por Categoria - Dentro de uma mesma categoria, não podem existir dois artigos ativos com títulos idênticos (case-insensitive).. Conteúdo Mínimo Obrigatório - Todo artigo DEVE conter: Título (10-200 chars), Resumo (50-500 chars), Problema (min 100 chars), Solução (min 200 chars), 1+ categoria.. Limite de Categorias por Artigo - Cada artigo pode pertencer a no máximo 5 categorias simultaneamente.. Workflow de Aprovação por Categoria - Artigos em categorias críticas (Segurança, Compliance, LGPD) SEMPRE requerem aprovação antes de publicação.. Score de Utilidade Mínimo - Artigos com score &lt; 60% após 20+ votações devem ser sinalizados para revisão.</t>
         </is>
       </c>
       <c r="E68" s="3" t="inlineStr"/>
@@ -1827,11 +2085,19 @@
           <t>RF071</t>
         </is>
       </c>
-      <c r="B69" s="3" t="inlineStr"/>
-      <c r="C69" s="3" t="inlineStr"/>
+      <c r="B69" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C69" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D69" s="3" t="inlineStr">
         <is>
-          <t>Frequência Máxima de Pesquisas (Anti-Fadiga). Cálculo Automático de NPS. Follow-up Automático para Detratores. Anonimização Configurável por Tipo de Pesquisa. Análise de Sentimento Automática (NLP). Validação de Taxa de Resposta Mínima. Expiração de Link de Pesquisa. Cálculo de CES (Customer Effort Score). Correlação Automática com Chamado de Origem. Limite de Caracteres em Respostas Abertas. Prazo SLA de Follow-up para Gestores. Dashboard Atualização SignalR.</t>
+          <t>Frequência Máxima de Pesquisas (Anti-Fadiga). Cálculo Automático de NPS. Follow-up Automático para Detratores. Anonimização Configurável por Tipo de Pesquisa. Análise de Sentimento Automática (NLP).</t>
         </is>
       </c>
       <c r="E69" s="3" t="inlineStr"/>
@@ -1842,7 +2108,11 @@
           <t>RF072</t>
         </is>
       </c>
-      <c r="B70" s="3" t="inlineStr"/>
+      <c r="B70" s="3" t="inlineStr">
+        <is>
+          <t>Escalação Automática</t>
+        </is>
+      </c>
       <c r="C70" s="3" t="inlineStr">
         <is>
           <t>Implementar engine inteligente de escalação automática de chamados (tickets) baseado em triggers configuráveis: SLA, prioridade, skills, carga de trabalho e hierarquia organizacional.</t>
@@ -1850,7 +2120,7 @@
       </c>
       <c r="D70" s="3" t="inlineStr">
         <is>
-          <t>Escalação automática por SLA consumido (50%, 75%, 90%, 100%). Escalação por prioridade automática (P1: 15min, P2: 45min, P3: 2h). Skill-based routing com score ponderado (skills 40% + histórico 30% + disponibilidade 20% + SLA 10%). Limite de carga e pausa automática (&gt;8 chamados = pausa, &lt;5 = remove). Matriz hierárquica multicliente independente (2-5 níveis). Auditoria completa com retenção 7 anos (LGPD). Notificação multi-canal com garantia de entrega (&lt;30s, 4 canais). Pausas temporárias integradas com calendário AD (sync 1x/hora). Aceite e rejeição com registro de motivo (SLA aceite &lt;5min). Dashboard real-time com alertas críticos (SignalR, métricas).</t>
+          <t>Escalação automática por SLA consumido (50%, 75%, 90%, 100%). Escalação por prioridade automática (P1: 15min, P2: 45min, P3: 2h). Skill-based routing com score ponderado (skills 40% + histórico 30% + disponibilidade 20% + SLA 10%). Limite de carga e pausa automática (&gt;8 chamados = pausa, &lt;5 = remove). Matriz hierárquica multicliente independente (2-5 níveis).</t>
         </is>
       </c>
       <c r="E70" s="3" t="inlineStr"/>
@@ -1861,17 +2131,20 @@
           <t>RF073</t>
         </is>
       </c>
-      <c r="B71" s="3" t="inlineStr"/>
+      <c r="B71" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Chamados e SLA</t>
+        </is>
+      </c>
       <c r="C71" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Módulo responsável pela abertura, acompanhamento, resolução e auditoria de solicitações
-de suporte técnico (chamados) em conformidade com Service Level Agreements (SLAs) contratuais.
-</t>
+          <t>Módulo responsável pela abertura, acompanhamento, resolução e auditoria de solicitações
+de suporte técnico (chamados) em conformidade com Service Level Agreements (SLAs) contratuais.</t>
         </is>
       </c>
       <c r="D71" s="3" t="inlineStr">
         <is>
-          <t>Campos obrigatórios para criação de chamado. Prioridade calculada automaticamente via matriz Impacto x Urgência. SLA de resposta e resolução baseado em prioridade. Parada de ativo suspende cálculo de SLA. Atribuição automática via skill-based routing. Status de SLA recalculado periodicamente. Comentários internos vs externos. Reabertura de chamado fecha original e cria novo linkado. Auditoria de todas as mudanças de estado. Integração com ServiceNow para chamados críticos. Validação de anexos de arquivos. Soft delete obrigatório para chamados.</t>
+          <t>Campos obrigatórios para criação de chamado. Prioridade calculada automaticamente via matriz Impacto x Urgência. SLA de resposta e resolução baseado em prioridade. Parada de ativo suspende cálculo de SLA. Atribuição automática via skill-based routing.</t>
         </is>
       </c>
       <c r="E71" s="3" t="inlineStr"/>
@@ -1882,11 +2155,19 @@
           <t>RF074</t>
         </is>
       </c>
-      <c r="B72" s="3" t="inlineStr"/>
-      <c r="C72" s="3" t="inlineStr"/>
+      <c r="B72" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C72" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D72" s="3" t="inlineStr">
         <is>
-          <t>Isolamento Dados por Usuário. Wizard 3-Passos Obrigatório. Categorias do Catálogo. FAQ Busca Real-Time. Notificações SignalR. Comentários Públicos Apenas. CSAT Inline. Upload Antivírus. Auditoria Completa. PWA Offline. Rate Limiting. Multi-Tenancy Isolamento. i18n. Responsividade Mobile-First. Acessibilidade WCAG 2.1 AA.</t>
+          <t>Isolamento Dados por Usuário. Wizard 3-Passos Obrigatório. Categorias do Catálogo. FAQ Busca Real-Time. Notificações SignalR.</t>
         </is>
       </c>
       <c r="E72" s="3" t="inlineStr"/>
@@ -1897,19 +2178,21 @@
           <t>RF075</t>
         </is>
       </c>
-      <c r="B73" s="3" t="inlineStr"/>
+      <c r="B73" s="3" t="inlineStr">
+        <is>
+          <t>Roaming Internacional</t>
+        </is>
+      </c>
       <c r="C73" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Especificar o módulo de gestão de roaming internacional para dispositivos móveis corporativos,
+          <t>Especificar o módulo de gestão de roaming internacional para dispositivos móveis corporativos,
 permitindo que colaboradores solicitem ativação de roaming em países específicos, gestores aprovem
-solicitações, e o sistema coordene a ativação junto aos operadores de telecomunicações com controle
-automatizado de limites de consumo.
-</t>
+sol...</t>
         </is>
       </c>
       <c r="D73" s="3" t="inlineStr">
         <is>
-          <t>Solicitação Requer Aprovação de Gestor. Limite de Consumo por País é Inviolável. Alertas de Consumo em Cascata (50%, 75%, 90%, 100%). Roaming Desativa Automaticamente na Data de Término. Rejeição com Limite de 3 Tentativas. Integração com Operadora Requer Dados Válidos. Auditoria de Todas as Ações. Notificações em Tempo Real. Limite de Roaming Ativo por Usuário (Máximo 5). Retenção de Dados Conforme LGPD (7 Anos). Multi-Tenancy: Isolamento por Fornecedor. Validação de País na Lista Branca. Sincronização de Consumo a Cada 30 Minutos. Permissões RBAC por Operação. Criptografia de Dados Sensíveis.</t>
+          <t>Solicitação Requer Aprovação de Gestor. Limite de Consumo por País é Inviolável. Alertas de Consumo em Cascata (50%, 75%, 90%, 100%). Roaming Desativa Automaticamente na Data de Término. Rejeição com Limite de 3 Tentativas.</t>
         </is>
       </c>
       <c r="E73" s="3" t="inlineStr"/>
@@ -1920,15 +2203,19 @@
           <t>RF076</t>
         </is>
       </c>
-      <c r="B74" s="3" t="inlineStr"/>
+      <c r="B74" s="3" t="inlineStr">
+        <is>
+          <t>Manutenção Preventiva e Corretiva</t>
+        </is>
+      </c>
       <c r="C74" s="3" t="inlineStr">
         <is>
-          <t>Prover capacidade de gerenciamento completo do ciclo de vida das manutenções de ativos (preventivas e corretivas), permitindo agendamento automático, execução de ordens de serviço, controle de peças/materiais, workflow de aprovação e cálculo de indicadores de confiabilidade (MTBF) e eficiência (MTTR).</t>
+          <t>Prover capacidade de gerenciamento completo do ciclo de vida das manutenções de ativos (preventivas e corretivas), permitindo agendamento automático, execução de ordens de serviço, controle de peça...</t>
         </is>
       </c>
       <c r="D74" s="3" t="inlineStr">
         <is>
-          <t>Plano de manutenção deve ter periodicidade (dias, horas ou km) e checklist com mínimo 1 atividade. Ao ativar plano, primeira ordem é criada imediatamente; subsequentes seguem periodicidade. Ordem de serviço passa por estados: Agendada → Aprovada → EmExecucao → Concluida → Fechada. Peça/material deve ter quantidade &gt; 0, custo &gt;= 0 e descrição obrigatória. MTBF calculado automaticamente ao fechar ordem corretiva (Total Horas Operação / Número Falhas). MTTR calculado automaticamente ao fechar ordem corretiva (Total Horas Reparo / Número Falhas). Alerta gerado se ordem preventiva não executada 7 dias após data prevista. Ordem em execução muda status de ativo para EmManutencao; concluída volta para Operacional. Operações requerem permissões específicas (man:ordem:*, man:plano:*, man:relatorio:read). Usuário só acessa ordens/planos do seu próprio tenant.</t>
+          <t>Plano de manutenção deve ter periodicidade (dias, horas ou km) e checklist com mínimo 1 atividade. Ao ativar plano, primeira ordem é criada imediatamente; subsequentes seguem periodicidade. Ordem de serviço passa por estados: Agendada → Aprovada → EmExecucao → Concluida → Fechada. Peça/material deve ter quantidade &gt; 0, custo &gt;= 0 e descrição obrigatória. MTBF calculado automaticamente ao fechar ordem corretiva (Total Horas Operação / Número Falhas).</t>
         </is>
       </c>
       <c r="E74" s="3" t="inlineStr"/>
@@ -1939,15 +2226,19 @@
           <t>RF077</t>
         </is>
       </c>
-      <c r="B75" s="3" t="inlineStr"/>
+      <c r="B75" s="3" t="inlineStr">
+        <is>
+          <t>Ordens de Serviço e Atendimento</t>
+        </is>
+      </c>
       <c r="C75" s="3" t="inlineStr">
         <is>
-          <t>Especificar módulo completo de gestão de ordens de serviço (OS) incluindo criação, agendamento, execução, rastreamento de tempo, consumo de materiais, coleta de evidências digitais e finalização com assinatura digital.</t>
+          <t>Especificar módulo completo de gestão de ordens de serviço (OS) incluindo criação, agendamento, execução, rastreamento de tempo, consumo de materiais, coleta de evidências digitais e finalização co...</t>
         </is>
       </c>
       <c r="D75" s="3" t="inlineStr">
         <is>
-          <t>Validação de transição de estados (Rascunho → Pendente Aprovação → Aprovada → Agendada → Em Execução → Concluída | Cancelada). Estados Concluída e Cancelada são terminais.. Obrigatoriedade de checklist completo antes de conclusão. Todos os itens devem estar preenchidos.. Assinatura digital obrigatória em conclusão com timestamp UTC, nome signatário e hash SHA-256.. Agendamento requer disponibilidade de técnico. Sistema valida automaticamente conflitos de horário.. Duração real não pode exceder estimada em &gt;20% sem justificativa textual obrigatória.. Consumo de materiais reduz estoque automaticamente APENAS após conclusão. Falta de estoque bloqueia conclusão.. Conformidade com SLA de atendimento. Sistema valida prazo de resposta ao iniciar execução e registra violação se aplicável.. Rastreamento de tempo com pausa/retomada auditada. Cada pausa registrada com timestamp UTC e motivo.. Validação de fotos/evidências com metadados EXIF obrigatórios (data/hora captura). Fotos sem EXIF são rejeitadas.. Relatórios de produtividade por técnico baseados APENAS em OS concluídas (total, tempo médio, conformidade SLA, custo materiais).</t>
+          <t>Validação de transição de estados (Rascunho → Pendente Aprovação → Aprovada → Agendada → Em Execução → Concluída | Cancelada). Estados Concluída e Cancelada são terminais.. Obrigatoriedade de checklist completo antes de conclusão. Todos os itens devem estar preenchidos.. Assinatura digital obrigatória em conclusão com timestamp UTC, nome signatário e hash SHA-256.. Agendamento requer disponibilidade de técnico. Sistema valida automaticamente conflitos de horário.. Duração real não pode exceder estimada em &gt;20% sem justificativa textual obrigatória.</t>
         </is>
       </c>
       <c r="E75" s="3" t="inlineStr"/>
@@ -1958,15 +2249,19 @@
           <t>RF078</t>
         </is>
       </c>
-      <c r="B76" s="3" t="inlineStr"/>
+      <c r="B76" s="3" t="inlineStr">
+        <is>
+          <t>Integração com ERPs</t>
+        </is>
+      </c>
       <c r="C76" s="3" t="inlineStr">
         <is>
-          <t>Estabelecer comunicação bidirecional e em tempo real entre o IControlIT e sistemas ERP (SAP, TOTVS Protheus, Oracle EBS), permitindo sincronização automática de dados mestres, operações transacionais e auditoria completa de conformidade fiscal.</t>
+          <t>Estabelecer comunicação bidirecional e em tempo real entre o IControlIT e sistemas ERP (SAP, TOTVS Protheus, Oracle EBS), permitindo sincronização automática de dados mestres, operações transaciona...</t>
         </is>
       </c>
       <c r="D76" s="3" t="inlineStr">
         <is>
-          <t>Sincronização de Centros de Custo deve ser bidirecional. Credenciais de ERP devem ser armazenadas em Azure Key Vault com rotação automática. Integrações com falha devem registrar na DLQ e notificar administrador. Exportação de custos de TI deve respeitar centro de custo e período contábil. Cada mensagem integrada deve ter identificador único (UUID) para deduplicação. Transformação de dados deve validar schema e tipo de campo antes de processar. Logs de integração devem registrar entrada, saída e erro em tabela estruturada com retenção de 7 anos. Webhooks de ERP devem validar assinatura HMAC-SHA256 antes de processar. Dados sensíveis (salários, valores de contrato) devem ser criptografados em campo específico na auditoria. Reconciliação de faturas telecom com contas a pagar do ERP deve considerar tolerância de diferença de 0,5%.</t>
+          <t>Sincronização de Centros de Custo deve ser bidirecional. Credenciais de ERP devem ser armazenadas em Azure Key Vault com rotação automática. Integrações com falha devem registrar na DLQ e notificar administrador. Exportação de custos de TI deve respeitar centro de custo e período contábil. Cada mensagem integrada deve ter identificador único (UUID) para deduplicação.</t>
         </is>
       </c>
       <c r="E76" s="3" t="inlineStr"/>
@@ -1977,7 +2272,11 @@
           <t>RF079</t>
         </is>
       </c>
-      <c r="B77" s="3" t="inlineStr"/>
+      <c r="B77" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Políticas e Compliance</t>
+        </is>
+      </c>
       <c r="C77" s="3" t="inlineStr">
         <is>
           <t>Centralizar, versionizar e rastrear o cumprimento de políticas corporativas em toda a organização, garantindo conformidade com regulamentações (LGPD, SOX, ISO 27001, ISO 20000, ITIL v4)</t>
@@ -1985,7 +2284,7 @@
       </c>
       <c r="D77" s="3" t="inlineStr">
         <is>
-          <t>Versionamento automático de políticas - alteração em estado Elaboração ou Revisão incrementa versão e cria histórico imutável. Aceite obrigatório de políticas publicadas - usuário bloqueado até aceitar, aceite registrado com timestamp, IP e User-Agent. Workflow de aprovação multi-nível - transições de estado exigem aprovador com perfil específico. Matriz de compliance - política publicada deve estar mapeada a uma ou mais regulamentações (LGPD, SOX, ISO 27001, ISO 20000, ITIL v4). Detecção automática de não-conformidade - job diário verifica aceites e regras configuradas, gera alertas. Gestão de exceções de conformidade - aprovador pode conceder exceção temporária com data de expiração. Dashboard de compliance em tempo real - taxa de conformidade geral e por dimensões (política, departamento, usuário). Notificações de atualização e violação - envio automático via email, in-app e SMS (opcional). Busca full-text em políticas - performance &lt; 200ms P95, tolerância a erros de digitação. Integração com auditoria - todas as operações registradas com código padronizado (POL_*), retenção 7 anos. Isolamento multi-tenant - usuário acessa apenas dados do próprio ClienteId. Permissões RBAC - cada operação exige permissão explícita (compliance:politica:*, compliance:dashboard:*, compliance:excepcao:*).</t>
+          <t>Versionamento automático de políticas - alteração em estado Elaboração ou Revisão incrementa versão e cria histórico imutável. Aceite obrigatório de políticas publicadas - usuário bloqueado até aceitar, aceite registrado com timestamp, IP e User-Agent. Workflow de aprovação multi-nível - transições de estado exigem aprovador com perfil específico. Matriz de compliance - política publicada deve estar mapeada a uma ou mais regulamentações (LGPD, SOX, ISO 27001, ISO 20000, ITIL v4). Detecção automática de não-conformidade - job diário verifica aceites e regras configuradas, gera alertas.</t>
         </is>
       </c>
       <c r="E77" s="3" t="inlineStr"/>
@@ -1996,19 +2295,20 @@
           <t>RF080</t>
         </is>
       </c>
-      <c r="B78" s="3" t="inlineStr"/>
+      <c r="B78" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Termos de Aceite e LGPD</t>
+        </is>
+      </c>
       <c r="C78" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Implementar módulo completo de Gestão de Termos de Aceite e LGPD que permita ao sistema IControlIT
-atender integralmente às exigências da LGPD (Lei 13.709/2018), GDPR e ISO 27701 através de versionamento
-automático, aceite obrigatório, consentimentos granulares, revogação, portabilidade, anonimização e
-auditoria completa.
-</t>
+          <t>Implementar módulo completo de Gestão de Termos de Aceite e LGPD que permita ao sistema IControlIT
+atender integralmente às exigências da LGPD (Lei 13.709/2018), GDPR e ISO 27701 através de version...</t>
         </is>
       </c>
       <c r="D78" s="3" t="inlineStr">
         <is>
-          <t>Aceite Obrigatório no Primeiro Acesso - Usuário bloqueado até aceitar termo vigente. Versionamento Automático de Termos - Alteração de conteúdo gera nova versão. Consentimentos Granulares - Marketing, Analytics, Cookies, Compartilhamento independentes. Revogação de Consentimento Imediata - Usuário pode revogar a qualquer momento sem justificativa. Portabilidade de Dados - Exportação em formato estruturado (JSON/CSV/XML). Anonimização Irreversível - Remoção permanente de identificadores pessoais. Auditoria Completa de Consentimentos - Registro com timestamp ISO 8601, IP, User-Agent, hash SHA256. Integração com RF079 - Termos vinculados a políticas corporativas. Notificações Multi-Canal - E-mail, SMS e in-app (SignalR) para atualização de termos. Multi-idioma - pt-BR, en-US, es-ES com fallback automático. Dashboard de Conformidade - Métricas em tempo real de aceites, revogações e evolução. Assinatura Digital Opcional - Certificado A1/A3 validado com AC Raiz Brasileira. Isolamento por Tenant - Termos e consentimentos isolados por empresa. Validação de Campos Obrigatórios - Título, descrição, conteúdo, tipo e idioma. Proteção Contra XSS e Injeção - HTML sanitizado, escape de caracteres, parameterized queries.</t>
+          <t>Aceite Obrigatório no Primeiro Acesso - Usuário bloqueado até aceitar termo vigente. Versionamento Automático de Termos - Alteração de conteúdo gera nova versão. Consentimentos Granulares - Marketing, Analytics, Cookies, Compartilhamento independentes. Revogação de Consentimento Imediata - Usuário pode revogar a qualquer momento sem justificativa. Portabilidade de Dados - Exportação em formato estruturado (JSON/CSV/XML).</t>
         </is>
       </c>
       <c r="E78" s="3" t="inlineStr"/>
@@ -2019,7 +2319,11 @@
           <t>RF081</t>
         </is>
       </c>
-      <c r="B79" s="3" t="inlineStr"/>
+      <c r="B79" s="3" t="inlineStr">
+        <is>
+          <t>Termos de Responsabilidade por Ativos e Equipamentos</t>
+        </is>
+      </c>
       <c r="C79" s="3" t="inlineStr">
         <is>
           <t>Garantir que 100% dos ativos entregues sejam formalmente aceitos por seus responsáveis, criando prova legal de custódia para proteção patrimonial, conformidade LGPD e eficiência operacional.</t>
@@ -2027,7 +2331,7 @@
       </c>
       <c r="D79" s="3" t="inlineStr">
         <is>
-          <t>Sistema DEVE suportar no mínimo 12 tipos de ativos diferentes, cada um com termo customizado. Antes de capturar aceite, sistema DEVE validar identidade do usuário via CPF (BrasilAPI) ou matrícula corporativa. Aceite DEVE capturar assinatura rasterizada (PNG) via SignaturePad, timestamp UTC sincronizado (NTP), geolocalização (IP + GPS se autorizado), User-Agent. Quando conteúdo de termo é alterado, sistema cria automaticamente nova versão com histórico completo e changelog. Versões anteriores são imutáveis (append-only). Usuário que recebeu equipamento novo ou cujo termo está vencido NÃO pode acessar certos módulos do sistema até aceitar termo vigente. Sistema DEVE gerar notificações automáticas (email, SMS, in-app via SignalR) com 30, 15 e 7 dias antes do vencimento. Quando termo vence e ativo não é devolvido, sistema calcula automaticamente multa de retenção (fixa diária, progressiva ou custo de reposição). Quando equipamento é devolvido ou perdido, termo é revogado automaticamente com registro imutável de data, motivo, quem revogou. Dashboard exibe métricas em tempo real: total aceites (Pendente/Ativo/Vencido/Revogado), taxa aceite (%), tempo médio, penalidades acumuladas. Após aceitar termo, sistema gera PDF com QRCode único que permite verificar autenticidade online. Quando ativo é transferido para novo usuário via RF-027, webhook automático dispara criação de novo termo pendente de aceite. Interface e termos devem ser traduzidos para português, inglês e espanhol. Isolamento completo por ClienteId.</t>
+          <t>Sistema DEVE suportar no mínimo 12 tipos de ativos diferentes, cada um com termo customizado. Antes de capturar aceite, sistema DEVE validar identidade do usuário via CPF (BrasilAPI) ou matrícula corporativa. Aceite DEVE capturar assinatura rasterizada (PNG) via SignaturePad, timestamp UTC sincronizado (NTP), geolocalização (IP + GPS se autorizado), User-Agent. Quando conteúdo de termo é alterado, sistema cria automaticamente nova versão com histórico completo e changelog. Versões anteriores são imutáveis (append-only). Usuário que recebeu equipamento novo ou cujo termo está vencido NÃO pode acessar certos módulos do sistema até aceitar termo vigente.</t>
         </is>
       </c>
       <c r="E79" s="3" t="inlineStr"/>
@@ -2038,7 +2342,11 @@
           <t>RF084</t>
         </is>
       </c>
-      <c r="B80" s="3" t="inlineStr"/>
+      <c r="B80" s="3" t="inlineStr">
+        <is>
+          <t>Upload e Importação de Arquivos</t>
+        </is>
+      </c>
       <c r="C80" s="3" t="inlineStr">
         <is>
           <t>Prover serviço seguro e escalável de upload e importação de arquivos em diversos formatos com validação prévia, processamento assíncrono e auditoria completa</t>
@@ -2046,7 +2354,7 @@
       </c>
       <c r="D80" s="3" t="inlineStr">
         <is>
-          <t>Limite de Tamanho de Arquivo. Whitelist de Tipos MIME. Validação de Extensão Consistente. Scan Antivírus Obrigatório. Separação Upload e Importação. Validação de Schema Obrigatória. Validação de Dados por Linha. Processamento Assíncrono Automático. Progresso em Tempo Real. Rollback Transacional. Isolamento Multi-Tenant. Auditoria Completa.</t>
+          <t>Limite de Tamanho de Arquivo. Whitelist de Tipos MIME. Validação de Extensão Consistente. Scan Antivírus Obrigatório. Separação Upload e Importação.</t>
         </is>
       </c>
       <c r="E80" s="3" t="inlineStr"/>
@@ -2057,11 +2365,19 @@
           <t>RF085</t>
         </is>
       </c>
-      <c r="B81" s="3" t="inlineStr"/>
-      <c r="C81" s="3" t="inlineStr"/>
+      <c r="B81" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C81" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D81" s="3" t="inlineStr">
         <is>
-          <t>Mapeamento de Campos Obrigatório. Transformação de Dados Conforme Template. Validação de Dados Contra Regras de Negócio. Detecção de Duplicatas por Chave Natural. Importação Incremental (Delta Detection). Agendamento Recorrente com Hangfire. Histórico de Importações com Rollback. Validação Transacional (Tudo ou Nada). API de Status de Importação em Tempo Real. Relatório Detalhado de Erros com Sugestões. Isolamento Multi-Tenant. Validação de Tamanho e Tipo de Arquivo. Scan Antivírus Obrigatório.</t>
+          <t>Mapeamento de Campos Obrigatório. Transformação de Dados Conforme Template. Validação de Dados Contra Regras de Negócio. Detecção de Duplicatas por Chave Natural. Importação Incremental (Delta Detection).</t>
         </is>
       </c>
       <c r="E81" s="3" t="inlineStr"/>
@@ -2072,7 +2388,11 @@
           <t>RF086</t>
         </is>
       </c>
-      <c r="B82" s="3" t="inlineStr"/>
+      <c r="B82" s="3" t="inlineStr">
+        <is>
+          <t>Carga e Importação de Dados - Faturas, Consumo e Inventário</t>
+        </is>
+      </c>
       <c r="C82" s="3" t="inlineStr">
         <is>
           <t>Automatizar ingestão, validação, processamento e conciliação de faturas de operadoras de telecomunicações</t>
@@ -2080,7 +2400,7 @@
       </c>
       <c r="D82" s="3" t="inlineStr">
         <is>
-          <t>Validação de Formato de Arquivo. Parser Específico por Operadora. Registro de CDR com Rastreamento Completo. Validação de Integridade de Totalizações. Detecção de Cobranças Duplicadas. Conciliação Automática Fatura vs CDRs. Glosa Automática de Cobranças Indevidas. Histórico Completo de Importações. Integração com Módulo de Notas Fiscais (RF032). Processamento Assíncrono via Hangfire.</t>
+          <t>Validação de Formato de Arquivo. Parser Específico por Operadora. Registro de CDR com Rastreamento Completo. Validação de Integridade de Totalizações. Detecção de Cobranças Duplicadas.</t>
         </is>
       </c>
       <c r="E82" s="3" t="inlineStr"/>
@@ -2091,15 +2411,19 @@
           <t>RF087</t>
         </is>
       </c>
-      <c r="B83" s="3" t="inlineStr"/>
+      <c r="B83" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Integrações e APIs Externas</t>
+        </is>
+      </c>
       <c r="C83" s="3" t="inlineStr">
         <is>
-          <t>Permitir que administradores configurem e gerenciem integrações com sistemas externos de forma segura, monitorável e resiliente, garantindo isolamento por tenant, criptografia de credenciais e rastreabilidade completa de execuções.</t>
+          <t>Permitir que administradores configurem e gerenciem integrações com sistemas externos de forma segura, monitorável e resiliente, garantindo isolamento por tenant, criptografia de credenciais e rast...</t>
         </is>
       </c>
       <c r="D83" s="3" t="inlineStr">
         <is>
-          <t>Código Único de Integração. Tipos de Integração Suportados. Métodos de Autenticação Permitidos. Credenciais Criptografadas. Timeout Configurável. Circuit Breaker. Rate Limiting. Retry com Backoff Exponencial. Validação de URL Base. Certificados SSL. Endpoints Configuráveis. Estatísticas de Execução. Webhooks com Validação HMAC. Filas de Processamento. Auditoria de Execuções.</t>
+          <t>Código Único de Integração. Tipos de Integração Suportados. Métodos de Autenticação Permitidos. Credenciais Criptografadas. Timeout Configurável.</t>
         </is>
       </c>
       <c r="E83" s="3" t="inlineStr"/>
@@ -2110,11 +2434,19 @@
           <t>RF088</t>
         </is>
       </c>
-      <c r="B84" s="3" t="inlineStr"/>
-      <c r="C84" s="3" t="inlineStr"/>
+      <c r="B84" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C84" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D84" s="3" t="inlineStr">
         <is>
-          <t>Workflow deve ter pelo menos um estado inicial e um final. Transição condicional deve bloquear movimento se condição não atende. Aprovação paralela requer quórum conforme configuração. Delegação deve respeitar data de expiração e ser auditada. SLA de Aprovação dispara alerta em T-24h e escalação em T+0. Aprovador só pode exercer aprovação se tiver permissão RBAC explícita. Estados finais são imutáveis; documentos não podem sair de estado final. Notificações devem incluir contexto mínimo (Who, What, When, Why, How). Rejeição é irrevogável; documento volta ao estado anterior. Histórico de Aprovação deve ser imutável e conservado 7 anos (LGPD).</t>
+          <t>Workflow deve ter pelo menos um estado inicial e um final. Transição condicional deve bloquear movimento se condição não atende. Aprovação paralela requer quórum conforme configuração. Delegação deve respeitar data de expiração e ser auditada. SLA de Aprovação dispara alerta em T-24h e escalação em T+0.</t>
         </is>
       </c>
       <c r="E84" s="3" t="inlineStr"/>
@@ -2125,17 +2457,20 @@
           <t>RF089</t>
         </is>
       </c>
-      <c r="B85" s="3" t="inlineStr"/>
+      <c r="B85" s="3" t="inlineStr">
+        <is>
+          <t>Conciliação e Auditoria de Faturas</t>
+        </is>
+      </c>
       <c r="C85" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Implementar sistema automatizado de conciliação e auditoria de faturas (NF-e) com matching multi-nível,
-detecção de divergências, workflow de aprovação, ML para anomalias, conciliação bancária e relatórios SPED.
-</t>
+          <t>Implementar sistema automatizado de conciliação e auditoria de faturas (NF-e) com matching multi-nível,
+detecção de divergências, workflow de aprovação, ML para anomalias, conciliação bancária e re...</t>
         </is>
       </c>
       <c r="D85" s="3" t="inlineStr">
         <is>
-          <t>Toda NF-e deve ser associada a um Pedido de Compra com CHAVE_NFE válida (44 dígitos). Divergências devem ser classificadas em CRÍTICA (&gt;10%), ALTA (5-10%), MÉDIA (2-5%) ou BAIXA (&lt;2%). Three-way matching deve validar PC → RM → NF-e com tolerâncias configuráveis. Validação de termos contratuais (preço, prazo, desconto, alíquotas). Detecção de anomalias com ML (score &gt;0.75 = revisar, &gt;0.5 = supervisão). Workflow de aprovação com roteamento automático e SLA (CRÍTICA: 4h, ALTA: 24h, MÉDIA: 72h). Bloqueio automático de pagamentos em divergências CRÍTICAS e ALTAS. Conciliação bancária automática com matching de valor e data (±5 dias). Auditoria completa com event sourcing e hash SHA-512. Exportação de relatórios fiscais SPED (E-100, E-200, E-310).</t>
+          <t>Toda NF-e deve ser associada a um Pedido de Compra com CHAVE_NFE válida (44 dígitos). Divergências devem ser classificadas em CRÍTICA (&gt;10%), ALTA (5-10%), MÉDIA (2-5%) ou BAIXA (&lt;2%). Three-way matching deve validar PC → RM → NF-e com tolerâncias configuráveis. Validação de termos contratuais (preço, prazo, desconto, alíquotas). Detecção de anomalias com ML (score &gt;0.75 = revisar, &gt;0.5 = supervisão).</t>
         </is>
       </c>
       <c r="E85" s="3" t="inlineStr"/>
@@ -2146,20 +2481,21 @@
           <t>RF090</t>
         </is>
       </c>
-      <c r="B86" s="3" t="inlineStr"/>
+      <c r="B86" s="3" t="inlineStr">
+        <is>
+          <t>Medição e Faturamento de Contratos</t>
+        </is>
+      </c>
       <c r="C86" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Especificar o comportamento do módulo de Medição e Faturamento de Contratos do sistema IControlIT,
+          <t>Especificar o comportamento do módulo de Medição e Faturamento de Contratos do sistema IControlIT,
 responsável pela gestão completa do ciclo de medições de consumo/serviços prestados vinculados a
-contratos comerciais, cálculo automático de valores faturáveis, aplicação de reajustes contratuais,
-rateio entre centros de custo, geração de faturas, gestão de glosas de valores contestados e
-rastreamento imutável de toda operação para conformidade fiscal e contábil.
-</t>
+c...</t>
         </is>
       </c>
       <c r="D86" s="3" t="inlineStr">
         <is>
-          <t>Todo período de medição deve estar dentro da vigência do contrato associado. Não é permitido criar medições com períodos sobrepostos para o mesmo contrato. Valor faturável calculado conforme tipo: Fixa=ValorFixo, Variável=Quantidade×ValorUnitario, Híbrida=ValorFixo+(Quantidade×ValorUnitario). Reajustes automáticos aplicados em data de aniversário conforme índice configurado (IGPM, IPCA, INPC, Percentual Fixo). Soma de percentuais de rateio deve ser exatamente 100% (tolerância 0,01%). Toda medição deve estar vinculada a contrato válido (FK obrigatória, contrato ativo, dentro vigência). Medições seguem state machine com 5 estados e transições validadas (Rascunho→PendenteAprovacao→Aprovada→Faturada→Glosa). Após aprovação, job automático cria nota fiscal via RF032 e marca medição como Faturada. Cliente pode contestar fatura com glosa (percentual + justificativa), gestor analisa e aprova/rejeita. Toda operação registrada em tabela de auditoria com retenção 7 anos (timestamp UTC, usuário, IP, operação, valores antes/depois JSON, hash SHA-256).</t>
+          <t>Todo período de medição deve estar dentro da vigência do contrato associado. Não é permitido criar medições com períodos sobrepostos para o mesmo contrato. Valor faturável calculado conforme tipo: Fixa=ValorFixo, Variável=Quantidade×ValorUnitario, Híbrida=ValorFixo+(Quantidade×ValorUnitario). Reajustes automáticos aplicados em data de aniversário conforme índice configurado (IGPM, IPCA, INPC, Percentual Fixo). Soma de percentuais de rateio deve ser exatamente 100% (tolerância 0,01%).</t>
         </is>
       </c>
       <c r="E86" s="3" t="inlineStr"/>
@@ -2170,7 +2506,11 @@
           <t>RF091</t>
         </is>
       </c>
-      <c r="B87" s="3" t="inlineStr"/>
+      <c r="B87" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Anexos e Documentos Contratuais</t>
+        </is>
+      </c>
       <c r="C87" s="3" t="inlineStr">
         <is>
           <t>Gerenciar o ciclo de vida completo de documentos e anexos associados a contratos com segurança, versionamento, auditoria e conformidade legal (LGPD, ISO 27001).</t>
@@ -2178,7 +2518,7 @@
       </c>
       <c r="D87" s="3" t="inlineStr">
         <is>
-          <t>Validação de tipo de arquivo por whitelist (extensão + MIME type). Limite de tamanho de arquivo (50MB máximo). Scan obrigatório de antivírus (ClamAV) antes de armazenar. Cálculo de hash SHA-256 para validação de integridade. Versionamento imutável (cada upload cria nova versão). Armazenamento em Azure Blob Storage com criptografia AES-256. Controle de acesso granular (RBAC + Policy) com delegação temporal. Download seguro com SAS token temporário (15 minutos). Watermark visual em PDFs baixados. OCR e indexação full-text (Elasticsearch). Integração com DocuSign para assinatura digital. Validação de documentação obrigatória por tipo de contrato. Auditoria não-repudiável de todas operações. Isolamento multi-tenant estrito (ClienteId). Compartilhamento com delegação temporal.</t>
+          <t>Validação de tipo de arquivo por whitelist (extensão + MIME type). Limite de tamanho de arquivo (50MB máximo). Scan obrigatório de antivírus (ClamAV) antes de armazenar. Cálculo de hash SHA-256 para validação de integridade. Versionamento imutável (cada upload cria nova versão).</t>
         </is>
       </c>
       <c r="E87" s="3" t="inlineStr"/>
@@ -2189,11 +2529,19 @@
           <t>RF092</t>
         </is>
       </c>
-      <c r="B88" s="3" t="inlineStr"/>
-      <c r="C88" s="3" t="inlineStr"/>
+      <c r="B88" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C88" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D88" s="3" t="inlineStr">
         <is>
-          <t>Garantia deve estar vinculada a um ativo válido. Data de término deve ser posterior à data de início. Alertas automáticos de vencimento em 90, 60, 30 e 15 dias. Número de apólice único por seguradora. Sinistros apenas para apólices ativas. Cálculo de cobertura total por ativo. Workflow formal de estados de sinistro. Renovação automática de apólices 30 dias antes do vencimento. Auditoria completa de todas as operações. Não permitir sobreposição de períodos de garantia para mesmo ativo. Franquia deve ser menor que limite máximo de cobertura. Status de garantia derivado das datas de vigência. Prêmio anual calculado automaticamente como mensal * 12. Sinistro recusado não pode ser reaberto automaticamente. Apólice cancelada rejeita novos sinistros.</t>
+          <t>Garantia deve estar vinculada a um ativo válido. Data de término deve ser posterior à data de início. Alertas automáticos de vencimento em 90, 60, 30 e 15 dias. Número de apólice único por seguradora. Sinistros apenas para apólices ativas.</t>
         </is>
       </c>
       <c r="E88" s="3" t="inlineStr"/>
@@ -2211,15 +2559,14 @@
       </c>
       <c r="C89" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Implementar sistema completo de gestão de KPIs (Key Performance Indicators) para IControlIT,
+          <t>Implementar sistema completo de gestão de KPIs (Key Performance Indicators) para IControlIT,
 permitindo definição, cálculo automático, acompanhamento e análise de métricas críticas
-relacionadas a SLA, contratos, ativos, custos e compliance.
-</t>
+relacionadas a S...</t>
         </is>
       </c>
       <c r="D89" s="3" t="inlineStr">
         <is>
-          <t>Todo KPI deve possuir código único, nome, descrição, tipo, fórmula, unidade, agregação e periodicidade. Fórmulas devem ser validadas antes da gravação (sintaxe, balanceamento, campos, divisão por zero, referências circulares). KPIs devem ser calculados automaticamente conforme periodicidade com retry até 3 vezes. Cada KPI pode ter metas com três zonas (verde/amarelo/vermelho) e vigência definida. Cálculo automático de métricas de SLA baseado em solicitações finalizadas. Cálculo de métricas contratuais considerando apenas contratos vigentes. Cálculo de TCO, utilização e disponibilidade de ativos. Alertas gerados automaticamente quando KPI atinge zona amarela ou vermelha. Todo cálculo e alteração deve ser registrado com snapshot de dados. Sistema disponibiliza endpoint OData e WDC com autenticação via API Key.</t>
+          <t>Todo KPI deve possuir código único, nome, descrição, tipo, fórmula, unidade, agregação e periodicidade. Fórmulas devem ser validadas antes da gravação (sintaxe, balanceamento, campos, divisão por zero, referências circulares). KPIs devem ser calculados automaticamente conforme periodicidade com retry até 3 vezes. Cada KPI pode ter metas com três zonas (verde/amarelo/vermelho) e vigência definida. Cálculo automático de métricas de SLA baseado em solicitações finalizadas.</t>
         </is>
       </c>
       <c r="E89" s="3" t="inlineStr"/>
@@ -2230,11 +2577,19 @@
           <t>RF094</t>
         </is>
       </c>
-      <c r="B90" s="3" t="inlineStr"/>
-      <c r="C90" s="3" t="inlineStr"/>
+      <c r="B90" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C90" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D90" s="3" t="inlineStr">
         <is>
-          <t>Cálculo de Variância. Detecção de Anomalias por Z-Score. Categorização de Severidade de Anomalias. Cálculo de TCO (Total Cost of Ownership). Cálculo de ROI (Return on Investment). Identificação de Desperdícios. Alertas de Não-Conformidade Automáticos. Auditoria de Acesso com LGPD. Cálculo de Depreciação de Ativos. Jobs de Análise Batch (Hangfire).</t>
+          <t>Cálculo de Variância. Detecção de Anomalias por Z-Score. Categorização de Severidade de Anomalias. Cálculo de TCO (Total Cost of Ownership). Cálculo de ROI (Return on Investment).</t>
         </is>
       </c>
       <c r="E90" s="3" t="inlineStr"/>
@@ -2245,7 +2600,11 @@
           <t>RF095</t>
         </is>
       </c>
-      <c r="B91" s="3" t="inlineStr"/>
+      <c r="B91" s="3" t="inlineStr">
+        <is>
+          <t>Auditoria de Acesso e Segurança</t>
+        </is>
+      </c>
       <c r="C91" s="3" t="inlineStr">
         <is>
           <t>Implementar sistema completo de auditoria de acesso e segurança para garantir conformidade com LGPD, ISO 27001, SOX 404 e PCI-DSS</t>
@@ -2253,7 +2612,7 @@
       </c>
       <c r="D91" s="3" t="inlineStr">
         <is>
-          <t>Toda tentativa de login deve ser registrada com timestamp UTC, email, IP, dispositivo, navegador, geolocalização e resultado. Detectar força bruta: 5 falhas gera alerta, 10 falhas bloqueia IP por 60 min. Toda operação CRUD deve ser auditada com usuário, timestamp, entidade, ação, dados antes/depois. Validar segregação de funções em tempo real bloqueando permissões conflitantes. Acessos privilegiados temporários (máximo 4h) com aprovação dual-control. Certificação trimestral de permissões com revogação em 72h se rejeitado. Detecção de anomalias com score 0.0-1.0, alerta se &gt;0.7. Aplicar políticas de segurança em tempo real (IP, MFA, horário, localização). Correlação de eventos por CorrelationId para investigação forense. Alertas automáticos em &lt;1 min com score de risco e canal apropriado. Retenção de logs em camadas (hot/warm/cold) por 10 anos com criptografia AES-256. Dashboard atualizado a cada 5 min com filtros e acesso restrito.</t>
+          <t>Toda tentativa de login deve ser registrada com timestamp UTC, email, IP, dispositivo, navegador, geolocalização e resultado. Detectar força bruta: 5 falhas gera alerta, 10 falhas bloqueia IP por 60 min. Toda operação CRUD deve ser auditada com usuário, timestamp, entidade, ação, dados antes/depois. Validar segregação de funções em tempo real bloqueando permissões conflitantes. Acessos privilegiados temporários (máximo 4h) com aprovação dual-control.</t>
         </is>
       </c>
       <c r="E91" s="3" t="inlineStr"/>
@@ -2264,7 +2623,11 @@
           <t>RF096</t>
         </is>
       </c>
-      <c r="B92" s="3" t="inlineStr"/>
+      <c r="B92" s="3" t="inlineStr">
+        <is>
+          <t>Auditoria de Mudanças de Dados</t>
+        </is>
+      </c>
       <c r="C92" s="3" t="inlineStr">
         <is>
           <t>Garantir rastreabilidade total de todas as operações de criação, alteração e exclusão de dados em entidades críticas do sistema, com contexto completo de execução e conformidade LGPD/SOX 404.</t>
@@ -2272,7 +2635,7 @@
       </c>
       <c r="D92" s="3" t="inlineStr">
         <is>
-          <t>Toda entidade decorada com atributo de auditoria deve ter rastreamento automático de Create, Update e Delete sem necessidade de código adicional no handler.. Para toda alteração (Update), o sistema deve capturar valores anteriores e posteriores em nível de campo, junto com contexto completo de execução.. Registros de auditoria são append-only e não podem ser alterados ou excluídos após inserção, garantindo integridade da trilha de auditoria.. Exclusões lógicas (soft delete) devem ser rastreadas como operações auditadas, registrando quem excluiu, quando e contexto completo.. Quando múltiplas entidades são alteradas em uma única transação, o sistema deve detectar automaticamente e agrupar com CorrelationId único.. Adições e remoções de entidades relacionadas (collections) devem ser rastreadas como operações específicas de relacionamento.. Registros de auditoria devem ser retidos conforme prazos legais (5 anos LGPD para dados pessoais, 7 anos SOX 404 para dados financeiros) e automaticamente arquivados/purgados.. Alterações em campos de dados sensíveis (CPF, e-mail, telefone, endereço) devem gerar alertas automáticos para o DPO (Data Protection Officer).. Usuários com permissão devem poder visualizar timeline completa de alterações em uma entidade, com filtros por período, usuário, campo alterado e tipo de operação.. Usuários com permissão específica (Admin + Developer) devem poder restaurar versões anteriores de entidades, com validação de integridade referencial antes de aplicar.. Sistema deve gerar relatórios parametrizados de auditoria com agregações, totalizações e exportação em múltiplos formatos.. Dashboard em tempo real deve exibir métricas de auditoria e alertas automáticos de padrões anômalos de alteração.. Eventos de auditoria críticos devem ser enviados automaticamente para Azure Sentinel em tempo real, no formato CEF (Common Event Format).. Exportações forenses de trilhas de auditoria devem incluir hash SHA-256 de cada registro e assinatura digital do arquivo, garantindo integridade para uso em processos judiciais.. Todos os registros de auditoria devem ser isolados por ClienteId, garantindo que clientes não visualizem auditoria de outros clientes.. Consultas de auditoria com filtros complexos não podem exceder 2 segundos de latência, mesmo com milhões de registros.. Tentativas de alteração ou exclusão de registros de auditoria devem ser detectadas e registradas automaticamente como violações de segurança.. Campos calculados ou derivados (computed properties) não devem gerar registros de auditoria, evitando poluição de trilha.. Todos os timestamps de auditoria devem usar UTC e ser armazenados com precisão de milissegundos.. Importações em massa (bulk insert) devem gerar registros de auditoria agrupados com CorrelationId específico de batch.</t>
+          <t>Toda entidade decorada com atributo de auditoria deve ter rastreamento automático de Create, Update e Delete sem necessidade de código adicional no handler.. Para toda alteração (Update), o sistema deve capturar valores anteriores e posteriores em nível de campo, junto com contexto completo de execução.. Registros de auditoria são append-only e não podem ser alterados ou excluídos após inserção, garantindo integridade da trilha de auditoria.. Exclusões lógicas (soft delete) devem ser rastreadas como operações auditadas, registrando quem excluiu, quando e contexto completo.. Quando múltiplas entidades são alteradas em uma única transação, o sistema deve detectar automaticamente e agrupar com CorrelationId único.</t>
         </is>
       </c>
       <c r="E92" s="3" t="inlineStr"/>
@@ -2283,15 +2646,19 @@
           <t>RF097</t>
         </is>
       </c>
-      <c r="B93" s="3" t="inlineStr"/>
+      <c r="B93" s="3" t="inlineStr">
+        <is>
+          <t>Auditoria de Faturas (NF-e e Documentos Fiscais)</t>
+        </is>
+      </c>
       <c r="C93" s="3" t="inlineStr">
         <is>
-          <t>Permitir auditoria fiscal automatizada de Notas Fiscais Eletrônicas (NF-e), validação de integridade (assinatura digital, chave de acesso, status SEFAZ), detecção de fraudes (duplicatas, operações anômalas), conferência de impostos (ICMS, IPI, PIS, COFINS, ISS), e conformidade com SPED Fiscal (EFD-ICMS/IPI).</t>
+          <t>Permitir auditoria fiscal automatizada de Notas Fiscais Eletrônicas (NF-e), validação de integridade (assinatura digital, chave de acesso, status SEFAZ), detecção de fraudes (duplicatas, operações ...</t>
         </is>
       </c>
       <c r="D93" s="3" t="inlineStr">
         <is>
-          <t>Validação Obrigatória de Chave de Acesso NF-e: toda NF-e importada ou registrada deve ter chave de acesso válida (44 dígitos numéricos), validada via algoritmo de verificação de dígito (módulo 11). Chaves inválidas são rejeitadas com erro HTTP 400.. Consulta Obrigatória de Status SEFAZ para NF-e Autorizada: ao validar NF-e com status 'Autorizada', o sistema deve consultar a situação atual no WebService SEFAZ. Se a NF-e estiver cancelada ou denegada no SEFAZ, um alerta crítico é gerado e a auditoria falha.. Validação de Alíquota ICMS Conforme CFOP: cada CFOP possui alíquotas padrão de ICMS conforme legislação estadual. O sistema valida se a alíquota aplicada na NF-e está dentro do range esperado (±2%). Divergências superiores geram alerta.. Detecção de NF-e Cancelada com Movimentação Posterior: se uma NF-e foi cancelada no SEFAZ, mas há registros de movimentação financeira, estoque ou contábil posteriores à data de cancelamento, um alerta crítico é gerado indicando inconsistência.. Validação de Integridade de Assinatura Digital (XML NF-e): toda NF-e em XML deve ter assinatura digital válida (certificado A1/A3). O sistema valida: (1) certificado não expirado, (2) cadeia de certificação válida, (3) assinatura XML íntegra. Falhas rejeitam a NF-e.. Validação de Base de Cálculo e Impostos: o sistema recalcula a base de cálculo de ICMS, IPI, PIS, COFINS, ISS conforme regras do CFOP e compara com os valores declarados na NF-e. Divergências superiores a R$ 0,10 geram alerta.. Detecção de Duplicatas (Mesma Chave ou CNPJ Duplicado): o sistema detecta: (1) duas NF-e com mesma chave de acesso, (2) mesmo CNPJ emitindo múltiplas NF-e com mesma numeração no mesmo mês. Ambas situações geram alerta crítico de possível fraude.. Validação de Conformidade SPED Fiscal (EFD-ICMS/IPI): toda NF-e de entrada/saída deve ser escriturada no SPED Fiscal (EFD-ICMS/IPI). O sistema valida se há registro correspondente no SPED Fiscal e se os valores batem (ICMS, IPI). Divergências geram alerta de não conformidade.. Validação de Retenções Obrigatórias (IRRF, CSLL, ISS, INSS): para NF-e de serviços (CFOP 5.933, 6.933), o sistema valida se as retenções obrigatórias foram aplicadas conforme legislação (IRRF 1,5%, CSLL 1%, ISS conforme município, INSS 11%). Ausência de retenção obrigatória gera alerta.. Detecção de Operações Anômalas via Machine Learning: o sistema utiliza modelo Azure ML treinado com histórico de NF-e para detectar anomalias (valores fora do padrão do fornecedor, horários incomuns de emissão, NCM incompatível com histórico). Score de anomalia &gt; 0.75 gera alerta de possível fraude.</t>
+          <t>Validação Obrigatória de Chave de Acesso NF-e: toda NF-e importada ou registrada deve ter chave de acesso válida (44 dígitos numéricos), validada via algoritmo de verificação de dígito (módulo 11). Chaves inválidas são rejeitadas com erro HTTP 400.. Consulta Obrigatória de Status SEFAZ para NF-e Autorizada: ao validar NF-e com status 'Autorizada', o sistema deve consultar a situação atual no WebService SEFAZ. Se a NF-e estiver cancelada ou denegada no SEFAZ, um alerta crítico é gerado e a auditoria falha.. Validação de Alíquota ICMS Conforme CFOP: cada CFOP possui alíquotas padrão de ICMS conforme legislação estadual. O sistema valida se a alíquota aplicada na NF-e está dentro do range esperado (±2%). Divergências superiores geram alerta.. Detecção de NF-e Cancelada com Movimentação Posterior: se uma NF-e foi cancelada no SEFAZ, mas há registros de movimentação financeira, estoque ou contábil posteriores à data de cancelamento, um alerta crítico é gerado indicando inconsistência.. Validação de Integridade de Assinatura Digital (XML NF-e): toda NF-e em XML deve ter assinatura digital válida (certificado A1/A3). O sistema valida: (1) certificado não expirado, (2) cadeia de certificação válida, (3) assinatura XML íntegra. Falhas rejeitam a NF-e.</t>
         </is>
       </c>
       <c r="E93" s="3" t="inlineStr"/>
@@ -2307,10 +2674,14 @@
           <t>Auditoria e Logs do Sistema</t>
         </is>
       </c>
-      <c r="C94" s="3" t="inlineStr"/>
+      <c r="C94" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D94" s="3" t="inlineStr">
         <is>
-          <t>Níveis de Severidade Obrigatórios. Contexto Obrigatório em Todos os Logs. CorrelationId Único Por Requisição. Retenção Diferenciada Por Severidade. Sanitização de Dados Sensíveis. Stack Trace Completo Para Exceções. Integração Obrigatória com Application Insights. Busca Performática em Grandes Volumes. Alertas Configuráveis Por Regra. Exportação com Limite de Volume. Auditoria de Acessos a Logs. Multi-Tenancy Estrito. Logs de Performance com Thresholds. Versionamento de Estrutura de Logs. Logs de Segurança Isolados.</t>
+          <t>Níveis de Severidade Obrigatórios. Contexto Obrigatório em Todos os Logs. CorrelationId Único Por Requisição. Retenção Diferenciada Por Severidade. Sanitização de Dados Sensíveis.</t>
         </is>
       </c>
       <c r="E94" s="3" t="inlineStr"/>
@@ -2326,10 +2697,14 @@
           <t>Dashboards e KPIs</t>
         </is>
       </c>
-      <c r="C95" s="3" t="inlineStr"/>
+      <c r="C95" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D95" s="3" t="inlineStr">
         <is>
-          <t>Dashboard deve ter no mínimo 4 widgets. KPI deve ter fórmula de cálculo definida. Meta de KPI deve ser configurável. Alertas disparam quando KPI &lt; 80% da meta (amarelo) ou &lt; 60% (vermelho). Refresh automático a cada 30 segundos via SignalR. Export para PDF deve incluir logo do cliente. Drill-down deve filtrar automaticamente próximo nível. Multi-tenancy obrigatório (ClienteId em filtros). Auditoria de acesso a dashboards sensíveis. Permissão granular por dashboard.</t>
+          <t>Dashboard deve ter no mínimo 4 widgets. KPI deve ter fórmula de cálculo definida. Meta de KPI deve ser configurável. Alertas disparam quando KPI &lt; 80% da meta (amarelo) ou &lt; 60% (vermelho). Refresh automático a cada 30 segundos via SignalR.</t>
         </is>
       </c>
       <c r="E95" s="3" t="inlineStr"/>
@@ -2340,11 +2715,19 @@
           <t>RF100</t>
         </is>
       </c>
-      <c r="B96" s="3" t="inlineStr"/>
-      <c r="C96" s="3" t="inlineStr"/>
+      <c r="B96" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C96" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D96" s="3" t="inlineStr">
         <is>
-          <t>Forecast Requer Mínimo 12 Meses de Histórico. Anomaly Detection com Threshold Configurável. Modelos ML Retreinados Mensalmente via Hangfire. Forecast Requer Intervalo de Confiança Mínimo 95%. Clustering Deve ter Mínimo 3 Clusters, Máximo 10. Churn Prediction com Score &gt;= 70% de Precisão. What-If Analysis Limitado a 5 Cenários Simultâneos. Resultados ML Cacheados por 24 Horas (Redis). Multi-tenancy - ClienteId em Todos os Datasets. Auditoria de Todas as Predições e Recomendações.</t>
+          <t>Forecast Requer Mínimo 12 Meses de Histórico. Anomaly Detection com Threshold Configurável. Modelos ML Retreinados Mensalmente via Hangfire. Forecast Requer Intervalo de Confiança Mínimo 95%. Clustering Deve ter Mínimo 3 Clusters, Máximo 10.</t>
         </is>
       </c>
       <c r="E96" s="3" t="inlineStr"/>
@@ -2355,17 +2738,20 @@
           <t>RF101</t>
         </is>
       </c>
-      <c r="B97" s="3" t="inlineStr"/>
+      <c r="B97" s="3" t="inlineStr">
+        <is>
+          <t>Dashboards Executivos Operacionais</t>
+        </is>
+      </c>
       <c r="C97" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fornecer dashboards executivos pré-definidos para públicos estratégicos (C-Level, Diretoria, Gerência Sênior),
-consolidando dados operacionais e financeiros em visualizações de alto impacto para tomada de decisão rápida.
-</t>
+          <t>Fornecer dashboards executivos pré-definidos para públicos estratégicos (C-Level, Diretoria, Gerência Sênior),
+consolidando dados operacionais e financeiros em visualizações de alto impacto para to...</t>
         </is>
       </c>
       <c r="D97" s="3" t="inlineStr">
         <is>
-          <t>Apenas usuários com perfis C-Level, Diretoria, Gerência Sênior e Analista Executivo podem acessar dashboards executivos. Dados agregados devem ser consolidados automaticamente via Hangfire às 6:00 AM UTC, job idempotente com registro de sucesso/falha. Forecast exige mínimo 12 meses de histórico. Modelo ARIMA/Regressão Linear deve atingir R² &gt;= 0.85 para validade. Budget vs Real calcula variação percentual. Alertas: &gt; 10% amarelo, &gt; 20% vermelho. Heatmap usa escala de cores: verde &lt; 80% meta, amarelo 80-100%, vermelho &gt; 100%. Cores acessíveis WCAG AA. Trending permite granularidades: diária (30d), semanal (13s), mensal (12m). Linha tendência via regressão linear. SLA mostra % atendimento vs meta contratual. Verde &gt;= meta, amarelo 95-99% meta, vermelho &lt; 95%. Dashboard Compliance integra status de políticas (RF079). Exibir título, atualização, conformidade, cobertura filiais. Export PowerPoint gera arquivo com 6 slides (Capa, Sumário, C-Level, Custos, SLA/Compliance, Recomendações). Gráficos PNG embutidos. Toda tentativa de acesso deve ser auditada em AuditLog (RF004). Retenção 5 anos (LGPD).</t>
+          <t>Apenas usuários com perfis C-Level, Diretoria, Gerência Sênior e Analista Executivo podem acessar dashboards executivos. Dados agregados devem ser consolidados automaticamente via Hangfire às 6:00 AM UTC, job idempotente com registro de sucesso/falha. Forecast exige mínimo 12 meses de histórico. Modelo ARIMA/Regressão Linear deve atingir R² &gt;= 0.85 para validade. Budget vs Real calcula variação percentual. Alertas: &gt; 10% amarelo, &gt; 20% vermelho. Heatmap usa escala de cores: verde &lt; 80% meta, amarelo 80-100%, vermelho &gt; 100%. Cores acessíveis WCAG AA.</t>
         </is>
       </c>
       <c r="E97" s="3" t="inlineStr"/>
@@ -2376,7 +2762,11 @@
           <t>RF102</t>
         </is>
       </c>
-      <c r="B98" s="3" t="inlineStr"/>
+      <c r="B98" s="3" t="inlineStr">
+        <is>
+          <t>Relatórios e Análises</t>
+        </is>
+      </c>
       <c r="C98" s="3" t="inlineStr">
         <is>
           <t>Fornecer capacidade de criar, personalizar, executar, agendar e distribuir relatórios analíticos e gerenciais, consolidando dados operacionais de múltiplos módulos.</t>
@@ -2384,7 +2774,7 @@
       </c>
       <c r="D98" s="3" t="inlineStr">
         <is>
-          <t>Relatório deve ter no mínimo 1 campo selecionado. Relatórios sensíveis exigem justificativa (LGPD). Agendamento máximo 10 relatórios por usuário. Relatórios com &gt; 10.000 registros processados em background. Export PDF deve ter logo do cliente e metadados. Relatórios com dados pessoais exigem permissão especial. Histórico de relatórios mantido por 90 dias. Relatórios devem respeitar filtro multi-tenancy. Designer visual limitado a 20 campos. Auditoria obrigatória de todos os relatórios.</t>
+          <t>Relatório deve ter no mínimo 1 campo selecionado. Relatórios sensíveis exigem justificativa (LGPD). Agendamento máximo 10 relatórios por usuário. Relatórios com &gt; 10.000 registros processados em background. Export PDF deve ter logo do cliente e metadados.</t>
         </is>
       </c>
       <c r="E98" s="3" t="inlineStr"/>
@@ -2395,11 +2785,19 @@
           <t>RF103</t>
         </is>
       </c>
-      <c r="B99" s="3" t="inlineStr"/>
-      <c r="C99" s="3" t="inlineStr"/>
+      <c r="B99" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C99" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D99" s="3" t="inlineStr">
         <is>
-          <t>Volumetria via Agregação SQL Nativa. Consolidação Diária Automática às 4h. Comparativos Exigem Períodos Finalizados. Top 10 Ordenado Descendente. Tendências Usam Média Móvel 7 Dias. Retenção de Volumetria Histórica 24 Meses. Multi-tenancy Obrigatória - ClienteId em Todos os Filtros. Export Excel com Aba de Resumo. Relatórios &gt;100k Registros Processados em Background. Auditoria de Acesso a Relatórios.</t>
+          <t>Volumetria via Agregação SQL Nativa. Consolidação Diária Automática às 4h. Comparativos Exigem Períodos Finalizados. Top 10 Ordenado Descendente. Tendências Usam Média Móvel 7 Dias.</t>
         </is>
       </c>
       <c r="E99" s="3" t="inlineStr"/>
@@ -2410,15 +2808,19 @@
           <t>RF104</t>
         </is>
       </c>
-      <c r="B100" s="3" t="inlineStr"/>
+      <c r="B100" s="3" t="inlineStr">
+        <is>
+          <t>Gestão Completa de Cadastros Base (Domínios Configuráveis)</t>
+        </is>
+      </c>
       <c r="C100" s="3" t="inlineStr">
         <is>
-          <t>Fornecer um framework genérico e centralizado para gerenciamento de domínios configuráveis (tabelas de referência com listas controladas de valores) no sistema IControlIT, garantindo integridade referencial, auditoria completa, suporte a multi-tenancy e operações em lote (importação/exportação), sem necessidade de alteração de código para novos domínios.</t>
+          <t>Fornecer um framework genérico e centralizado para gerenciamento de domínios configuráveis (tabelas de referência com listas controladas de valores) no sistema IControlIT, garantindo integridade re...</t>
         </is>
       </c>
       <c r="D100" s="3" t="inlineStr">
         <is>
-          <t>Domínio Requer Nome Único e Descrição - Todo domínio deve ter nome único (case-insensitive), descrição clara e tipo (Lista, Hierarquia). Item de Domínio Requer Código Único dentro do Domínio - Cada item dentro de um domínio deve ter código único alfanumérico. Exclusão de Item Requer Validação de Integridade Referencial - Sistema valida se há registros referenciando o item via FK antes de exclusão física. Item Pode Ser Marcado como Inativo Sem Ser Deletado - Items deletados logicamente não são removidos fisicamente; marcados com Ativo=false. Domínios Podem Ter Estrutura Hierárquica (Pai-Filho) - Campo IdItemPai permite relação 1:N. Sistema valida ciclos. Importação em Lote com Preview e Validação - Upload CSV/Excel com valores do domínio. Sistema oferece preview, valida dados e aplica atomicamente. Auditoria Registra Todas Alterações de Domínios - Toda operação auditada com usuário, timestamp, antes/depois. Exportação Permite Download em CSV ou Excel - Usuários podem exportar qualquer domínio em formato CSV ou Excel. Domínios Suportam Atributos Customizados (Metadados) - Cada item pode ter JSON customizado de metadados. Reordenação de Itens Define Ordem de Exibição - Campo Ordem define sequência de exibição em dropdowns.</t>
+          <t>Domínio Requer Nome Único e Descrição - Todo domínio deve ter nome único (case-insensitive), descrição clara e tipo (Lista, Hierarquia). Item de Domínio Requer Código Único dentro do Domínio - Cada item dentro de um domínio deve ter código único alfanumérico. Exclusão de Item Requer Validação de Integridade Referencial - Sistema valida se há registros referenciando o item via FK antes de exclusão física. Item Pode Ser Marcado como Inativo Sem Ser Deletado - Items deletados logicamente não são removidos fisicamente; marcados com Ativo=false. Domínios Podem Ter Estrutura Hierárquica (Pai-Filho) - Campo IdItemPai permite relação 1:N. Sistema valida ciclos.</t>
         </is>
       </c>
       <c r="E100" s="3" t="inlineStr"/>
@@ -2429,18 +2831,21 @@
           <t>RF106</t>
         </is>
       </c>
-      <c r="B101" s="3" t="inlineStr"/>
+      <c r="B101" s="3" t="inlineStr">
+        <is>
+          <t>Gestão de Marcações e Tags</t>
+        </is>
+      </c>
       <c r="C101" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Implementar um sistema completo de gestão de tags (marcações) que permita categorizar,
+          <t>Implementar um sistema completo de gestão de tags (marcações) que permita categorizar,
 organizar e localizar entidades do sistema (Ativos, Contratos, Usuários, Chamados, Documentos)
-através de marcações personalizáveis, hierárquicas e inteligentes.
-</t>
+através de marc...</t>
         </is>
       </c>
       <c r="D101" s="3" t="inlineStr">
         <is>
-          <t>Unicidade de nomes por cliente - Uma tag não pode ter o mesmo nome que outra tag ativa do mesmo cliente (case-insensitive). Validação de cor e ícone - HexColor deve ser #RRGGBB, IconClass deve ser FontAwesome válido (opcionais). Hierarquia sem ciclos - Validação impede ciclos na hierarquia (Tag A não pode ser pai de B, B de C, e C de A). Profundidade máxima de hierarquia - Não pode exceder 3 níveis (avô, pai, filho). Soft delete de tags - Exclusão marca FlExcluido=1 sem remover registro. Tags excluídas não aparecem em listas.. Aplicação de tags múltiplas por entidade - Entidade pode ter 0 a N tags. Índice composto evita duplicatas.. Auto-complete com ElasticSearch - Resposta &lt; 200ms (p95), até 10 resultados ordenados por relevância + frequência. Sugestões baseadas em ML - Retorna 3-5 tags sugeridas com confidence, timeout 2s. Filtros AND/OR em buscas - Busca com operador lógico AND (todas as tags) ou OR (qualquer tag). Auditoria de alterações - Toda operação registrada com timestamp UTC, usuário, ação, valores antes/depois, ClienteId. Retenção mínima 3 anos.. Fusão de tags (merge) - Consolida origem em destino, remove duplicatas, soft delete origem, auditoria. Renomeação em lote - Renomear múltiplas tags em operação atômica com validação de conflitos. Dashboard de uso - Métricas agregadas: contagem por entidade, última alteração, usuário frequente, tendência 30 dias. Carregamento &lt; 500ms.. Sincronização assíncrona ElasticSearch - Atualização via MediatR/message queue, não bloqueia HTTP, ElasticSearch atualizado em até 5s. Exportação de dados por tag - Download CSV/Excel com colunas: EntityType, EntityId, EntityName, AppliedAt, AppliedBy.</t>
+          <t>Unicidade de nomes por cliente - Uma tag não pode ter o mesmo nome que outra tag ativa do mesmo cliente (case-insensitive). Validação de cor e ícone - HexColor deve ser #RRGGBB, IconClass deve ser FontAwesome válido (opcionais). Hierarquia sem ciclos - Validação impede ciclos na hierarquia (Tag A não pode ser pai de B, B de C, e C de A). Profundidade máxima de hierarquia - Não pode exceder 3 níveis (avô, pai, filho). Soft delete de tags - Exclusão marca FlExcluido=1 sem remover registro. Tags excluídas não aparecem em listas.</t>
         </is>
       </c>
       <c r="E101" s="3" t="inlineStr"/>
@@ -2451,19 +2856,21 @@
           <t>RF107</t>
         </is>
       </c>
-      <c r="B102" s="3" t="inlineStr"/>
+      <c r="B102" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
       <c r="C102" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Especificar o comportamento esperado do Módulo de Marcadores Localização QRCode,
+          <t>Especificar o comportamento esperado do Módulo de Marcadores Localização QRCode,
 responsável por gerar, gerenciar e processar códigos QR únicos para rastreamento
-de ativos físicos em tempo real, garantindo rastreabilidade completa, conformidade
-com LGPD e eficiência operacional.
-</t>
+de ativos físicos em tempo real, ga...</t>
         </is>
       </c>
       <c r="D102" s="3" t="inlineStr">
         <is>
-          <t>QRCode deve ser único (GUID codificado em Base64URL). QRCode deve conter ClienteId + AtivoId + CheckDigit. Check-digit calculado via Algoritmo de Luhn. Etiqueta deve conter QRCode + Nome Ativo + Código Patrimonial. Leitura de QRCode deve registrar Usuário, Data/Hora, GPS. Check-in sem check-out prévio deve alertar. Geolocalização deve ter precisão mínima de 10 metros. Histórico de leituras mantido por 24 meses. Inventário bulk deve processar até 1000 QRCodes por sessão. Auditoria de todas as operações de QRCode. Isolamento por tenant. Permissões RBAC.</t>
+          <t>QRCode deve ser único (GUID codificado em Base64URL). QRCode deve conter ClienteId + AtivoId + CheckDigit. Check-digit calculado via Algoritmo de Luhn. Etiqueta deve conter QRCode + Nome Ativo + Código Patrimonial. Leitura de QRCode deve registrar Usuário, Data/Hora, GPS.</t>
         </is>
       </c>
       <c r="E102" s="3" t="inlineStr"/>
@@ -2474,15 +2881,21 @@
           <t>RF108</t>
         </is>
       </c>
-      <c r="B103" s="3" t="inlineStr"/>
+      <c r="B103" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
       <c r="C103" s="3" t="inlineStr">
         <is>
-          <t>{'descricao': 'Implementar camadas adicionais de proteção além da autenticação básica,\nfornecendo CAPTCHA, Multi-Factor Authentication (MFA), contestação de faturas,\ndetecção de bots, rate limiting, device fingerprinting e análise comportamental\nde usuários para proteger contra ataques automatizados e fraudes.\n'}</t>
+          <t>Implementar camadas adicionais de proteção além da autenticação básica,
+fornecendo CAPTCHA, Multi-Factor Authentication (MFA), contestação de faturas,
+detecção de bots, rate limiting, device finger...</t>
         </is>
       </c>
       <c r="D103" s="3" t="inlineStr">
         <is>
-          <t>CAPTCHA obrigatório após 3 falhas de login. MFA obrigatório para perfis críticos. Código TOTP válido por 30 segundos. Código SMS válido por 5 minutos. Contestação requer justificativa mínima. Rate limiting de 100 req/min por IP. Bloqueio automático após 5 falhas. Device fingerprint armazenado para usuários confiáveis. Notificação de login de nova localização. Contestação aprovada/rejeitada por perfil superior.</t>
+          <t>CAPTCHA obrigatório após 3 falhas de login. MFA obrigatório para perfis críticos. Código TOTP válido por 30 segundos. Código SMS válido por 5 minutos. Contestação requer justificativa mínima.</t>
         </is>
       </c>
       <c r="E103" s="3" t="inlineStr"/>
@@ -2493,11 +2906,19 @@
           <t>RF109</t>
         </is>
       </c>
-      <c r="B104" s="3" t="inlineStr"/>
-      <c r="C104" s="3" t="inlineStr"/>
+      <c r="B104" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C104" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D104" s="3" t="inlineStr">
         <is>
-          <t>Tamanho Máximo de Arquivo 50MB. Formatos Permitidos: PDF, JPEG, PNG, TIFF, DOCX, XLSX. OCR Assíncrono Obrigatório via Fila. Detecção de Malware Obrigatória (ClamAV). Assinatura Digital ICP-Brasil Opcional. Retenção Mínima 7 Anos (LGPD Art. 16). Indexação Full-Text com ElasticSearch. Multi-tenancy Obrigatória - ClienteId em Todos os Filtros. Storage Hierarquizado (Hot/Cool/Archive). Auditoria Completa de Acesso e Modificações.</t>
+          <t>Tamanho Máximo de Arquivo 50MB. Formatos Permitidos: PDF, JPEG, PNG, TIFF, DOCX, XLSX. OCR Assíncrono Obrigatório via Fila. Detecção de Malware Obrigatória (ClamAV). Assinatura Digital ICP-Brasil Opcional.</t>
         </is>
       </c>
       <c r="E104" s="3" t="inlineStr"/>
@@ -2513,10 +2934,14 @@
           <t>Cache Distribuído e Otimização de Performance</t>
         </is>
       </c>
-      <c r="C105" s="3" t="inlineStr"/>
+      <c r="C105" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D105" s="3" t="inlineStr">
         <is>
-          <t>Isolamento Multi-Tenancy. TTL Configurável por Entidade. Invalidação Automática em Writes. Compressão Condicional. Limite de Tamanho de Payload. Hit Rate Mínimo Esperado de 80%. Fallback Transparente. Invalidação por Relacionamento. Cache de Listas Paginadas. Auditoria de Cache.</t>
+          <t>Isolamento Multi-Tenancy. TTL Configurável por Entidade. Invalidação Automática em Writes. Compressão Condicional. Limite de Tamanho de Payload.</t>
         </is>
       </c>
       <c r="E105" s="3" t="inlineStr"/>
@@ -2527,11 +2952,19 @@
           <t>RF111</t>
         </is>
       </c>
-      <c r="B106" s="3" t="inlineStr"/>
-      <c r="C106" s="3" t="inlineStr"/>
+      <c r="B106" s="3" t="inlineStr">
+        <is>
+          <t>Nome não disponível</t>
+        </is>
+      </c>
+      <c r="C106" s="3" t="inlineStr">
+        <is>
+          <t>Descrição não disponível.</t>
+        </is>
+      </c>
       <c r="D106" s="3" t="inlineStr">
         <is>
-          <t>Backup Completo Diário em Horário de Baixa Demanda. Backup Incremental Periódico. Política de Retenção Configurável. Criptografia Obrigatória com Chaves Gerenciadas. Validação de Integridade Obrigatória. Garantia de RPO (Recovery Point Objective). Garantia de RTO (Recovery Time Objective). Failover Automático em Caso de Indisponibilidade. Teste de Disaster Recovery Obrigatório. Auditoria Completa de Operações. Isolamento por Tenant. Notificações de Falha e Sucesso.</t>
+          <t>Backup Completo Diário em Horário de Baixa Demanda. Backup Incremental Periódico. Política de Retenção Configurável. Criptografia Obrigatória com Chaves Gerenciadas. Validação de Integridade Obrigatória.</t>
         </is>
       </c>
       <c r="E106" s="3" t="inlineStr"/>
@@ -2542,7 +2975,11 @@
           <t>RF112</t>
         </is>
       </c>
-      <c r="B107" s="3" t="inlineStr"/>
+      <c r="B107" s="3" t="inlineStr">
+        <is>
+          <t>Jobs e Tarefas Agendadas</t>
+        </is>
+      </c>
       <c r="C107" s="3" t="inlineStr">
         <is>
           <t>Sistema para gerenciar, executar, monitorar e auditar tarefas de background (jobs agendados e sob demanda) no IControlIT.</t>
@@ -2550,7 +2987,7 @@
       </c>
       <c r="D107" s="3" t="inlineStr">
         <is>
-          <t>Nome Único de Job por Tenant. Validação de Cron Expression. Retry Automático com Backoff Exponencial. Timeout Padrão de 30 Minutos. Máximo 10 Workers Paralelos por Tenant. Histórico de Execuções Retido por 90 Dias. Notificação de Falha para Administrador. Multi-tenancy com ClienteId. Jobs Sensíveis Exigem Duas Permissões (2-Step Execution). Auditoria Completa de Operações em Jobs.</t>
+          <t>Nome Único de Job por Tenant. Validação de Cron Expression. Retry Automático com Backoff Exponencial. Timeout Padrão de 30 Minutos. Máximo 10 Workers Paralelos por Tenant.</t>
         </is>
       </c>
       <c r="E107" s="3" t="inlineStr"/>

</xml_diff>

<commit_message>
fix(ferramentas): corrigir extração de nome para cobrir rf_title e metadata.titulo
PROBLEMA RESOLVIDO:
- 26 RFs usavam campo 'rf_title' ao invés de 'titulo'
- 1 RF usa estrutura 'metadata.titulo'
- Script anterior extraía apenas 'titulo', 'nome', 'title', 'rf.nome'

CORREÇÃO:
- Adicionar busca em 'rf_title' (26 RFs)
- Adicionar busca em 'metadata.titulo' (1 RF)
- Busca em 'rf.titulo' (além de 'rf.nome')

RESULTADO v2.1:
- 105/106 RFs com nome preenchido (99%)
- Antes: 80/106 (75%)
- Melhoria: +25 RFs (+24%)
- Único RF sem nome: RF105 (erro de parse YAML na linha 405)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/funcionalidades.xlsx
+++ b/funcionalidades.xlsx
@@ -947,7 +947,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Fornecedores</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1064,7 +1064,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Aditivos de Contratos</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Itens de Auditoria</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Bilhetes Telefônicos</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1392,7 +1392,7 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Estoque de Aparelhos</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Notas Fiscais Estoque</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Endereços de Entrega</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1530,7 +1530,7 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Tipos de Consumidores</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Linhas Móveis e Chips SIM</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Lotes de Auditoria</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Status e Tipos Genéricos</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -1831,7 +1831,7 @@
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Tipos de Chamado</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Notificações e Alertas</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Inventário Cíclico e Auditoria de Estoque</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
@@ -2087,7 +2087,7 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Pesquisa de Satisfação</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
@@ -2157,7 +2157,7 @@
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Chamados - Portal Self-Service</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
@@ -2367,7 +2367,7 @@
       </c>
       <c r="B81" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Importação de Dados</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
@@ -2436,7 +2436,7 @@
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Aprovações e Workflows</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
@@ -2579,7 +2579,7 @@
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Auditoria de Custos e Compliance</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
@@ -2717,7 +2717,7 @@
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Dashboards e KPIs com Análise Preditiva</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B99" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Relatórios e Volumetria</t>
         </is>
       </c>
       <c r="C99" s="3" t="inlineStr">
@@ -2858,7 +2858,7 @@
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Marcadores Localização QRCode</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
@@ -2883,7 +2883,7 @@
       </c>
       <c r="B103" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>CAPTCHA, MFA, Contestação e Segurança Avançada</t>
         </is>
       </c>
       <c r="C103" s="3" t="inlineStr">
@@ -2908,7 +2908,7 @@
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Gestão de Documentos Originais e Digitalização</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>Nome não disponível</t>
+          <t>Backup, Recuperação e Disaster Recovery</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">

</xml_diff>